<commit_message>
MioConfig initial push & Modbus.Core working with Attributes
</commit_message>
<xml_diff>
--- a/Карта конфигурации.xlsx
+++ b/Карта конфигурации.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\MFC\PROJECTS\МВВ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\MFC\PROJECTS\MIO\GIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="19020" windowHeight="8580" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="60" windowWidth="19020" windowHeight="8580"/>
   </bookViews>
   <sheets>
     <sheet name="Общая таблица настроек" sheetId="1" r:id="rId1"/>
@@ -647,7 +647,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -668,12 +668,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -681,6 +675,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -806,7 +812,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -950,7 +956,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -958,6 +964,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -971,7 +989,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -983,13 +1001,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -997,6 +1024,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -1007,25 +1046,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1361,8 +1394,8 @@
   </sheetPr>
   <dimension ref="A1:X11988"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J1"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1380,18 +1413,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="58" t="s">
+      <c r="A1" s="62" t="s">
         <v>187</v>
       </c>
-      <c r="B1" s="58"/>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B2" s="26"/>
@@ -1401,15 +1434,15 @@
       <c r="A3" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="77">
+      <c r="B3" s="85">
         <v>1000</v>
       </c>
-      <c r="C3" s="77"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="77"/>
-      <c r="F3" s="77"/>
-      <c r="G3" s="77"/>
-      <c r="H3" s="77"/>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
+      <c r="E3" s="85"/>
+      <c r="F3" s="85"/>
+      <c r="G3" s="85"/>
+      <c r="H3" s="85"/>
       <c r="I3" s="47"/>
       <c r="J3" s="49"/>
       <c r="K3" s="2"/>
@@ -1472,28 +1505,28 @@
       <c r="X4" s="1"/>
     </row>
     <row r="5" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="65" t="s">
+      <c r="A5" s="72" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="61">
+      <c r="B5" s="86">
         <v>0</v>
       </c>
-      <c r="C5" s="38">
+      <c r="C5" s="56">
         <v>0</v>
       </c>
-      <c r="D5" s="62" t="s">
+      <c r="D5" s="66" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="61" t="s">
+      <c r="E5" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61"/>
-      <c r="H5" s="61" t="s">
+      <c r="F5" s="86"/>
+      <c r="G5" s="86"/>
+      <c r="H5" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="63"/>
-      <c r="J5" s="62" t="s">
+      <c r="I5" s="70"/>
+      <c r="J5" s="66" t="s">
         <v>179</v>
       </c>
       <c r="K5" s="3"/>
@@ -1512,18 +1545,18 @@
       <c r="X5" s="1"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="65"/>
-      <c r="B6" s="61"/>
-      <c r="C6" s="38">
+      <c r="A6" s="72"/>
+      <c r="B6" s="86"/>
+      <c r="C6" s="56">
         <v>1</v>
       </c>
-      <c r="D6" s="62"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="61"/>
-      <c r="I6" s="64"/>
-      <c r="J6" s="62"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
+      <c r="H6" s="86"/>
+      <c r="I6" s="71"/>
+      <c r="J6" s="66"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
@@ -1540,26 +1573,26 @@
       <c r="X6" s="1"/>
     </row>
     <row r="7" spans="1:24" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="65"/>
-      <c r="B7" s="61">
+      <c r="A7" s="72"/>
+      <c r="B7" s="65">
         <v>1</v>
       </c>
       <c r="C7" s="38">
         <v>2</v>
       </c>
-      <c r="D7" s="62" t="s">
+      <c r="D7" s="67" t="s">
         <v>96</v>
       </c>
-      <c r="E7" s="61" t="s">
+      <c r="E7" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="61"/>
-      <c r="G7" s="61"/>
-      <c r="H7" s="61" t="s">
+      <c r="F7" s="65"/>
+      <c r="G7" s="65"/>
+      <c r="H7" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="63"/>
-      <c r="J7" s="71" t="s">
+      <c r="I7" s="68"/>
+      <c r="J7" s="74" t="s">
         <v>98</v>
       </c>
       <c r="K7" s="3"/>
@@ -1578,18 +1611,18 @@
       <c r="X7" s="1"/>
     </row>
     <row r="8" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="65"/>
-      <c r="B8" s="61"/>
+      <c r="A8" s="72"/>
+      <c r="B8" s="65"/>
       <c r="C8" s="38">
         <v>3</v>
       </c>
-      <c r="D8" s="62"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="61"/>
-      <c r="G8" s="61"/>
-      <c r="H8" s="61"/>
-      <c r="I8" s="64"/>
-      <c r="J8" s="71"/>
+      <c r="D8" s="67"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="65"/>
+      <c r="G8" s="65"/>
+      <c r="H8" s="65"/>
+      <c r="I8" s="69"/>
+      <c r="J8" s="74"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
@@ -1606,26 +1639,26 @@
       <c r="X8" s="1"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9" s="65"/>
-      <c r="B9" s="61">
+      <c r="A9" s="72"/>
+      <c r="B9" s="65">
         <v>2</v>
       </c>
       <c r="C9" s="38">
         <v>4</v>
       </c>
-      <c r="D9" s="62" t="s">
+      <c r="D9" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="61" t="s">
+      <c r="E9" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="61"/>
-      <c r="G9" s="61"/>
-      <c r="H9" s="61" t="s">
+      <c r="F9" s="65"/>
+      <c r="G9" s="65"/>
+      <c r="H9" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="63"/>
-      <c r="J9" s="71" t="s">
+      <c r="I9" s="68"/>
+      <c r="J9" s="74" t="s">
         <v>101</v>
       </c>
       <c r="K9" s="3"/>
@@ -1644,18 +1677,18 @@
       <c r="X9" s="1"/>
     </row>
     <row r="10" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="65"/>
-      <c r="B10" s="61"/>
+      <c r="A10" s="72"/>
+      <c r="B10" s="65"/>
       <c r="C10" s="38">
         <v>5</v>
       </c>
-      <c r="D10" s="62"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="61"/>
-      <c r="G10" s="61"/>
-      <c r="H10" s="61"/>
-      <c r="I10" s="64"/>
-      <c r="J10" s="71"/>
+      <c r="D10" s="67"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="65"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="69"/>
+      <c r="J10" s="74"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
@@ -1672,26 +1705,26 @@
       <c r="X10" s="1"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" s="65"/>
-      <c r="B11" s="75">
+      <c r="A11" s="72"/>
+      <c r="B11" s="77">
         <v>3</v>
       </c>
-      <c r="C11" s="38">
+      <c r="C11" s="57">
         <v>6</v>
       </c>
       <c r="D11" s="76" t="s">
         <v>97</v>
       </c>
-      <c r="E11" s="75" t="s">
+      <c r="E11" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="75"/>
-      <c r="G11" s="75"/>
-      <c r="H11" s="75" t="s">
+      <c r="F11" s="77"/>
+      <c r="G11" s="77"/>
+      <c r="H11" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="63"/>
-      <c r="J11" s="71" t="s">
+      <c r="I11" s="68"/>
+      <c r="J11" s="74" t="s">
         <v>99</v>
       </c>
       <c r="K11" s="3"/>
@@ -1710,18 +1743,18 @@
       <c r="X11" s="1"/>
     </row>
     <row r="12" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="65"/>
-      <c r="B12" s="75"/>
-      <c r="C12" s="38">
+      <c r="A12" s="72"/>
+      <c r="B12" s="77"/>
+      <c r="C12" s="57">
         <v>7</v>
       </c>
       <c r="D12" s="76"/>
-      <c r="E12" s="75"/>
-      <c r="F12" s="75"/>
-      <c r="G12" s="75"/>
-      <c r="H12" s="75"/>
-      <c r="I12" s="64"/>
-      <c r="J12" s="71"/>
+      <c r="E12" s="77"/>
+      <c r="F12" s="77"/>
+      <c r="G12" s="77"/>
+      <c r="H12" s="77"/>
+      <c r="I12" s="69"/>
+      <c r="J12" s="74"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
@@ -1738,25 +1771,25 @@
       <c r="X12" s="1"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A13" s="65"/>
-      <c r="B13" s="61">
+      <c r="A13" s="72"/>
+      <c r="B13" s="65">
         <v>4</v>
       </c>
       <c r="C13" s="38">
         <v>8</v>
       </c>
-      <c r="D13" s="74" t="s">
+      <c r="D13" s="76" t="s">
         <v>95</v>
       </c>
-      <c r="E13" s="61" t="s">
+      <c r="E13" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="61"/>
-      <c r="G13" s="61"/>
-      <c r="H13" s="54" t="s">
+      <c r="F13" s="65"/>
+      <c r="G13" s="65"/>
+      <c r="H13" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="63"/>
+      <c r="I13" s="68"/>
       <c r="J13" s="45"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
@@ -1774,17 +1807,17 @@
       <c r="X13" s="1"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A14" s="65"/>
-      <c r="B14" s="61"/>
+      <c r="A14" s="72"/>
+      <c r="B14" s="65"/>
       <c r="C14" s="38">
         <v>9</v>
       </c>
-      <c r="D14" s="74"/>
-      <c r="E14" s="61"/>
-      <c r="F14" s="61"/>
-      <c r="G14" s="61"/>
-      <c r="H14" s="55"/>
-      <c r="I14" s="64"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="65"/>
+      <c r="F14" s="65"/>
+      <c r="G14" s="65"/>
+      <c r="H14" s="59"/>
+      <c r="I14" s="69"/>
       <c r="J14" s="45"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
@@ -1802,26 +1835,26 @@
       <c r="X14" s="1"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A15" s="66"/>
-      <c r="B15" s="61">
+      <c r="A15" s="73"/>
+      <c r="B15" s="65">
         <v>5</v>
       </c>
       <c r="C15" s="38">
         <v>10</v>
       </c>
-      <c r="D15" s="62" t="s">
+      <c r="D15" s="84" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="61" t="s">
+      <c r="E15" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="F15" s="61"/>
-      <c r="G15" s="61"/>
-      <c r="H15" s="61" t="s">
+      <c r="F15" s="75"/>
+      <c r="G15" s="75"/>
+      <c r="H15" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="I15" s="63"/>
-      <c r="J15" s="62" t="s">
+      <c r="I15" s="68"/>
+      <c r="J15" s="67" t="s">
         <v>179</v>
       </c>
       <c r="K15" s="3"/>
@@ -1840,18 +1873,18 @@
       <c r="X15" s="1"/>
     </row>
     <row r="16" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="66"/>
-      <c r="B16" s="61"/>
+      <c r="A16" s="73"/>
+      <c r="B16" s="65"/>
       <c r="C16" s="38">
         <v>11</v>
       </c>
-      <c r="D16" s="62"/>
-      <c r="E16" s="61"/>
-      <c r="F16" s="61"/>
-      <c r="G16" s="61"/>
-      <c r="H16" s="61"/>
-      <c r="I16" s="64"/>
-      <c r="J16" s="62"/>
+      <c r="D16" s="84"/>
+      <c r="E16" s="75"/>
+      <c r="F16" s="75"/>
+      <c r="G16" s="75"/>
+      <c r="H16" s="75"/>
+      <c r="I16" s="69"/>
+      <c r="J16" s="67"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
@@ -1868,10 +1901,12 @@
       <c r="X16" s="1"/>
     </row>
     <row r="17" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="67" t="s">
+      <c r="A17" s="78" t="s">
         <v>88</v>
       </c>
-      <c r="B17" s="61"/>
+      <c r="B17" s="65">
+        <v>1</v>
+      </c>
       <c r="C17" s="38" t="s">
         <v>104</v>
       </c>
@@ -1912,8 +1947,8 @@
       <c r="X17" s="1"/>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A18" s="68"/>
-      <c r="B18" s="61"/>
+      <c r="A18" s="79"/>
+      <c r="B18" s="65"/>
       <c r="C18" s="38" t="s">
         <v>105</v>
       </c>
@@ -1952,27 +1987,29 @@
       <c r="X18" s="1"/>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A19" s="68"/>
-      <c r="B19" s="61"/>
+      <c r="A19" s="79"/>
+      <c r="B19" s="65">
+        <v>2</v>
+      </c>
       <c r="C19" s="38" t="s">
         <v>106</v>
       </c>
-      <c r="D19" s="62" t="s">
+      <c r="D19" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="61" t="s">
+      <c r="E19" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="F19" s="61">
+      <c r="F19" s="65">
         <v>1200</v>
       </c>
-      <c r="G19" s="61">
+      <c r="G19" s="65">
         <v>57600</v>
       </c>
-      <c r="H19" s="61" t="s">
+      <c r="H19" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="I19" s="54">
+      <c r="I19" s="58">
         <v>9600</v>
       </c>
       <c r="J19" s="45"/>
@@ -1992,17 +2029,17 @@
       <c r="X19" s="1"/>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A20" s="68"/>
-      <c r="B20" s="61"/>
+      <c r="A20" s="79"/>
+      <c r="B20" s="65"/>
       <c r="C20" s="38" t="s">
         <v>107</v>
       </c>
-      <c r="D20" s="62"/>
-      <c r="E20" s="61"/>
-      <c r="F20" s="61"/>
-      <c r="G20" s="61"/>
-      <c r="H20" s="61"/>
-      <c r="I20" s="55"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="65"/>
+      <c r="F20" s="65"/>
+      <c r="G20" s="65"/>
+      <c r="H20" s="65"/>
+      <c r="I20" s="59"/>
       <c r="J20" s="45"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
@@ -2020,8 +2057,10 @@
       <c r="X20" s="1"/>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A21" s="68"/>
-      <c r="B21" s="61"/>
+      <c r="A21" s="79"/>
+      <c r="B21" s="65">
+        <v>3</v>
+      </c>
       <c r="C21" s="38" t="s">
         <v>108</v>
       </c>
@@ -2060,8 +2099,8 @@
       <c r="X21" s="1"/>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A22" s="68"/>
-      <c r="B22" s="61"/>
+      <c r="A22" s="79"/>
+      <c r="B22" s="65"/>
       <c r="C22" s="38" t="s">
         <v>109</v>
       </c>
@@ -2102,8 +2141,10 @@
       <c r="X22" s="1"/>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A23" s="68"/>
-      <c r="B23" s="61"/>
+      <c r="A23" s="79"/>
+      <c r="B23" s="65">
+        <v>4</v>
+      </c>
       <c r="C23" s="38" t="s">
         <v>110</v>
       </c>
@@ -2142,30 +2183,30 @@
       <c r="X23" s="1"/>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A24" s="68"/>
-      <c r="B24" s="61"/>
+      <c r="A24" s="79"/>
+      <c r="B24" s="65"/>
       <c r="C24" s="38" t="s">
         <v>111</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="55" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="14" t="s">
+      <c r="E24" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="F24" s="15">
+      <c r="F24" s="54">
         <v>0</v>
       </c>
-      <c r="G24" s="15">
+      <c r="G24" s="54">
         <v>0</v>
       </c>
-      <c r="H24" s="14" t="s">
+      <c r="H24" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="I24" s="44">
+      <c r="I24" s="54">
         <v>0</v>
       </c>
-      <c r="J24" s="45" t="s">
+      <c r="J24" s="55" t="s">
         <v>191</v>
       </c>
       <c r="K24" s="3"/>
@@ -2184,8 +2225,10 @@
       <c r="X24" s="1"/>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A25" s="68"/>
-      <c r="B25" s="61"/>
+      <c r="A25" s="79"/>
+      <c r="B25" s="65">
+        <v>5</v>
+      </c>
       <c r="C25" s="38" t="s">
         <v>112</v>
       </c>
@@ -2226,30 +2269,30 @@
       <c r="X25" s="1"/>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A26" s="68"/>
-      <c r="B26" s="61"/>
+      <c r="A26" s="79"/>
+      <c r="B26" s="65"/>
       <c r="C26" s="38" t="s">
         <v>113</v>
       </c>
-      <c r="D26" s="56" t="s">
+      <c r="D26" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="E26" s="61" t="s">
+      <c r="E26" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="F26" s="54">
+      <c r="F26" s="58">
         <v>0</v>
       </c>
-      <c r="G26" s="54">
+      <c r="G26" s="58">
         <v>65535</v>
       </c>
       <c r="H26" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I26" s="54">
+      <c r="I26" s="58">
         <v>200</v>
       </c>
-      <c r="J26" s="56" t="s">
+      <c r="J26" s="60" t="s">
         <v>183</v>
       </c>
       <c r="K26" s="3"/>
@@ -2268,20 +2311,22 @@
       <c r="X26" s="1"/>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A27" s="68"/>
-      <c r="B27" s="61"/>
+      <c r="A27" s="79"/>
+      <c r="B27" s="65">
+        <v>6</v>
+      </c>
       <c r="C27" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="D27" s="57"/>
-      <c r="E27" s="61"/>
-      <c r="F27" s="55"/>
-      <c r="G27" s="55"/>
+      <c r="D27" s="61"/>
+      <c r="E27" s="65"/>
+      <c r="F27" s="59"/>
+      <c r="G27" s="59"/>
       <c r="H27" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I27" s="55"/>
-      <c r="J27" s="57"/>
+      <c r="I27" s="59"/>
+      <c r="J27" s="61"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
@@ -2298,8 +2343,8 @@
       <c r="X27" s="1"/>
     </row>
     <row r="28" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="68"/>
-      <c r="B28" s="61"/>
+      <c r="A28" s="79"/>
+      <c r="B28" s="65"/>
       <c r="C28" s="38" t="s">
         <v>115</v>
       </c>
@@ -2340,8 +2385,10 @@
       <c r="X28" s="1"/>
     </row>
     <row r="29" spans="1:24" ht="60" x14ac:dyDescent="0.25">
-      <c r="A29" s="68"/>
-      <c r="B29" s="61"/>
+      <c r="A29" s="79"/>
+      <c r="B29" s="65">
+        <v>7</v>
+      </c>
       <c r="C29" s="38" t="s">
         <v>116</v>
       </c>
@@ -2382,8 +2429,8 @@
       <c r="X29" s="1"/>
     </row>
     <row r="30" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="69"/>
-      <c r="B30" s="61"/>
+      <c r="A30" s="80"/>
+      <c r="B30" s="65"/>
       <c r="C30" s="38" t="s">
         <v>117</v>
       </c>
@@ -2424,10 +2471,10 @@
       <c r="X30" s="1"/>
     </row>
     <row r="31" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="67" t="s">
+      <c r="A31" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="61"/>
+      <c r="B31" s="65"/>
       <c r="C31" s="38" t="s">
         <v>118</v>
       </c>
@@ -2466,30 +2513,30 @@
       <c r="X31" s="1"/>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A32" s="68"/>
-      <c r="B32" s="61"/>
+      <c r="A32" s="79"/>
+      <c r="B32" s="65"/>
       <c r="C32" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="D32" s="56" t="s">
+      <c r="D32" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="E32" s="61" t="s">
+      <c r="E32" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="F32" s="54">
+      <c r="F32" s="58">
         <v>0</v>
       </c>
-      <c r="G32" s="54">
+      <c r="G32" s="58">
         <v>65535</v>
       </c>
       <c r="H32" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I32" s="54">
+      <c r="I32" s="58">
         <v>10</v>
       </c>
-      <c r="J32" s="56" t="s">
+      <c r="J32" s="60" t="s">
         <v>183</v>
       </c>
       <c r="K32" s="3"/>
@@ -2508,20 +2555,20 @@
       <c r="X32" s="1"/>
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A33" s="68"/>
-      <c r="B33" s="61"/>
+      <c r="A33" s="79"/>
+      <c r="B33" s="65"/>
       <c r="C33" s="38" t="s">
         <v>120</v>
       </c>
-      <c r="D33" s="57"/>
-      <c r="E33" s="61"/>
-      <c r="F33" s="55"/>
-      <c r="G33" s="55"/>
+      <c r="D33" s="61"/>
+      <c r="E33" s="65"/>
+      <c r="F33" s="59"/>
+      <c r="G33" s="59"/>
       <c r="H33" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I33" s="55"/>
-      <c r="J33" s="57"/>
+      <c r="I33" s="59"/>
+      <c r="J33" s="61"/>
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
@@ -2538,8 +2585,8 @@
       <c r="X33" s="1"/>
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A34" s="68"/>
-      <c r="B34" s="61"/>
+      <c r="A34" s="79"/>
+      <c r="B34" s="65"/>
       <c r="C34" s="38" t="s">
         <v>121</v>
       </c>
@@ -2570,8 +2617,8 @@
       <c r="X34" s="1"/>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A35" s="68"/>
-      <c r="B35" s="61"/>
+      <c r="A35" s="79"/>
+      <c r="B35" s="65"/>
       <c r="C35" s="38" t="s">
         <v>122</v>
       </c>
@@ -2602,8 +2649,8 @@
       <c r="X35" s="1"/>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A36" s="68"/>
-      <c r="B36" s="61"/>
+      <c r="A36" s="79"/>
+      <c r="B36" s="65"/>
       <c r="C36" s="38" t="s">
         <v>123</v>
       </c>
@@ -2634,8 +2681,8 @@
       <c r="X36" s="1"/>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A37" s="68"/>
-      <c r="B37" s="61"/>
+      <c r="A37" s="79"/>
+      <c r="B37" s="65"/>
       <c r="C37" s="38" t="s">
         <v>124</v>
       </c>
@@ -2666,8 +2713,8 @@
       <c r="X37" s="1"/>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A38" s="68"/>
-      <c r="B38" s="61"/>
+      <c r="A38" s="79"/>
+      <c r="B38" s="65"/>
       <c r="C38" s="38" t="s">
         <v>125</v>
       </c>
@@ -2698,10 +2745,10 @@
       <c r="X38" s="1"/>
     </row>
     <row r="39" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="67" t="s">
+      <c r="A39" s="78" t="s">
         <v>36</v>
       </c>
-      <c r="B39" s="54"/>
+      <c r="B39" s="58"/>
       <c r="C39" s="38" t="s">
         <v>126</v>
       </c>
@@ -2740,30 +2787,30 @@
       <c r="X39" s="1"/>
     </row>
     <row r="40" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="72"/>
-      <c r="B40" s="55"/>
+      <c r="A40" s="81"/>
+      <c r="B40" s="59"/>
       <c r="C40" s="38" t="s">
         <v>127</v>
       </c>
-      <c r="D40" s="59" t="s">
+      <c r="D40" s="63" t="s">
         <v>37</v>
       </c>
-      <c r="E40" s="61" t="s">
+      <c r="E40" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="F40" s="54">
+      <c r="F40" s="58">
         <v>0</v>
       </c>
-      <c r="G40" s="54">
+      <c r="G40" s="58">
         <v>65535</v>
       </c>
       <c r="H40" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I40" s="54">
+      <c r="I40" s="58">
         <v>10</v>
       </c>
-      <c r="J40" s="56" t="s">
+      <c r="J40" s="60" t="s">
         <v>183</v>
       </c>
       <c r="K40" s="3"/>
@@ -2782,20 +2829,20 @@
       <c r="X40" s="1"/>
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A41" s="72"/>
-      <c r="B41" s="54"/>
+      <c r="A41" s="81"/>
+      <c r="B41" s="58"/>
       <c r="C41" s="38" t="s">
         <v>128</v>
       </c>
-      <c r="D41" s="60"/>
-      <c r="E41" s="61"/>
-      <c r="F41" s="55"/>
-      <c r="G41" s="55"/>
+      <c r="D41" s="64"/>
+      <c r="E41" s="65"/>
+      <c r="F41" s="59"/>
+      <c r="G41" s="59"/>
       <c r="H41" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I41" s="55"/>
-      <c r="J41" s="57"/>
+      <c r="I41" s="59"/>
+      <c r="J41" s="61"/>
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
@@ -2812,8 +2859,8 @@
       <c r="X41" s="1"/>
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A42" s="72"/>
-      <c r="B42" s="55"/>
+      <c r="A42" s="81"/>
+      <c r="B42" s="59"/>
       <c r="C42" s="38" t="s">
         <v>129</v>
       </c>
@@ -2844,8 +2891,8 @@
       <c r="X42" s="1"/>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A43" s="72"/>
-      <c r="B43" s="54"/>
+      <c r="A43" s="81"/>
+      <c r="B43" s="58"/>
       <c r="C43" s="38" t="s">
         <v>130</v>
       </c>
@@ -2886,8 +2933,8 @@
       <c r="X43" s="1"/>
     </row>
     <row r="44" spans="1:24" ht="45" x14ac:dyDescent="0.25">
-      <c r="A44" s="72"/>
-      <c r="B44" s="55"/>
+      <c r="A44" s="81"/>
+      <c r="B44" s="59"/>
       <c r="C44" s="38" t="s">
         <v>131</v>
       </c>
@@ -2928,27 +2975,27 @@
       <c r="X44" s="1"/>
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A45" s="72"/>
-      <c r="B45" s="54"/>
+      <c r="A45" s="81"/>
+      <c r="B45" s="58"/>
       <c r="C45" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="D45" s="56" t="s">
+      <c r="D45" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="E45" s="61" t="s">
+      <c r="E45" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="F45" s="54" t="s">
+      <c r="F45" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="G45" s="54" t="s">
+      <c r="G45" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="H45" s="54" t="s">
+      <c r="H45" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="I45" s="54">
+      <c r="I45" s="58">
         <v>0</v>
       </c>
       <c r="J45" s="45" t="s">
@@ -2970,17 +3017,17 @@
       <c r="X45" s="1"/>
     </row>
     <row r="46" spans="1:24" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="72"/>
-      <c r="B46" s="55"/>
+      <c r="A46" s="81"/>
+      <c r="B46" s="59"/>
       <c r="C46" s="38" t="s">
         <v>133</v>
       </c>
-      <c r="D46" s="57"/>
-      <c r="E46" s="61"/>
-      <c r="F46" s="55"/>
-      <c r="G46" s="55"/>
-      <c r="H46" s="55"/>
-      <c r="I46" s="55"/>
+      <c r="D46" s="61"/>
+      <c r="E46" s="65"/>
+      <c r="F46" s="59"/>
+      <c r="G46" s="59"/>
+      <c r="H46" s="59"/>
+      <c r="I46" s="59"/>
       <c r="J46" s="45" t="s">
         <v>188</v>
       </c>
@@ -3000,8 +3047,8 @@
       <c r="X46" s="1"/>
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A47" s="72"/>
-      <c r="B47" s="54"/>
+      <c r="A47" s="81"/>
+      <c r="B47" s="58"/>
       <c r="C47" s="38" t="s">
         <v>134</v>
       </c>
@@ -3042,8 +3089,8 @@
       <c r="X47" s="1"/>
     </row>
     <row r="48" spans="1:24" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="72"/>
-      <c r="B48" s="55"/>
+      <c r="A48" s="81"/>
+      <c r="B48" s="59"/>
       <c r="C48" s="38" t="s">
         <v>135</v>
       </c>
@@ -3084,24 +3131,24 @@
       <c r="X48" s="1"/>
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A49" s="72"/>
-      <c r="B49" s="54"/>
+      <c r="A49" s="81"/>
+      <c r="B49" s="58"/>
       <c r="C49" s="38" t="s">
         <v>136</v>
       </c>
-      <c r="D49" s="56" t="s">
+      <c r="D49" s="60" t="s">
         <v>46</v>
       </c>
-      <c r="E49" s="61" t="s">
+      <c r="E49" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="F49" s="54" t="s">
+      <c r="F49" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="G49" s="54" t="s">
+      <c r="G49" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="H49" s="54" t="s">
+      <c r="H49" s="58" t="s">
         <v>13</v>
       </c>
       <c r="I49" s="44">
@@ -3126,16 +3173,16 @@
       <c r="X49" s="1"/>
     </row>
     <row r="50" spans="1:24" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="72"/>
-      <c r="B50" s="55"/>
+      <c r="A50" s="81"/>
+      <c r="B50" s="59"/>
       <c r="C50" s="38" t="s">
         <v>137</v>
       </c>
-      <c r="D50" s="57"/>
-      <c r="E50" s="61"/>
-      <c r="F50" s="55"/>
-      <c r="G50" s="55"/>
-      <c r="H50" s="55"/>
+      <c r="D50" s="61"/>
+      <c r="E50" s="65"/>
+      <c r="F50" s="59"/>
+      <c r="G50" s="59"/>
+      <c r="H50" s="59"/>
       <c r="I50" s="44"/>
       <c r="J50" s="45" t="s">
         <v>188</v>
@@ -3156,8 +3203,8 @@
       <c r="X50" s="1"/>
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A51" s="72"/>
-      <c r="B51" s="54"/>
+      <c r="A51" s="81"/>
+      <c r="B51" s="58"/>
       <c r="C51" s="38" t="s">
         <v>138</v>
       </c>
@@ -3198,8 +3245,8 @@
       <c r="X51" s="1"/>
     </row>
     <row r="52" spans="1:24" ht="45" x14ac:dyDescent="0.25">
-      <c r="A52" s="72"/>
-      <c r="B52" s="55"/>
+      <c r="A52" s="81"/>
+      <c r="B52" s="59"/>
       <c r="C52" s="38" t="s">
         <v>139</v>
       </c>
@@ -3240,27 +3287,27 @@
       <c r="X52" s="1"/>
     </row>
     <row r="53" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A53" s="72"/>
-      <c r="B53" s="54"/>
+      <c r="A53" s="81"/>
+      <c r="B53" s="58"/>
       <c r="C53" s="38" t="s">
         <v>140</v>
       </c>
-      <c r="D53" s="56" t="s">
+      <c r="D53" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="E53" s="61" t="s">
+      <c r="E53" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="F53" s="54" t="s">
+      <c r="F53" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="G53" s="54" t="s">
+      <c r="G53" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="H53" s="54" t="s">
+      <c r="H53" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="I53" s="54">
+      <c r="I53" s="58">
         <v>0</v>
       </c>
       <c r="J53" s="45" t="s">
@@ -3282,17 +3329,17 @@
       <c r="X53" s="1"/>
     </row>
     <row r="54" spans="1:24" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="72"/>
-      <c r="B54" s="55"/>
+      <c r="A54" s="81"/>
+      <c r="B54" s="59"/>
       <c r="C54" s="38" t="s">
         <v>141</v>
       </c>
-      <c r="D54" s="57"/>
-      <c r="E54" s="61"/>
-      <c r="F54" s="55"/>
-      <c r="G54" s="55"/>
-      <c r="H54" s="55"/>
-      <c r="I54" s="55"/>
+      <c r="D54" s="61"/>
+      <c r="E54" s="65"/>
+      <c r="F54" s="59"/>
+      <c r="G54" s="59"/>
+      <c r="H54" s="59"/>
+      <c r="I54" s="59"/>
       <c r="J54" s="45" t="s">
         <v>188</v>
       </c>
@@ -3312,8 +3359,8 @@
       <c r="X54" s="1"/>
     </row>
     <row r="55" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A55" s="72"/>
-      <c r="B55" s="54"/>
+      <c r="A55" s="81"/>
+      <c r="B55" s="58"/>
       <c r="C55" s="38" t="s">
         <v>142</v>
       </c>
@@ -3354,8 +3401,8 @@
       <c r="X55" s="1"/>
     </row>
     <row r="56" spans="1:24" ht="45" x14ac:dyDescent="0.25">
-      <c r="A56" s="72"/>
-      <c r="B56" s="55"/>
+      <c r="A56" s="81"/>
+      <c r="B56" s="59"/>
       <c r="C56" s="38" t="s">
         <v>143</v>
       </c>
@@ -3396,27 +3443,27 @@
       <c r="X56" s="1"/>
     </row>
     <row r="57" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A57" s="72"/>
-      <c r="B57" s="54"/>
+      <c r="A57" s="81"/>
+      <c r="B57" s="58"/>
       <c r="C57" s="38" t="s">
         <v>144</v>
       </c>
-      <c r="D57" s="56" t="s">
+      <c r="D57" s="60" t="s">
         <v>50</v>
       </c>
-      <c r="E57" s="61" t="s">
+      <c r="E57" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="F57" s="54" t="s">
+      <c r="F57" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="G57" s="54" t="s">
+      <c r="G57" s="58" t="s">
         <v>41</v>
       </c>
-      <c r="H57" s="54" t="s">
+      <c r="H57" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="I57" s="54">
+      <c r="I57" s="58">
         <v>0</v>
       </c>
       <c r="J57" s="45" t="s">
@@ -3438,17 +3485,17 @@
       <c r="X57" s="1"/>
     </row>
     <row r="58" spans="1:24" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="73"/>
-      <c r="B58" s="55"/>
+      <c r="A58" s="82"/>
+      <c r="B58" s="59"/>
       <c r="C58" s="38" t="s">
         <v>145</v>
       </c>
-      <c r="D58" s="57"/>
-      <c r="E58" s="61"/>
-      <c r="F58" s="55"/>
-      <c r="G58" s="55"/>
-      <c r="H58" s="55"/>
-      <c r="I58" s="55"/>
+      <c r="D58" s="61"/>
+      <c r="E58" s="65"/>
+      <c r="F58" s="59"/>
+      <c r="G58" s="59"/>
+      <c r="H58" s="59"/>
+      <c r="I58" s="59"/>
       <c r="J58" s="45" t="s">
         <v>188</v>
       </c>
@@ -3468,29 +3515,29 @@
       <c r="X58" s="1"/>
     </row>
     <row r="59" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="80" t="s">
+      <c r="A59" s="89" t="s">
         <v>51</v>
       </c>
-      <c r="B59" s="54"/>
+      <c r="B59" s="58"/>
       <c r="C59" s="38" t="s">
         <v>146</v>
       </c>
-      <c r="D59" s="59" t="s">
+      <c r="D59" s="63" t="s">
         <v>34</v>
       </c>
-      <c r="E59" s="54" t="s">
+      <c r="E59" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="F59" s="54">
+      <c r="F59" s="58">
         <v>0</v>
       </c>
-      <c r="G59" s="54">
+      <c r="G59" s="58">
         <v>1</v>
       </c>
-      <c r="H59" s="54" t="s">
+      <c r="H59" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="I59" s="54">
+      <c r="I59" s="58">
         <v>0</v>
       </c>
       <c r="J59" s="45"/>
@@ -3510,17 +3557,17 @@
       <c r="X59" s="1"/>
     </row>
     <row r="60" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="81"/>
-      <c r="B60" s="55"/>
+      <c r="A60" s="90"/>
+      <c r="B60" s="59"/>
       <c r="C60" s="51" t="s">
         <v>147</v>
       </c>
-      <c r="D60" s="60"/>
-      <c r="E60" s="55"/>
-      <c r="F60" s="55"/>
-      <c r="G60" s="55"/>
-      <c r="H60" s="55"/>
-      <c r="I60" s="55"/>
+      <c r="D60" s="64"/>
+      <c r="E60" s="59"/>
+      <c r="F60" s="59"/>
+      <c r="G60" s="59"/>
+      <c r="H60" s="59"/>
+      <c r="I60" s="59"/>
       <c r="J60" s="50" t="s">
         <v>100</v>
       </c>
@@ -3540,30 +3587,30 @@
       <c r="X60" s="1"/>
     </row>
     <row r="61" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="81"/>
-      <c r="B61" s="54"/>
+      <c r="A61" s="90"/>
+      <c r="B61" s="58"/>
       <c r="C61" s="38" t="s">
         <v>148</v>
       </c>
-      <c r="D61" s="59" t="s">
+      <c r="D61" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="E61" s="61" t="s">
+      <c r="E61" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="F61" s="54">
+      <c r="F61" s="58">
         <v>0</v>
       </c>
-      <c r="G61" s="78" t="s">
+      <c r="G61" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="H61" s="54" t="s">
+      <c r="H61" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="I61" s="54">
+      <c r="I61" s="58">
         <v>0</v>
       </c>
-      <c r="J61" s="56" t="s">
+      <c r="J61" s="60" t="s">
         <v>189</v>
       </c>
       <c r="K61" s="3"/>
@@ -3582,18 +3629,18 @@
       <c r="X61" s="1"/>
     </row>
     <row r="62" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A62" s="81"/>
-      <c r="B62" s="55"/>
+      <c r="A62" s="90"/>
+      <c r="B62" s="59"/>
       <c r="C62" s="38" t="s">
         <v>149</v>
       </c>
-      <c r="D62" s="60"/>
-      <c r="E62" s="61"/>
-      <c r="F62" s="55"/>
-      <c r="G62" s="79"/>
-      <c r="H62" s="55"/>
-      <c r="I62" s="55"/>
-      <c r="J62" s="57"/>
+      <c r="D62" s="64"/>
+      <c r="E62" s="65"/>
+      <c r="F62" s="59"/>
+      <c r="G62" s="88"/>
+      <c r="H62" s="59"/>
+      <c r="I62" s="59"/>
+      <c r="J62" s="61"/>
       <c r="K62" s="3"/>
       <c r="L62" s="3"/>
       <c r="M62" s="3"/>
@@ -3610,30 +3657,30 @@
       <c r="X62" s="1"/>
     </row>
     <row r="63" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="81"/>
-      <c r="B63" s="54"/>
+      <c r="A63" s="90"/>
+      <c r="B63" s="58"/>
       <c r="C63" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="D63" s="59" t="s">
+      <c r="D63" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="E63" s="61" t="s">
+      <c r="E63" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="F63" s="54">
+      <c r="F63" s="58">
         <v>0</v>
       </c>
-      <c r="G63" s="54" t="s">
+      <c r="G63" s="58" t="s">
         <v>194</v>
       </c>
-      <c r="H63" s="54" t="s">
+      <c r="H63" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="I63" s="54" t="s">
+      <c r="I63" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="J63" s="56" t="s">
+      <c r="J63" s="60" t="s">
         <v>189</v>
       </c>
       <c r="K63" s="3"/>
@@ -3652,18 +3699,18 @@
       <c r="X63" s="1"/>
     </row>
     <row r="64" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="81"/>
-      <c r="B64" s="55"/>
+      <c r="A64" s="90"/>
+      <c r="B64" s="59"/>
       <c r="C64" s="38" t="s">
         <v>151</v>
       </c>
-      <c r="D64" s="60"/>
-      <c r="E64" s="61"/>
-      <c r="F64" s="55"/>
-      <c r="G64" s="55"/>
-      <c r="H64" s="55"/>
-      <c r="I64" s="55"/>
-      <c r="J64" s="57"/>
+      <c r="D64" s="64"/>
+      <c r="E64" s="65"/>
+      <c r="F64" s="59"/>
+      <c r="G64" s="59"/>
+      <c r="H64" s="59"/>
+      <c r="I64" s="59"/>
+      <c r="J64" s="61"/>
       <c r="K64" s="3"/>
       <c r="L64" s="3"/>
       <c r="M64" s="3"/>
@@ -3680,30 +3727,30 @@
       <c r="X64" s="1"/>
     </row>
     <row r="65" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="81"/>
-      <c r="B65" s="54"/>
+      <c r="A65" s="90"/>
+      <c r="B65" s="58"/>
       <c r="C65" s="38" t="s">
         <v>152</v>
       </c>
-      <c r="D65" s="59" t="s">
+      <c r="D65" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="E65" s="61" t="s">
+      <c r="E65" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="F65" s="54">
+      <c r="F65" s="58">
         <v>0</v>
       </c>
-      <c r="G65" s="78" t="s">
+      <c r="G65" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="H65" s="54" t="s">
+      <c r="H65" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="I65" s="54" t="s">
+      <c r="I65" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="J65" s="56" t="s">
+      <c r="J65" s="60" t="s">
         <v>189</v>
       </c>
       <c r="K65" s="3"/>
@@ -3722,18 +3769,18 @@
       <c r="X65" s="1"/>
     </row>
     <row r="66" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A66" s="81"/>
-      <c r="B66" s="55"/>
+      <c r="A66" s="90"/>
+      <c r="B66" s="59"/>
       <c r="C66" s="38" t="s">
         <v>153</v>
       </c>
-      <c r="D66" s="60"/>
-      <c r="E66" s="61"/>
-      <c r="F66" s="55"/>
-      <c r="G66" s="79"/>
-      <c r="H66" s="55"/>
-      <c r="I66" s="55"/>
-      <c r="J66" s="57"/>
+      <c r="D66" s="64"/>
+      <c r="E66" s="65"/>
+      <c r="F66" s="59"/>
+      <c r="G66" s="88"/>
+      <c r="H66" s="59"/>
+      <c r="I66" s="59"/>
+      <c r="J66" s="61"/>
       <c r="K66" s="3"/>
       <c r="L66" s="3"/>
       <c r="M66" s="3"/>
@@ -3750,30 +3797,30 @@
       <c r="X66" s="1"/>
     </row>
     <row r="67" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="81"/>
-      <c r="B67" s="54"/>
+      <c r="A67" s="90"/>
+      <c r="B67" s="58"/>
       <c r="C67" s="38" t="s">
         <v>154</v>
       </c>
-      <c r="D67" s="59" t="s">
+      <c r="D67" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="E67" s="61" t="s">
+      <c r="E67" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="F67" s="54">
+      <c r="F67" s="58">
         <v>0</v>
       </c>
-      <c r="G67" s="54" t="s">
+      <c r="G67" s="58" t="s">
         <v>194</v>
       </c>
-      <c r="H67" s="54" t="s">
+      <c r="H67" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="I67" s="54" t="s">
+      <c r="I67" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="J67" s="56" t="s">
+      <c r="J67" s="60" t="s">
         <v>189</v>
       </c>
       <c r="K67" s="3"/>
@@ -3792,18 +3839,18 @@
       <c r="X67" s="1"/>
     </row>
     <row r="68" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="81"/>
-      <c r="B68" s="55"/>
+      <c r="A68" s="90"/>
+      <c r="B68" s="59"/>
       <c r="C68" s="38" t="s">
         <v>155</v>
       </c>
-      <c r="D68" s="60"/>
-      <c r="E68" s="61"/>
-      <c r="F68" s="55"/>
-      <c r="G68" s="55"/>
-      <c r="H68" s="55"/>
-      <c r="I68" s="55"/>
-      <c r="J68" s="57"/>
+      <c r="D68" s="64"/>
+      <c r="E68" s="65"/>
+      <c r="F68" s="59"/>
+      <c r="G68" s="59"/>
+      <c r="H68" s="59"/>
+      <c r="I68" s="59"/>
+      <c r="J68" s="61"/>
       <c r="K68" s="3"/>
       <c r="L68" s="3"/>
       <c r="M68" s="3"/>
@@ -3820,30 +3867,30 @@
       <c r="X68" s="1"/>
     </row>
     <row r="69" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="81"/>
-      <c r="B69" s="54"/>
+      <c r="A69" s="90"/>
+      <c r="B69" s="58"/>
       <c r="C69" s="38" t="s">
         <v>156</v>
       </c>
-      <c r="D69" s="59" t="s">
+      <c r="D69" s="63" t="s">
         <v>56</v>
       </c>
-      <c r="E69" s="61" t="s">
+      <c r="E69" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="F69" s="54">
+      <c r="F69" s="58">
         <v>0</v>
       </c>
-      <c r="G69" s="78" t="s">
+      <c r="G69" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="H69" s="54" t="s">
+      <c r="H69" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="I69" s="54" t="s">
+      <c r="I69" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="J69" s="56" t="s">
+      <c r="J69" s="60" t="s">
         <v>189</v>
       </c>
       <c r="K69" s="3"/>
@@ -3862,18 +3909,18 @@
       <c r="X69" s="1"/>
     </row>
     <row r="70" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A70" s="81"/>
-      <c r="B70" s="55"/>
+      <c r="A70" s="90"/>
+      <c r="B70" s="59"/>
       <c r="C70" s="38" t="s">
         <v>157</v>
       </c>
-      <c r="D70" s="60"/>
-      <c r="E70" s="61"/>
-      <c r="F70" s="55"/>
-      <c r="G70" s="79"/>
-      <c r="H70" s="55"/>
-      <c r="I70" s="55"/>
-      <c r="J70" s="57"/>
+      <c r="D70" s="64"/>
+      <c r="E70" s="65"/>
+      <c r="F70" s="59"/>
+      <c r="G70" s="88"/>
+      <c r="H70" s="59"/>
+      <c r="I70" s="59"/>
+      <c r="J70" s="61"/>
       <c r="K70" s="3"/>
       <c r="L70" s="3"/>
       <c r="M70" s="3"/>
@@ -3890,30 +3937,30 @@
       <c r="X70" s="1"/>
     </row>
     <row r="71" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="81"/>
-      <c r="B71" s="54"/>
+      <c r="A71" s="90"/>
+      <c r="B71" s="58"/>
       <c r="C71" s="38" t="s">
         <v>158</v>
       </c>
-      <c r="D71" s="59" t="s">
+      <c r="D71" s="63" t="s">
         <v>57</v>
       </c>
-      <c r="E71" s="61" t="s">
+      <c r="E71" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="F71" s="54">
+      <c r="F71" s="58">
         <v>0</v>
       </c>
-      <c r="G71" s="54" t="s">
+      <c r="G71" s="58" t="s">
         <v>194</v>
       </c>
-      <c r="H71" s="54" t="s">
+      <c r="H71" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="I71" s="54" t="s">
+      <c r="I71" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="J71" s="56" t="s">
+      <c r="J71" s="60" t="s">
         <v>189</v>
       </c>
       <c r="K71" s="3"/>
@@ -3932,18 +3979,18 @@
       <c r="X71" s="1"/>
     </row>
     <row r="72" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="81"/>
-      <c r="B72" s="55"/>
+      <c r="A72" s="90"/>
+      <c r="B72" s="59"/>
       <c r="C72" s="38" t="s">
         <v>159</v>
       </c>
-      <c r="D72" s="60"/>
-      <c r="E72" s="61"/>
-      <c r="F72" s="55"/>
-      <c r="G72" s="55"/>
-      <c r="H72" s="55"/>
-      <c r="I72" s="55"/>
-      <c r="J72" s="57"/>
+      <c r="D72" s="64"/>
+      <c r="E72" s="65"/>
+      <c r="F72" s="59"/>
+      <c r="G72" s="59"/>
+      <c r="H72" s="59"/>
+      <c r="I72" s="59"/>
+      <c r="J72" s="61"/>
       <c r="K72" s="3"/>
       <c r="L72" s="3"/>
       <c r="M72" s="3"/>
@@ -3960,30 +4007,30 @@
       <c r="X72" s="1"/>
     </row>
     <row r="73" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="81"/>
-      <c r="B73" s="54"/>
+      <c r="A73" s="90"/>
+      <c r="B73" s="58"/>
       <c r="C73" s="38" t="s">
         <v>160</v>
       </c>
-      <c r="D73" s="59" t="s">
+      <c r="D73" s="63" t="s">
         <v>58</v>
       </c>
-      <c r="E73" s="61" t="s">
+      <c r="E73" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="F73" s="54">
+      <c r="F73" s="58">
         <v>0</v>
       </c>
-      <c r="G73" s="78" t="s">
+      <c r="G73" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="H73" s="54" t="s">
+      <c r="H73" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="I73" s="54" t="s">
+      <c r="I73" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="J73" s="56" t="s">
+      <c r="J73" s="60" t="s">
         <v>189</v>
       </c>
       <c r="K73" s="3"/>
@@ -4002,18 +4049,18 @@
       <c r="X73" s="1"/>
     </row>
     <row r="74" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A74" s="81"/>
-      <c r="B74" s="55"/>
+      <c r="A74" s="90"/>
+      <c r="B74" s="59"/>
       <c r="C74" s="38" t="s">
         <v>161</v>
       </c>
-      <c r="D74" s="60"/>
-      <c r="E74" s="61"/>
-      <c r="F74" s="55"/>
-      <c r="G74" s="79"/>
-      <c r="H74" s="55"/>
-      <c r="I74" s="55"/>
-      <c r="J74" s="57"/>
+      <c r="D74" s="64"/>
+      <c r="E74" s="65"/>
+      <c r="F74" s="59"/>
+      <c r="G74" s="88"/>
+      <c r="H74" s="59"/>
+      <c r="I74" s="59"/>
+      <c r="J74" s="61"/>
       <c r="K74" s="3"/>
       <c r="L74" s="3"/>
       <c r="M74" s="3"/>
@@ -4030,30 +4077,30 @@
       <c r="X74" s="1"/>
     </row>
     <row r="75" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="81"/>
-      <c r="B75" s="54"/>
+      <c r="A75" s="90"/>
+      <c r="B75" s="58"/>
       <c r="C75" s="38" t="s">
         <v>162</v>
       </c>
-      <c r="D75" s="59" t="s">
+      <c r="D75" s="63" t="s">
         <v>102</v>
       </c>
-      <c r="E75" s="61" t="s">
+      <c r="E75" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="F75" s="54">
+      <c r="F75" s="58">
         <v>0</v>
       </c>
-      <c r="G75" s="54" t="s">
+      <c r="G75" s="58" t="s">
         <v>194</v>
       </c>
-      <c r="H75" s="54" t="s">
+      <c r="H75" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="I75" s="54" t="s">
+      <c r="I75" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="J75" s="56" t="s">
+      <c r="J75" s="60" t="s">
         <v>189</v>
       </c>
       <c r="K75" s="3"/>
@@ -4072,18 +4119,18 @@
       <c r="X75" s="1"/>
     </row>
     <row r="76" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="81"/>
-      <c r="B76" s="55"/>
+      <c r="A76" s="90"/>
+      <c r="B76" s="59"/>
       <c r="C76" s="38" t="s">
         <v>163</v>
       </c>
-      <c r="D76" s="60"/>
-      <c r="E76" s="61"/>
-      <c r="F76" s="55"/>
-      <c r="G76" s="55"/>
-      <c r="H76" s="55"/>
-      <c r="I76" s="55"/>
-      <c r="J76" s="57"/>
+      <c r="D76" s="64"/>
+      <c r="E76" s="65"/>
+      <c r="F76" s="59"/>
+      <c r="G76" s="59"/>
+      <c r="H76" s="59"/>
+      <c r="I76" s="59"/>
+      <c r="J76" s="61"/>
       <c r="K76" s="3"/>
       <c r="L76" s="3"/>
       <c r="M76" s="3"/>
@@ -4100,30 +4147,30 @@
       <c r="X76" s="1"/>
     </row>
     <row r="77" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="81"/>
-      <c r="B77" s="54"/>
+      <c r="A77" s="90"/>
+      <c r="B77" s="58"/>
       <c r="C77" s="38" t="s">
         <v>164</v>
       </c>
-      <c r="D77" s="59" t="s">
+      <c r="D77" s="63" t="s">
         <v>103</v>
       </c>
-      <c r="E77" s="61" t="s">
+      <c r="E77" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="F77" s="54">
+      <c r="F77" s="58">
         <v>0</v>
       </c>
-      <c r="G77" s="78" t="s">
+      <c r="G77" s="87" t="s">
         <v>101</v>
       </c>
-      <c r="H77" s="54" t="s">
+      <c r="H77" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="I77" s="54" t="s">
+      <c r="I77" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="J77" s="56" t="s">
+      <c r="J77" s="60" t="s">
         <v>189</v>
       </c>
       <c r="K77" s="3"/>
@@ -4142,18 +4189,18 @@
       <c r="X77" s="1"/>
     </row>
     <row r="78" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="82"/>
-      <c r="B78" s="83"/>
+      <c r="A78" s="91"/>
+      <c r="B78" s="92"/>
       <c r="C78" s="38" t="s">
         <v>165</v>
       </c>
-      <c r="D78" s="60"/>
-      <c r="E78" s="61"/>
-      <c r="F78" s="55"/>
-      <c r="G78" s="79"/>
-      <c r="H78" s="55"/>
-      <c r="I78" s="55"/>
-      <c r="J78" s="57"/>
+      <c r="D78" s="64"/>
+      <c r="E78" s="65"/>
+      <c r="F78" s="59"/>
+      <c r="G78" s="88"/>
+      <c r="H78" s="59"/>
+      <c r="I78" s="59"/>
+      <c r="J78" s="61"/>
       <c r="K78" s="3"/>
       <c r="L78" s="3"/>
       <c r="M78" s="3"/>
@@ -4170,29 +4217,29 @@
       <c r="X78" s="1"/>
     </row>
     <row r="79" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="67" t="s">
+      <c r="A79" s="78" t="s">
         <v>85</v>
       </c>
-      <c r="B79" s="54"/>
+      <c r="B79" s="58"/>
       <c r="C79" s="43" t="s">
         <v>166</v>
       </c>
-      <c r="D79" s="59" t="s">
+      <c r="D79" s="63" t="s">
         <v>60</v>
       </c>
-      <c r="E79" s="61" t="s">
+      <c r="E79" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="F79" s="54">
+      <c r="F79" s="58">
         <v>0</v>
       </c>
-      <c r="G79" s="54">
+      <c r="G79" s="58">
         <v>255</v>
       </c>
-      <c r="H79" s="54" t="s">
+      <c r="H79" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="I79" s="54">
+      <c r="I79" s="58">
         <v>0</v>
       </c>
       <c r="J79" s="52" t="s">
@@ -4214,17 +4261,17 @@
       <c r="X79" s="1"/>
     </row>
     <row r="80" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A80" s="68"/>
-      <c r="B80" s="55"/>
+      <c r="A80" s="79"/>
+      <c r="B80" s="59"/>
       <c r="C80" s="51" t="s">
         <v>167</v>
       </c>
-      <c r="D80" s="60"/>
-      <c r="E80" s="61"/>
-      <c r="F80" s="55"/>
-      <c r="G80" s="55"/>
-      <c r="H80" s="55"/>
-      <c r="I80" s="55"/>
+      <c r="D80" s="64"/>
+      <c r="E80" s="65"/>
+      <c r="F80" s="59"/>
+      <c r="G80" s="59"/>
+      <c r="H80" s="59"/>
+      <c r="I80" s="59"/>
       <c r="J80" s="53" t="s">
         <v>100</v>
       </c>
@@ -4244,8 +4291,8 @@
       <c r="X80" s="1"/>
     </row>
     <row r="81" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="68"/>
-      <c r="B81" s="54"/>
+      <c r="A81" s="79"/>
+      <c r="B81" s="58"/>
       <c r="C81" s="38" t="s">
         <v>168</v>
       </c>
@@ -4284,8 +4331,8 @@
       <c r="X81" s="1"/>
     </row>
     <row r="82" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A82" s="68"/>
-      <c r="B82" s="55"/>
+      <c r="A82" s="79"/>
+      <c r="B82" s="59"/>
       <c r="C82" s="38" t="s">
         <v>169</v>
       </c>
@@ -4322,30 +4369,30 @@
       <c r="X82" s="1"/>
     </row>
     <row r="83" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A83" s="68"/>
-      <c r="B83" s="54"/>
+      <c r="A83" s="79"/>
+      <c r="B83" s="58"/>
       <c r="C83" s="38" t="s">
         <v>170</v>
       </c>
-      <c r="D83" s="70" t="s">
+      <c r="D83" s="83" t="s">
         <v>63</v>
       </c>
-      <c r="E83" s="61" t="s">
+      <c r="E83" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="F83" s="61">
+      <c r="F83" s="65">
         <v>0</v>
       </c>
-      <c r="G83" s="61">
+      <c r="G83" s="65">
         <v>65535</v>
       </c>
-      <c r="H83" s="61" t="s">
+      <c r="H83" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="I83" s="54">
+      <c r="I83" s="58">
         <v>1</v>
       </c>
-      <c r="J83" s="56" t="s">
+      <c r="J83" s="60" t="s">
         <v>186</v>
       </c>
       <c r="K83" s="3"/>
@@ -4364,18 +4411,18 @@
       <c r="X83" s="1"/>
     </row>
     <row r="84" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="68"/>
-      <c r="B84" s="55"/>
+      <c r="A84" s="79"/>
+      <c r="B84" s="59"/>
       <c r="C84" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="D84" s="70"/>
-      <c r="E84" s="61"/>
-      <c r="F84" s="61"/>
-      <c r="G84" s="61"/>
-      <c r="H84" s="61"/>
-      <c r="I84" s="55"/>
-      <c r="J84" s="57"/>
+      <c r="D84" s="83"/>
+      <c r="E84" s="65"/>
+      <c r="F84" s="65"/>
+      <c r="G84" s="65"/>
+      <c r="H84" s="65"/>
+      <c r="I84" s="59"/>
+      <c r="J84" s="61"/>
       <c r="K84" s="3"/>
       <c r="L84" s="3"/>
       <c r="M84" s="3"/>
@@ -4392,30 +4439,30 @@
       <c r="X84" s="1"/>
     </row>
     <row r="85" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="68"/>
-      <c r="B85" s="54"/>
+      <c r="A85" s="79"/>
+      <c r="B85" s="58"/>
       <c r="C85" s="38" t="s">
         <v>172</v>
       </c>
-      <c r="D85" s="70" t="s">
+      <c r="D85" s="83" t="s">
         <v>64</v>
       </c>
-      <c r="E85" s="61" t="s">
+      <c r="E85" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="F85" s="61">
+      <c r="F85" s="65">
         <v>0</v>
       </c>
-      <c r="G85" s="61" t="s">
+      <c r="G85" s="65" t="s">
         <v>67</v>
       </c>
-      <c r="H85" s="61" t="s">
+      <c r="H85" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="I85" s="54">
+      <c r="I85" s="58">
         <v>1</v>
       </c>
-      <c r="J85" s="56" t="s">
+      <c r="J85" s="60" t="s">
         <v>186</v>
       </c>
       <c r="K85" s="3"/>
@@ -4434,18 +4481,18 @@
       <c r="X85" s="1"/>
     </row>
     <row r="86" spans="1:24" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="68"/>
-      <c r="B86" s="55"/>
+      <c r="A86" s="79"/>
+      <c r="B86" s="59"/>
       <c r="C86" s="38" t="s">
         <v>173</v>
       </c>
-      <c r="D86" s="70"/>
-      <c r="E86" s="61"/>
-      <c r="F86" s="61"/>
-      <c r="G86" s="61"/>
-      <c r="H86" s="61"/>
-      <c r="I86" s="55"/>
-      <c r="J86" s="57"/>
+      <c r="D86" s="83"/>
+      <c r="E86" s="65"/>
+      <c r="F86" s="65"/>
+      <c r="G86" s="65"/>
+      <c r="H86" s="65"/>
+      <c r="I86" s="59"/>
+      <c r="J86" s="61"/>
       <c r="K86" s="34"/>
       <c r="L86" s="34"/>
       <c r="M86" s="34"/>
@@ -4462,28 +4509,28 @@
       <c r="X86" s="1"/>
     </row>
     <row r="87" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="68"/>
-      <c r="B87" s="54"/>
+      <c r="A87" s="79"/>
+      <c r="B87" s="58"/>
       <c r="C87" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="D87" s="70" t="s">
+      <c r="D87" s="83" t="s">
         <v>66</v>
       </c>
-      <c r="E87" s="61" t="s">
+      <c r="E87" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="F87" s="61" t="s">
+      <c r="F87" s="65" t="s">
         <v>68</v>
       </c>
-      <c r="G87" s="61" t="s">
+      <c r="G87" s="65" t="s">
         <v>69</v>
       </c>
-      <c r="H87" s="61" t="s">
+      <c r="H87" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="I87" s="54"/>
-      <c r="J87" s="62" t="s">
+      <c r="I87" s="58"/>
+      <c r="J87" s="67" t="s">
         <v>89</v>
       </c>
       <c r="K87" s="34"/>
@@ -4502,18 +4549,18 @@
       <c r="X87" s="1"/>
     </row>
     <row r="88" spans="1:24" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="68"/>
-      <c r="B88" s="55"/>
+      <c r="A88" s="79"/>
+      <c r="B88" s="59"/>
       <c r="C88" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="D88" s="70"/>
-      <c r="E88" s="61"/>
-      <c r="F88" s="61"/>
-      <c r="G88" s="61"/>
-      <c r="H88" s="61"/>
-      <c r="I88" s="55"/>
-      <c r="J88" s="62"/>
+      <c r="D88" s="83"/>
+      <c r="E88" s="65"/>
+      <c r="F88" s="65"/>
+      <c r="G88" s="65"/>
+      <c r="H88" s="65"/>
+      <c r="I88" s="59"/>
+      <c r="J88" s="67"/>
       <c r="K88" s="34"/>
       <c r="L88" s="34"/>
       <c r="M88" s="34"/>
@@ -4530,28 +4577,28 @@
       <c r="X88" s="1"/>
     </row>
     <row r="89" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A89" s="68"/>
-      <c r="B89" s="54"/>
+      <c r="A89" s="79"/>
+      <c r="B89" s="58"/>
       <c r="C89" s="38" t="s">
         <v>176</v>
       </c>
-      <c r="D89" s="70" t="s">
+      <c r="D89" s="83" t="s">
         <v>65</v>
       </c>
-      <c r="E89" s="61" t="s">
+      <c r="E89" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="F89" s="61" t="s">
+      <c r="F89" s="65" t="s">
         <v>68</v>
       </c>
-      <c r="G89" s="61" t="s">
+      <c r="G89" s="65" t="s">
         <v>69</v>
       </c>
-      <c r="H89" s="61" t="s">
+      <c r="H89" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="I89" s="54"/>
-      <c r="J89" s="62" t="s">
+      <c r="I89" s="58"/>
+      <c r="J89" s="67" t="s">
         <v>90</v>
       </c>
       <c r="K89" s="34"/>
@@ -4570,18 +4617,18 @@
       <c r="X89" s="1"/>
     </row>
     <row r="90" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A90" s="69"/>
-      <c r="B90" s="55"/>
+      <c r="A90" s="80"/>
+      <c r="B90" s="59"/>
       <c r="C90" s="38" t="s">
         <v>177</v>
       </c>
-      <c r="D90" s="70"/>
-      <c r="E90" s="61"/>
-      <c r="F90" s="61"/>
-      <c r="G90" s="61"/>
-      <c r="H90" s="61"/>
-      <c r="I90" s="55"/>
-      <c r="J90" s="62"/>
+      <c r="D90" s="83"/>
+      <c r="E90" s="65"/>
+      <c r="F90" s="65"/>
+      <c r="G90" s="65"/>
+      <c r="H90" s="65"/>
+      <c r="I90" s="59"/>
+      <c r="J90" s="67"/>
       <c r="K90" s="3"/>
       <c r="L90" s="3"/>
       <c r="M90" s="3"/>
@@ -58135,8 +58182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E20" sqref="E20:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -58149,112 +58196,112 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="95" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="61">
+      <c r="B1" s="65">
         <v>1</v>
       </c>
       <c r="C1" s="19">
         <v>1</v>
       </c>
-      <c r="D1" s="62" t="s">
+      <c r="D1" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="61" t="s">
+      <c r="E1" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61" t="s">
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="86"/>
-      <c r="B2" s="61"/>
+      <c r="A2" s="95"/>
+      <c r="B2" s="65"/>
       <c r="C2" s="19">
         <v>2</v>
       </c>
-      <c r="D2" s="62"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="86"/>
-      <c r="B3" s="61">
+      <c r="A3" s="95"/>
+      <c r="B3" s="65">
         <v>2</v>
       </c>
       <c r="C3" s="19">
         <v>3</v>
       </c>
-      <c r="D3" s="62" t="s">
+      <c r="D3" s="67" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="61" t="s">
+      <c r="E3" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="61"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61" t="s">
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="65" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="86"/>
-      <c r="B4" s="61"/>
+      <c r="A4" s="95"/>
+      <c r="B4" s="65"/>
       <c r="C4" s="19">
         <v>4</v>
       </c>
-      <c r="D4" s="62"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="65"/>
+      <c r="F4" s="65"/>
+      <c r="G4" s="65"/>
+      <c r="H4" s="65"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="86"/>
-      <c r="B5" s="61">
+      <c r="A5" s="95"/>
+      <c r="B5" s="65">
         <v>3</v>
       </c>
       <c r="C5" s="19">
         <v>5</v>
       </c>
-      <c r="D5" s="62" t="s">
+      <c r="D5" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="61" t="s">
+      <c r="E5" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="61"/>
-      <c r="G5" s="61"/>
-      <c r="H5" s="61" t="s">
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="86"/>
-      <c r="B6" s="61"/>
+      <c r="A6" s="95"/>
+      <c r="B6" s="65"/>
       <c r="C6" s="19">
         <v>6</v>
       </c>
-      <c r="D6" s="62"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="61"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="65"/>
+      <c r="H6" s="65"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="86"/>
+      <c r="A7" s="95"/>
       <c r="B7" s="75">
         <v>4</v>
       </c>
       <c r="C7" s="20">
         <v>7</v>
       </c>
-      <c r="D7" s="76" t="s">
+      <c r="D7" s="84" t="s">
         <v>28</v>
       </c>
       <c r="E7" s="75" t="s">
@@ -58267,86 +58314,86 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="86"/>
+      <c r="A8" s="95"/>
       <c r="B8" s="75"/>
       <c r="C8" s="20">
         <v>8</v>
       </c>
-      <c r="D8" s="76"/>
+      <c r="D8" s="84"/>
       <c r="E8" s="75"/>
       <c r="F8" s="75"/>
       <c r="G8" s="75"/>
       <c r="H8" s="75"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="86"/>
-      <c r="B9" s="61">
+      <c r="A9" s="95"/>
+      <c r="B9" s="65">
         <v>5</v>
       </c>
       <c r="C9" s="19">
         <v>9</v>
       </c>
-      <c r="D9" s="85" t="s">
+      <c r="D9" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="61" t="s">
+      <c r="E9" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="61"/>
-      <c r="G9" s="61"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="65"/>
       <c r="H9" s="19"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="86"/>
-      <c r="B10" s="61"/>
+      <c r="A10" s="95"/>
+      <c r="B10" s="65"/>
       <c r="C10" s="19">
         <v>10</v>
       </c>
-      <c r="D10" s="85"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="61"/>
-      <c r="G10" s="61"/>
+      <c r="D10" s="94"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="65"/>
       <c r="H10" s="19" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="84"/>
-      <c r="B11" s="61">
+      <c r="A11" s="93"/>
+      <c r="B11" s="65">
         <v>6</v>
       </c>
       <c r="C11" s="19">
         <v>11</v>
       </c>
-      <c r="D11" s="62" t="s">
+      <c r="D11" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="61" t="s">
+      <c r="E11" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="61"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="61" t="s">
+      <c r="F11" s="65"/>
+      <c r="G11" s="65"/>
+      <c r="H11" s="65" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="84"/>
-      <c r="B12" s="61"/>
+      <c r="A12" s="93"/>
+      <c r="B12" s="65"/>
       <c r="C12" s="19">
         <v>12</v>
       </c>
-      <c r="D12" s="62"/>
-      <c r="E12" s="61"/>
-      <c r="F12" s="61"/>
-      <c r="G12" s="61"/>
-      <c r="H12" s="61"/>
+      <c r="D12" s="67"/>
+      <c r="E12" s="65"/>
+      <c r="F12" s="65"/>
+      <c r="G12" s="65"/>
+      <c r="H12" s="65"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="84" t="s">
+      <c r="A14" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="84"/>
+      <c r="B14" s="93"/>
       <c r="C14" s="25" t="s">
         <v>9</v>
       </c>
@@ -58511,10 +58558,10 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="61" t="s">
+      <c r="A33" s="65" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="61"/>
+      <c r="B33" s="65"/>
       <c r="C33" s="32" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
added classes for reading and writing device config via modbus
</commit_message>
<xml_diff>
--- a/Карта конфигурации.xlsx
+++ b/Карта конфигурации.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="209">
   <si>
     <t>програмный модуль</t>
   </si>
@@ -645,6 +645,9 @@
   <si>
     <t>26-31</t>
   </si>
+  <si>
+    <t>c 1014</t>
+  </si>
 </sst>
 </file>
 
@@ -851,7 +854,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1016,24 +1019,23 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1044,50 +1046,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1109,12 +1070,63 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1124,21 +1136,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1446,10 +1468,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:X11988"/>
+  <dimension ref="A1:X11989"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17:J30"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1467,18 +1489,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="92" t="s">
+      <c r="A1" s="65" t="s">
         <v>191</v>
       </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="92"/>
-      <c r="J1" s="92"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
+      <c r="H1" s="65"/>
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B2" s="26"/>
@@ -1488,15 +1510,15 @@
       <c r="A3" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="70">
+      <c r="B3" s="89">
         <v>1000</v>
       </c>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
+      <c r="C3" s="89"/>
+      <c r="D3" s="89"/>
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="89"/>
       <c r="I3" s="47"/>
       <c r="J3" s="49"/>
       <c r="K3" s="2"/>
@@ -1559,28 +1581,28 @@
       <c r="X4" s="1"/>
     </row>
     <row r="5" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="88" t="s">
+      <c r="A5" s="74" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="71">
+      <c r="B5" s="77">
         <v>0</v>
       </c>
       <c r="C5" s="54">
         <v>0</v>
       </c>
-      <c r="D5" s="72" t="s">
+      <c r="D5" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="71" t="s">
+      <c r="E5" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71" t="s">
+      <c r="F5" s="77"/>
+      <c r="G5" s="77"/>
+      <c r="H5" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="86"/>
-      <c r="J5" s="72" t="s">
+      <c r="I5" s="72"/>
+      <c r="J5" s="69" t="s">
         <v>173</v>
       </c>
       <c r="K5" s="3"/>
@@ -1599,18 +1621,18 @@
       <c r="X5" s="1"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="88"/>
-      <c r="B6" s="71"/>
+      <c r="A6" s="74"/>
+      <c r="B6" s="77"/>
       <c r="C6" s="54">
         <v>1</v>
       </c>
-      <c r="D6" s="72"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="71"/>
-      <c r="H6" s="71"/>
-      <c r="I6" s="87"/>
-      <c r="J6" s="72"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="77"/>
+      <c r="F6" s="77"/>
+      <c r="G6" s="77"/>
+      <c r="H6" s="77"/>
+      <c r="I6" s="73"/>
+      <c r="J6" s="69"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
@@ -1627,26 +1649,28 @@
       <c r="X6" s="1"/>
     </row>
     <row r="7" spans="1:24" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="88"/>
-      <c r="B7" s="67">
+      <c r="A7" s="74"/>
+      <c r="B7" s="68">
         <v>1</v>
       </c>
       <c r="C7" s="38">
         <v>2</v>
       </c>
-      <c r="D7" s="64" t="s">
+      <c r="D7" s="90" t="s">
         <v>91</v>
       </c>
-      <c r="E7" s="67" t="s">
+      <c r="E7" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="67"/>
-      <c r="G7" s="67"/>
-      <c r="H7" s="67" t="s">
+      <c r="F7" s="68">
+        <v>1</v>
+      </c>
+      <c r="G7" s="68"/>
+      <c r="H7" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="84"/>
-      <c r="J7" s="90" t="s">
+      <c r="I7" s="70"/>
+      <c r="J7" s="76" t="s">
         <v>92</v>
       </c>
       <c r="K7" s="3"/>
@@ -1665,18 +1689,18 @@
       <c r="X7" s="1"/>
     </row>
     <row r="8" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="88"/>
-      <c r="B8" s="67"/>
+      <c r="A8" s="74"/>
+      <c r="B8" s="68"/>
       <c r="C8" s="38">
         <v>3</v>
       </c>
-      <c r="D8" s="64"/>
-      <c r="E8" s="67"/>
-      <c r="F8" s="67"/>
-      <c r="G8" s="67"/>
-      <c r="H8" s="67"/>
-      <c r="I8" s="85"/>
-      <c r="J8" s="90"/>
+      <c r="D8" s="90"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="68"/>
+      <c r="H8" s="68"/>
+      <c r="I8" s="71"/>
+      <c r="J8" s="76"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
@@ -1693,26 +1717,26 @@
       <c r="X8" s="1"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9" s="88"/>
-      <c r="B9" s="67">
+      <c r="A9" s="74"/>
+      <c r="B9" s="68">
         <v>2</v>
       </c>
       <c r="C9" s="38">
         <v>4</v>
       </c>
-      <c r="D9" s="64" t="s">
+      <c r="D9" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="67" t="s">
+      <c r="E9" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="67"/>
-      <c r="G9" s="67"/>
-      <c r="H9" s="67" t="s">
+      <c r="F9" s="68"/>
+      <c r="G9" s="68"/>
+      <c r="H9" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="84"/>
-      <c r="J9" s="90" t="s">
+      <c r="I9" s="70"/>
+      <c r="J9" s="76" t="s">
         <v>95</v>
       </c>
       <c r="K9" s="3"/>
@@ -1731,18 +1755,18 @@
       <c r="X9" s="1"/>
     </row>
     <row r="10" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="88"/>
-      <c r="B10" s="67"/>
+      <c r="A10" s="74"/>
+      <c r="B10" s="68"/>
       <c r="C10" s="38">
         <v>5</v>
       </c>
-      <c r="D10" s="64"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="67"/>
-      <c r="H10" s="67"/>
-      <c r="I10" s="85"/>
-      <c r="J10" s="90"/>
+      <c r="D10" s="90"/>
+      <c r="E10" s="68"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="68"/>
+      <c r="H10" s="68"/>
+      <c r="I10" s="71"/>
+      <c r="J10" s="76"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
@@ -1759,26 +1783,26 @@
       <c r="X10" s="1"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" s="88"/>
-      <c r="B11" s="73">
+      <c r="A11" s="74"/>
+      <c r="B11" s="79">
         <v>3</v>
       </c>
       <c r="C11" s="55">
         <v>6</v>
       </c>
-      <c r="D11" s="91" t="s">
+      <c r="D11" s="78" t="s">
         <v>190</v>
       </c>
-      <c r="E11" s="73" t="s">
+      <c r="E11" s="79" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="73"/>
-      <c r="G11" s="73"/>
-      <c r="H11" s="96" t="s">
+      <c r="F11" s="79"/>
+      <c r="G11" s="79"/>
+      <c r="H11" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="84"/>
-      <c r="J11" s="90" t="s">
+      <c r="I11" s="70"/>
+      <c r="J11" s="76" t="s">
         <v>93</v>
       </c>
       <c r="K11" s="3"/>
@@ -1797,18 +1821,18 @@
       <c r="X11" s="1"/>
     </row>
     <row r="12" spans="1:24" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="88"/>
-      <c r="B12" s="73"/>
+      <c r="A12" s="74"/>
+      <c r="B12" s="79"/>
       <c r="C12" s="55">
         <v>7</v>
       </c>
-      <c r="D12" s="91"/>
-      <c r="E12" s="73"/>
-      <c r="F12" s="73"/>
-      <c r="G12" s="73"/>
-      <c r="H12" s="96"/>
-      <c r="I12" s="85"/>
-      <c r="J12" s="90"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="79"/>
+      <c r="F12" s="79"/>
+      <c r="G12" s="79"/>
+      <c r="H12" s="91"/>
+      <c r="I12" s="71"/>
+      <c r="J12" s="76"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
@@ -1825,25 +1849,25 @@
       <c r="X12" s="1"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A13" s="88"/>
-      <c r="B13" s="67">
+      <c r="A13" s="74"/>
+      <c r="B13" s="68">
         <v>4</v>
       </c>
       <c r="C13" s="38">
         <v>8</v>
       </c>
-      <c r="D13" s="91" t="s">
+      <c r="D13" s="78" t="s">
         <v>90</v>
       </c>
-      <c r="E13" s="67" t="s">
+      <c r="E13" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="67"/>
-      <c r="G13" s="67"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="68"/>
       <c r="H13" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="84"/>
+      <c r="I13" s="70"/>
       <c r="J13" s="45"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
@@ -1861,17 +1885,17 @@
       <c r="X13" s="1"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A14" s="88"/>
-      <c r="B14" s="67"/>
+      <c r="A14" s="74"/>
+      <c r="B14" s="68"/>
       <c r="C14" s="38">
         <v>9</v>
       </c>
-      <c r="D14" s="91"/>
-      <c r="E14" s="67"/>
-      <c r="F14" s="67"/>
-      <c r="G14" s="67"/>
-      <c r="H14" s="63"/>
-      <c r="I14" s="85"/>
+      <c r="D14" s="78"/>
+      <c r="E14" s="68"/>
+      <c r="F14" s="68"/>
+      <c r="G14" s="68"/>
+      <c r="H14" s="62"/>
+      <c r="I14" s="71"/>
       <c r="J14" s="45"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
@@ -1889,26 +1913,26 @@
       <c r="X14" s="1"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A15" s="89"/>
-      <c r="B15" s="100" t="s">
+      <c r="A15" s="75"/>
+      <c r="B15" s="88" t="s">
         <v>203</v>
       </c>
       <c r="C15" s="54">
         <v>10.11</v>
       </c>
-      <c r="D15" s="72" t="s">
+      <c r="D15" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="71" t="s">
+      <c r="E15" s="77" t="s">
         <v>195</v>
       </c>
-      <c r="F15" s="71"/>
-      <c r="G15" s="71"/>
-      <c r="H15" s="71" t="s">
+      <c r="F15" s="77"/>
+      <c r="G15" s="77"/>
+      <c r="H15" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="I15" s="86"/>
-      <c r="J15" s="72" t="s">
+      <c r="I15" s="72"/>
+      <c r="J15" s="69" t="s">
         <v>173</v>
       </c>
       <c r="K15" s="3"/>
@@ -1927,18 +1951,18 @@
       <c r="X15" s="1"/>
     </row>
     <row r="16" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="89"/>
-      <c r="B16" s="71"/>
+      <c r="A16" s="75"/>
+      <c r="B16" s="77"/>
       <c r="C16" s="54">
         <v>12.13</v>
       </c>
-      <c r="D16" s="72"/>
-      <c r="E16" s="71"/>
-      <c r="F16" s="71"/>
-      <c r="G16" s="71"/>
-      <c r="H16" s="71"/>
-      <c r="I16" s="87"/>
-      <c r="J16" s="72"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="77"/>
+      <c r="F16" s="77"/>
+      <c r="G16" s="77"/>
+      <c r="H16" s="77"/>
+      <c r="I16" s="73"/>
+      <c r="J16" s="69"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
@@ -1955,10 +1979,10 @@
       <c r="X16" s="1"/>
     </row>
     <row r="17" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="79" t="s">
+      <c r="A17" s="80" t="s">
         <v>84</v>
       </c>
-      <c r="B17" s="71">
+      <c r="B17" s="77">
         <v>1</v>
       </c>
       <c r="C17" s="54" t="s">
@@ -2001,8 +2025,8 @@
       <c r="X17" s="1"/>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A18" s="80"/>
-      <c r="B18" s="71"/>
+      <c r="A18" s="81"/>
+      <c r="B18" s="77"/>
       <c r="C18" s="54" t="s">
         <v>99</v>
       </c>
@@ -2041,29 +2065,29 @@
       <c r="X18" s="1"/>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A19" s="80"/>
-      <c r="B19" s="71">
+      <c r="A19" s="81"/>
+      <c r="B19" s="77">
         <v>2</v>
       </c>
       <c r="C19" s="54" t="s">
         <v>100</v>
       </c>
-      <c r="D19" s="72" t="s">
+      <c r="D19" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="71" t="s">
+      <c r="E19" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="F19" s="71">
+      <c r="F19" s="77">
         <v>1200</v>
       </c>
-      <c r="G19" s="71">
+      <c r="G19" s="77">
         <v>57600</v>
       </c>
-      <c r="H19" s="71" t="s">
+      <c r="H19" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="I19" s="86">
+      <c r="I19" s="72">
         <v>9600</v>
       </c>
       <c r="J19" s="56"/>
@@ -2083,17 +2107,17 @@
       <c r="X19" s="1"/>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A20" s="80"/>
-      <c r="B20" s="71"/>
+      <c r="A20" s="81"/>
+      <c r="B20" s="77"/>
       <c r="C20" s="54" t="s">
         <v>101</v>
       </c>
-      <c r="D20" s="72"/>
-      <c r="E20" s="71"/>
-      <c r="F20" s="71"/>
-      <c r="G20" s="71"/>
-      <c r="H20" s="71"/>
-      <c r="I20" s="87"/>
+      <c r="D20" s="69"/>
+      <c r="E20" s="77"/>
+      <c r="F20" s="77"/>
+      <c r="G20" s="77"/>
+      <c r="H20" s="77"/>
+      <c r="I20" s="73"/>
       <c r="J20" s="56"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
@@ -2111,8 +2135,8 @@
       <c r="X20" s="1"/>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A21" s="80"/>
-      <c r="B21" s="71">
+      <c r="A21" s="81"/>
+      <c r="B21" s="77">
         <v>3</v>
       </c>
       <c r="C21" s="54" t="s">
@@ -2134,7 +2158,7 @@
         <v>13</v>
       </c>
       <c r="I21" s="57">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J21" s="56"/>
       <c r="K21" s="3"/>
@@ -2153,8 +2177,8 @@
       <c r="X21" s="1"/>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A22" s="80"/>
-      <c r="B22" s="71"/>
+      <c r="A22" s="81"/>
+      <c r="B22" s="77"/>
       <c r="C22" s="54" t="s">
         <v>103</v>
       </c>
@@ -2195,8 +2219,8 @@
       <c r="X22" s="1"/>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A23" s="80"/>
-      <c r="B23" s="71">
+      <c r="A23" s="81"/>
+      <c r="B23" s="77">
         <v>4</v>
       </c>
       <c r="C23" s="54" t="s">
@@ -2237,8 +2261,8 @@
       <c r="X23" s="1"/>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A24" s="80"/>
-      <c r="B24" s="71"/>
+      <c r="A24" s="81"/>
+      <c r="B24" s="77"/>
       <c r="C24" s="54" t="s">
         <v>105</v>
       </c>
@@ -2279,8 +2303,8 @@
       <c r="X24" s="1"/>
     </row>
     <row r="25" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="80"/>
-      <c r="B25" s="71">
+      <c r="A25" s="81"/>
+      <c r="B25" s="77">
         <v>5</v>
       </c>
       <c r="C25" s="54" t="s">
@@ -2323,30 +2347,30 @@
       <c r="X25" s="1"/>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A26" s="80"/>
-      <c r="B26" s="71"/>
+      <c r="A26" s="81"/>
+      <c r="B26" s="77"/>
       <c r="C26" s="54" t="s">
         <v>107</v>
       </c>
-      <c r="D26" s="101" t="s">
+      <c r="D26" s="86" t="s">
         <v>30</v>
       </c>
-      <c r="E26" s="71" t="s">
+      <c r="E26" s="77" t="s">
         <v>10</v>
       </c>
-      <c r="F26" s="86">
+      <c r="F26" s="72">
         <v>0</v>
       </c>
-      <c r="G26" s="86">
+      <c r="G26" s="72">
         <v>65535</v>
       </c>
       <c r="H26" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="I26" s="86">
+      <c r="I26" s="72">
         <v>200</v>
       </c>
-      <c r="J26" s="101" t="s">
+      <c r="J26" s="86" t="s">
         <v>177</v>
       </c>
       <c r="K26" s="3"/>
@@ -2365,22 +2389,22 @@
       <c r="X26" s="1"/>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A27" s="80"/>
-      <c r="B27" s="71">
+      <c r="A27" s="81"/>
+      <c r="B27" s="77">
         <v>6</v>
       </c>
       <c r="C27" s="54" t="s">
         <v>108</v>
       </c>
-      <c r="D27" s="102"/>
-      <c r="E27" s="71"/>
-      <c r="F27" s="87"/>
-      <c r="G27" s="87"/>
+      <c r="D27" s="87"/>
+      <c r="E27" s="77"/>
+      <c r="F27" s="73"/>
+      <c r="G27" s="73"/>
       <c r="H27" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="I27" s="87"/>
-      <c r="J27" s="102"/>
+      <c r="I27" s="73"/>
+      <c r="J27" s="87"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
@@ -2397,8 +2421,8 @@
       <c r="X27" s="1"/>
     </row>
     <row r="28" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="80"/>
-      <c r="B28" s="71"/>
+      <c r="A28" s="81"/>
+      <c r="B28" s="77"/>
       <c r="C28" s="54" t="s">
         <v>109</v>
       </c>
@@ -2439,8 +2463,8 @@
       <c r="X28" s="1"/>
     </row>
     <row r="29" spans="1:24" ht="60" x14ac:dyDescent="0.25">
-      <c r="A29" s="80"/>
-      <c r="B29" s="71">
+      <c r="A29" s="81"/>
+      <c r="B29" s="77">
         <v>7</v>
       </c>
       <c r="C29" s="54" t="s">
@@ -2483,8 +2507,8 @@
       <c r="X29" s="1"/>
     </row>
     <row r="30" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="81"/>
-      <c r="B30" s="71"/>
+      <c r="A30" s="82"/>
+      <c r="B30" s="77"/>
       <c r="C30" s="54" t="s">
         <v>111</v>
       </c>
@@ -2524,75 +2548,61 @@
       <c r="W30" s="1"/>
       <c r="X30" s="1"/>
     </row>
-    <row r="31" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="79" t="s">
+    <row r="31" spans="1:24" s="109" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="103"/>
+      <c r="B31" s="104" t="s">
+        <v>208</v>
+      </c>
+      <c r="C31" s="105"/>
+      <c r="D31" s="106"/>
+      <c r="E31" s="104"/>
+      <c r="F31" s="104"/>
+      <c r="G31" s="104"/>
+      <c r="H31" s="104"/>
+      <c r="I31" s="104"/>
+      <c r="J31" s="106"/>
+      <c r="K31" s="107"/>
+      <c r="L31" s="107"/>
+      <c r="M31" s="107"/>
+      <c r="N31" s="107"/>
+      <c r="O31" s="107"/>
+      <c r="P31" s="107"/>
+      <c r="Q31" s="107"/>
+      <c r="R31" s="107"/>
+      <c r="S31" s="107"/>
+      <c r="T31" s="107"/>
+      <c r="U31" s="107"/>
+      <c r="V31" s="107"/>
+      <c r="W31" s="108"/>
+      <c r="X31" s="108"/>
+    </row>
+    <row r="32" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="80" t="s">
         <v>31</v>
       </c>
-      <c r="B31" s="67"/>
-      <c r="C31" s="38" t="s">
+      <c r="B32" s="68"/>
+      <c r="C32" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="D32" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="E31" s="15" t="s">
+      <c r="E32" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="F31" s="15">
+      <c r="F32" s="15">
         <v>0</v>
       </c>
-      <c r="G31" s="15">
+      <c r="G32" s="15">
         <v>1</v>
-      </c>
-      <c r="H31" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I31" s="44">
-        <v>1</v>
-      </c>
-      <c r="J31" s="45"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3"/>
-      <c r="O31" s="3"/>
-      <c r="P31" s="3"/>
-      <c r="Q31" s="3"/>
-      <c r="R31" s="3"/>
-      <c r="S31" s="3"/>
-      <c r="T31" s="3"/>
-      <c r="U31" s="3"/>
-      <c r="V31" s="3"/>
-      <c r="W31" s="1"/>
-      <c r="X31" s="1"/>
-    </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A32" s="80"/>
-      <c r="B32" s="67"/>
-      <c r="C32" s="38" t="s">
-        <v>113</v>
-      </c>
-      <c r="D32" s="74" t="s">
-        <v>32</v>
-      </c>
-      <c r="E32" s="67" t="s">
-        <v>10</v>
-      </c>
-      <c r="F32" s="61">
-        <v>0</v>
-      </c>
-      <c r="G32" s="61">
-        <v>65535</v>
       </c>
       <c r="H32" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I32" s="61">
-        <v>10</v>
+      <c r="I32" s="44">
+        <v>1</v>
       </c>
-      <c r="J32" s="74" t="s">
-        <v>177</v>
-      </c>
+      <c r="J32" s="45"/>
       <c r="K32" s="3"/>
       <c r="L32" s="3"/>
       <c r="M32" s="3"/>
@@ -2609,20 +2619,32 @@
       <c r="X32" s="1"/>
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A33" s="80"/>
-      <c r="B33" s="67"/>
+      <c r="A33" s="81"/>
+      <c r="B33" s="68"/>
       <c r="C33" s="38" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
-      <c r="D33" s="75"/>
-      <c r="E33" s="67"/>
-      <c r="F33" s="63"/>
-      <c r="G33" s="63"/>
+      <c r="D33" s="63" t="s">
+        <v>32</v>
+      </c>
+      <c r="E33" s="68" t="s">
+        <v>10</v>
+      </c>
+      <c r="F33" s="61">
+        <v>0</v>
+      </c>
+      <c r="G33" s="61">
+        <v>65535</v>
+      </c>
       <c r="H33" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I33" s="63"/>
-      <c r="J33" s="75"/>
+      <c r="I33" s="61">
+        <v>10</v>
+      </c>
+      <c r="J33" s="63" t="s">
+        <v>177</v>
+      </c>
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
@@ -2639,22 +2661,20 @@
       <c r="X33" s="1"/>
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A34" s="80"/>
-      <c r="B34" s="67"/>
+      <c r="A34" s="81"/>
+      <c r="B34" s="68"/>
       <c r="C34" s="38" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
-      <c r="D34" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="E34" s="14"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
+      <c r="D34" s="64"/>
+      <c r="E34" s="68"/>
+      <c r="F34" s="62"/>
+      <c r="G34" s="62"/>
       <c r="H34" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I34" s="46"/>
-      <c r="J34" s="45"/>
+      <c r="I34" s="62"/>
+      <c r="J34" s="64"/>
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
@@ -2671,10 +2691,10 @@
       <c r="X34" s="1"/>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A35" s="80"/>
-      <c r="B35" s="67"/>
+      <c r="A35" s="81"/>
+      <c r="B35" s="68"/>
       <c r="C35" s="38" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D35" s="21" t="s">
         <v>8</v>
@@ -2703,10 +2723,10 @@
       <c r="X35" s="1"/>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A36" s="80"/>
-      <c r="B36" s="67"/>
+      <c r="A36" s="81"/>
+      <c r="B36" s="68"/>
       <c r="C36" s="38" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D36" s="21" t="s">
         <v>8</v>
@@ -2735,10 +2755,10 @@
       <c r="X36" s="1"/>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A37" s="80"/>
-      <c r="B37" s="67"/>
+      <c r="A37" s="81"/>
+      <c r="B37" s="68"/>
       <c r="C37" s="38" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D37" s="21" t="s">
         <v>8</v>
@@ -2767,10 +2787,10 @@
       <c r="X37" s="1"/>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A38" s="80"/>
-      <c r="B38" s="67"/>
+      <c r="A38" s="81"/>
+      <c r="B38" s="68"/>
       <c r="C38" s="38" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D38" s="21" t="s">
         <v>8</v>
@@ -2798,32 +2818,22 @@
       <c r="W38" s="1"/>
       <c r="X38" s="1"/>
     </row>
-    <row r="39" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="79" t="s">
-        <v>35</v>
+    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A39" s="81"/>
+      <c r="B39" s="68"/>
+      <c r="C39" s="38" t="s">
+        <v>119</v>
       </c>
-      <c r="B39" s="61"/>
-      <c r="C39" s="38" t="s">
-        <v>120</v>
+      <c r="D39" s="21" t="s">
+        <v>8</v>
       </c>
-      <c r="D39" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="E39" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F39" s="15">
-        <v>0</v>
-      </c>
-      <c r="G39" s="15">
-        <v>1</v>
-      </c>
+      <c r="E39" s="14"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="15"/>
       <c r="H39" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I39" s="44">
-        <v>1</v>
-      </c>
+      <c r="I39" s="46"/>
       <c r="J39" s="45"/>
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
@@ -2841,32 +2851,32 @@
       <c r="X39" s="1"/>
     </row>
     <row r="40" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="82"/>
-      <c r="B40" s="63"/>
+      <c r="A40" s="80" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40" s="61"/>
       <c r="C40" s="38" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
-      <c r="D40" s="65" t="s">
-        <v>36</v>
+      <c r="D40" s="33" t="s">
+        <v>33</v>
       </c>
-      <c r="E40" s="67" t="s">
-        <v>10</v>
+      <c r="E40" s="15" t="s">
+        <v>15</v>
       </c>
-      <c r="F40" s="61">
+      <c r="F40" s="15">
         <v>0</v>
       </c>
-      <c r="G40" s="61">
-        <v>65535</v>
+      <c r="G40" s="15">
+        <v>1</v>
       </c>
       <c r="H40" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I40" s="61">
-        <v>10</v>
+      <c r="I40" s="44">
+        <v>1</v>
       </c>
-      <c r="J40" s="74" t="s">
-        <v>177</v>
-      </c>
+      <c r="J40" s="45"/>
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
       <c r="M40" s="3"/>
@@ -2882,21 +2892,33 @@
       <c r="W40" s="1"/>
       <c r="X40" s="1"/>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A41" s="82"/>
-      <c r="B41" s="61"/>
+    <row r="41" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="83"/>
+      <c r="B41" s="62"/>
       <c r="C41" s="38" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
-      <c r="D41" s="66"/>
-      <c r="E41" s="67"/>
-      <c r="F41" s="63"/>
-      <c r="G41" s="63"/>
+      <c r="D41" s="66" t="s">
+        <v>36</v>
+      </c>
+      <c r="E41" s="68" t="s">
+        <v>10</v>
+      </c>
+      <c r="F41" s="61">
+        <v>0</v>
+      </c>
+      <c r="G41" s="61">
+        <v>65535</v>
+      </c>
       <c r="H41" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I41" s="63"/>
-      <c r="J41" s="75"/>
+      <c r="I41" s="61">
+        <v>10</v>
+      </c>
+      <c r="J41" s="63" t="s">
+        <v>177</v>
+      </c>
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
       <c r="M41" s="3"/>
@@ -2913,22 +2935,20 @@
       <c r="X41" s="1"/>
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A42" s="82"/>
-      <c r="B42" s="63"/>
+      <c r="A42" s="83"/>
+      <c r="B42" s="61"/>
       <c r="C42" s="38" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
-      <c r="D42" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="E42" s="14"/>
-      <c r="F42" s="15"/>
-      <c r="G42" s="15"/>
+      <c r="D42" s="67"/>
+      <c r="E42" s="68"/>
+      <c r="F42" s="62"/>
+      <c r="G42" s="62"/>
       <c r="H42" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I42" s="46"/>
-      <c r="J42" s="45"/>
+      <c r="I42" s="62"/>
+      <c r="J42" s="64"/>
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
@@ -2945,32 +2965,22 @@
       <c r="X42" s="1"/>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A43" s="82"/>
-      <c r="B43" s="61"/>
+      <c r="A43" s="83"/>
+      <c r="B43" s="62"/>
       <c r="C43" s="38" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
-      <c r="D43" s="22" t="s">
-        <v>37</v>
+      <c r="D43" s="21" t="s">
+        <v>8</v>
       </c>
-      <c r="E43" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F43" s="15">
-        <v>0</v>
-      </c>
-      <c r="G43" s="15">
-        <v>3</v>
-      </c>
-      <c r="H43" s="15" t="s">
+      <c r="E43" s="14"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+      <c r="H43" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I43" s="44">
-        <v>2</v>
-      </c>
-      <c r="J43" s="45" t="s">
-        <v>181</v>
-      </c>
+      <c r="I43" s="46"/>
+      <c r="J43" s="45"/>
       <c r="K43" s="3"/>
       <c r="L43" s="3"/>
       <c r="M43" s="3"/>
@@ -2986,14 +2996,14 @@
       <c r="W43" s="1"/>
       <c r="X43" s="1"/>
     </row>
-    <row r="44" spans="1:24" ht="45" x14ac:dyDescent="0.25">
-      <c r="A44" s="82"/>
-      <c r="B44" s="63"/>
+    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A44" s="83"/>
+      <c r="B44" s="61"/>
       <c r="C44" s="38" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D44" s="22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E44" s="15" t="s">
         <v>15</v>
@@ -3002,13 +3012,13 @@
         <v>0</v>
       </c>
       <c r="G44" s="15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H44" s="15" t="s">
         <v>13</v>
       </c>
       <c r="I44" s="44">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J44" s="45" t="s">
         <v>181</v>
@@ -3028,28 +3038,28 @@
       <c r="W44" s="1"/>
       <c r="X44" s="1"/>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A45" s="82"/>
-      <c r="B45" s="61"/>
+    <row r="45" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" s="83"/>
+      <c r="B45" s="62"/>
       <c r="C45" s="38" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
-      <c r="D45" s="74" t="s">
-        <v>39</v>
+      <c r="D45" s="22" t="s">
+        <v>38</v>
       </c>
-      <c r="E45" s="67" t="s">
-        <v>10</v>
+      <c r="E45" s="15" t="s">
+        <v>15</v>
       </c>
-      <c r="F45" s="61" t="s">
-        <v>40</v>
+      <c r="F45" s="15">
+        <v>0</v>
       </c>
-      <c r="G45" s="61" t="s">
-        <v>40</v>
+      <c r="G45" s="15">
+        <v>1</v>
       </c>
-      <c r="H45" s="61" t="s">
+      <c r="H45" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="I45" s="61">
+      <c r="I45" s="44">
         <v>0</v>
       </c>
       <c r="J45" s="45" t="s">
@@ -3070,18 +3080,30 @@
       <c r="W45" s="1"/>
       <c r="X45" s="1"/>
     </row>
-    <row r="46" spans="1:24" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="82"/>
-      <c r="B46" s="63"/>
+    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A46" s="83"/>
+      <c r="B46" s="61"/>
       <c r="C46" s="38" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
-      <c r="D46" s="75"/>
-      <c r="E46" s="67"/>
-      <c r="F46" s="63"/>
-      <c r="G46" s="63"/>
-      <c r="H46" s="63"/>
-      <c r="I46" s="63"/>
+      <c r="D46" s="63" t="s">
+        <v>39</v>
+      </c>
+      <c r="E46" s="68" t="s">
+        <v>10</v>
+      </c>
+      <c r="F46" s="61" t="s">
+        <v>40</v>
+      </c>
+      <c r="G46" s="61" t="s">
+        <v>40</v>
+      </c>
+      <c r="H46" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="I46" s="61">
+        <v>0</v>
+      </c>
       <c r="J46" s="45" t="s">
         <v>181</v>
       </c>
@@ -3100,30 +3122,18 @@
       <c r="W46" s="1"/>
       <c r="X46" s="1"/>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A47" s="82"/>
-      <c r="B47" s="61"/>
+    <row r="47" spans="1:24" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="83"/>
+      <c r="B47" s="62"/>
       <c r="C47" s="38" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
-      <c r="D47" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E47" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F47" s="15">
-        <v>0</v>
-      </c>
-      <c r="G47" s="15">
-        <v>3</v>
-      </c>
-      <c r="H47" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="I47" s="44">
-        <v>0</v>
-      </c>
+      <c r="D47" s="64"/>
+      <c r="E47" s="68"/>
+      <c r="F47" s="62"/>
+      <c r="G47" s="62"/>
+      <c r="H47" s="62"/>
+      <c r="I47" s="62"/>
       <c r="J47" s="45" t="s">
         <v>181</v>
       </c>
@@ -3142,14 +3152,14 @@
       <c r="W47" s="1"/>
       <c r="X47" s="1"/>
     </row>
-    <row r="48" spans="1:24" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="82"/>
-      <c r="B48" s="63"/>
+    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A48" s="83"/>
+      <c r="B48" s="61"/>
       <c r="C48" s="38" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D48" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E48" s="15" t="s">
         <v>15</v>
@@ -3158,7 +3168,7 @@
         <v>0</v>
       </c>
       <c r="G48" s="15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H48" s="15" t="s">
         <v>13</v>
@@ -3184,25 +3194,25 @@
       <c r="W48" s="1"/>
       <c r="X48" s="1"/>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A49" s="82"/>
-      <c r="B49" s="61"/>
+    <row r="49" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+      <c r="A49" s="83"/>
+      <c r="B49" s="62"/>
       <c r="C49" s="38" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
-      <c r="D49" s="74" t="s">
-        <v>45</v>
+      <c r="D49" s="13" t="s">
+        <v>42</v>
       </c>
-      <c r="E49" s="67" t="s">
-        <v>10</v>
+      <c r="E49" s="15" t="s">
+        <v>15</v>
       </c>
-      <c r="F49" s="61" t="s">
-        <v>40</v>
+      <c r="F49" s="15">
+        <v>0</v>
       </c>
-      <c r="G49" s="61" t="s">
-        <v>40</v>
+      <c r="G49" s="15">
+        <v>1</v>
       </c>
-      <c r="H49" s="61" t="s">
+      <c r="H49" s="15" t="s">
         <v>13</v>
       </c>
       <c r="I49" s="44">
@@ -3226,18 +3236,30 @@
       <c r="W49" s="1"/>
       <c r="X49" s="1"/>
     </row>
-    <row r="50" spans="1:24" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="82"/>
-      <c r="B50" s="63"/>
+    <row r="50" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A50" s="83"/>
+      <c r="B50" s="61"/>
       <c r="C50" s="38" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
-      <c r="D50" s="75"/>
-      <c r="E50" s="67"/>
-      <c r="F50" s="63"/>
-      <c r="G50" s="63"/>
-      <c r="H50" s="63"/>
-      <c r="I50" s="44"/>
+      <c r="D50" s="63" t="s">
+        <v>45</v>
+      </c>
+      <c r="E50" s="68" t="s">
+        <v>10</v>
+      </c>
+      <c r="F50" s="61" t="s">
+        <v>40</v>
+      </c>
+      <c r="G50" s="61" t="s">
+        <v>40</v>
+      </c>
+      <c r="H50" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="I50" s="44">
+        <v>0</v>
+      </c>
       <c r="J50" s="45" t="s">
         <v>181</v>
       </c>
@@ -3256,30 +3278,18 @@
       <c r="W50" s="1"/>
       <c r="X50" s="1"/>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A51" s="82"/>
-      <c r="B51" s="61"/>
+    <row r="51" spans="1:24" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="83"/>
+      <c r="B51" s="62"/>
       <c r="C51" s="38" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
-      <c r="D51" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E51" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F51" s="15">
-        <v>0</v>
-      </c>
-      <c r="G51" s="15">
-        <v>3</v>
-      </c>
-      <c r="H51" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="I51" s="44">
-        <v>1</v>
-      </c>
+      <c r="D51" s="64"/>
+      <c r="E51" s="68"/>
+      <c r="F51" s="62"/>
+      <c r="G51" s="62"/>
+      <c r="H51" s="62"/>
+      <c r="I51" s="44"/>
       <c r="J51" s="45" t="s">
         <v>181</v>
       </c>
@@ -3298,14 +3308,14 @@
       <c r="W51" s="1"/>
       <c r="X51" s="1"/>
     </row>
-    <row r="52" spans="1:24" ht="45" x14ac:dyDescent="0.25">
-      <c r="A52" s="82"/>
-      <c r="B52" s="63"/>
+    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A52" s="83"/>
+      <c r="B52" s="61"/>
       <c r="C52" s="38" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D52" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E52" s="15" t="s">
         <v>15</v>
@@ -3314,13 +3324,13 @@
         <v>0</v>
       </c>
       <c r="G52" s="15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H52" s="15" t="s">
         <v>13</v>
       </c>
       <c r="I52" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J52" s="45" t="s">
         <v>181</v>
@@ -3340,28 +3350,28 @@
       <c r="W52" s="1"/>
       <c r="X52" s="1"/>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A53" s="82"/>
-      <c r="B53" s="61"/>
+    <row r="53" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+      <c r="A53" s="83"/>
+      <c r="B53" s="62"/>
       <c r="C53" s="38" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
-      <c r="D53" s="74" t="s">
-        <v>46</v>
+      <c r="D53" s="13" t="s">
+        <v>43</v>
       </c>
-      <c r="E53" s="67" t="s">
-        <v>10</v>
+      <c r="E53" s="15" t="s">
+        <v>15</v>
       </c>
-      <c r="F53" s="61" t="s">
-        <v>40</v>
+      <c r="F53" s="15">
+        <v>0</v>
       </c>
-      <c r="G53" s="61" t="s">
-        <v>40</v>
+      <c r="G53" s="15">
+        <v>1</v>
       </c>
-      <c r="H53" s="61" t="s">
+      <c r="H53" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="I53" s="61">
+      <c r="I53" s="44">
         <v>0</v>
       </c>
       <c r="J53" s="45" t="s">
@@ -3382,18 +3392,30 @@
       <c r="W53" s="1"/>
       <c r="X53" s="1"/>
     </row>
-    <row r="54" spans="1:24" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="82"/>
-      <c r="B54" s="63"/>
+    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A54" s="83"/>
+      <c r="B54" s="61"/>
       <c r="C54" s="38" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
-      <c r="D54" s="75"/>
-      <c r="E54" s="67"/>
-      <c r="F54" s="63"/>
-      <c r="G54" s="63"/>
-      <c r="H54" s="63"/>
-      <c r="I54" s="63"/>
+      <c r="D54" s="63" t="s">
+        <v>46</v>
+      </c>
+      <c r="E54" s="68" t="s">
+        <v>10</v>
+      </c>
+      <c r="F54" s="61" t="s">
+        <v>40</v>
+      </c>
+      <c r="G54" s="61" t="s">
+        <v>40</v>
+      </c>
+      <c r="H54" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="I54" s="61">
+        <v>0</v>
+      </c>
       <c r="J54" s="45" t="s">
         <v>181</v>
       </c>
@@ -3412,30 +3434,18 @@
       <c r="W54" s="1"/>
       <c r="X54" s="1"/>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A55" s="82"/>
-      <c r="B55" s="61"/>
+    <row r="55" spans="1:24" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="83"/>
+      <c r="B55" s="62"/>
       <c r="C55" s="38" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
-      <c r="D55" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E55" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F55" s="15">
-        <v>0</v>
-      </c>
-      <c r="G55" s="15">
-        <v>3</v>
-      </c>
-      <c r="H55" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="I55" s="44">
-        <v>1</v>
-      </c>
+      <c r="D55" s="64"/>
+      <c r="E55" s="68"/>
+      <c r="F55" s="62"/>
+      <c r="G55" s="62"/>
+      <c r="H55" s="62"/>
+      <c r="I55" s="62"/>
       <c r="J55" s="45" t="s">
         <v>181</v>
       </c>
@@ -3454,14 +3464,14 @@
       <c r="W55" s="1"/>
       <c r="X55" s="1"/>
     </row>
-    <row r="56" spans="1:24" ht="45" x14ac:dyDescent="0.25">
-      <c r="A56" s="82"/>
-      <c r="B56" s="63"/>
+    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A56" s="83"/>
+      <c r="B56" s="61"/>
       <c r="C56" s="38" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D56" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E56" s="15" t="s">
         <v>15</v>
@@ -3470,13 +3480,13 @@
         <v>0</v>
       </c>
       <c r="G56" s="15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H56" s="15" t="s">
         <v>13</v>
       </c>
       <c r="I56" s="44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J56" s="45" t="s">
         <v>181</v>
@@ -3496,28 +3506,28 @@
       <c r="W56" s="1"/>
       <c r="X56" s="1"/>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A57" s="82"/>
-      <c r="B57" s="61"/>
+    <row r="57" spans="1:24" ht="45" x14ac:dyDescent="0.25">
+      <c r="A57" s="83"/>
+      <c r="B57" s="62"/>
       <c r="C57" s="38" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
-      <c r="D57" s="74" t="s">
-        <v>49</v>
+      <c r="D57" s="13" t="s">
+        <v>48</v>
       </c>
-      <c r="E57" s="67" t="s">
-        <v>10</v>
+      <c r="E57" s="15" t="s">
+        <v>15</v>
       </c>
-      <c r="F57" s="61" t="s">
-        <v>40</v>
+      <c r="F57" s="15">
+        <v>0</v>
       </c>
-      <c r="G57" s="61" t="s">
-        <v>40</v>
+      <c r="G57" s="15">
+        <v>1</v>
       </c>
-      <c r="H57" s="61" t="s">
+      <c r="H57" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="I57" s="61">
+      <c r="I57" s="44">
         <v>0</v>
       </c>
       <c r="J57" s="45" t="s">
@@ -3538,18 +3548,30 @@
       <c r="W57" s="1"/>
       <c r="X57" s="1"/>
     </row>
-    <row r="58" spans="1:24" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A58" s="83"/>
-      <c r="B58" s="63"/>
+      <c r="B58" s="61"/>
       <c r="C58" s="38" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
-      <c r="D58" s="75"/>
-      <c r="E58" s="67"/>
-      <c r="F58" s="63"/>
-      <c r="G58" s="63"/>
-      <c r="H58" s="63"/>
-      <c r="I58" s="63"/>
+      <c r="D58" s="63" t="s">
+        <v>49</v>
+      </c>
+      <c r="E58" s="68" t="s">
+        <v>10</v>
+      </c>
+      <c r="F58" s="61" t="s">
+        <v>40</v>
+      </c>
+      <c r="G58" s="61" t="s">
+        <v>40</v>
+      </c>
+      <c r="H58" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="I58" s="61">
+        <v>0</v>
+      </c>
       <c r="J58" s="45" t="s">
         <v>181</v>
       </c>
@@ -3568,33 +3590,21 @@
       <c r="W58" s="1"/>
       <c r="X58" s="1"/>
     </row>
-    <row r="59" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="58" t="s">
-        <v>50</v>
+    <row r="59" spans="1:24" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="84"/>
+      <c r="B59" s="62"/>
+      <c r="C59" s="38" t="s">
+        <v>139</v>
       </c>
-      <c r="B59" s="61"/>
-      <c r="C59" s="38" t="s">
-        <v>140</v>
+      <c r="D59" s="64"/>
+      <c r="E59" s="68"/>
+      <c r="F59" s="62"/>
+      <c r="G59" s="62"/>
+      <c r="H59" s="62"/>
+      <c r="I59" s="62"/>
+      <c r="J59" s="45" t="s">
+        <v>181</v>
       </c>
-      <c r="D59" s="65" t="s">
-        <v>33</v>
-      </c>
-      <c r="E59" s="61" t="s">
-        <v>15</v>
-      </c>
-      <c r="F59" s="61">
-        <v>0</v>
-      </c>
-      <c r="G59" s="61">
-        <v>1</v>
-      </c>
-      <c r="H59" s="61" t="s">
-        <v>13</v>
-      </c>
-      <c r="I59" s="61">
-        <v>0</v>
-      </c>
-      <c r="J59" s="45"/>
       <c r="K59" s="3"/>
       <c r="L59" s="3"/>
       <c r="M59" s="3"/>
@@ -3610,21 +3620,33 @@
       <c r="W59" s="1"/>
       <c r="X59" s="1"/>
     </row>
-    <row r="60" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="59"/>
-      <c r="B60" s="63"/>
-      <c r="C60" s="51" t="s">
-        <v>141</v>
+    <row r="60" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="94" t="s">
+        <v>50</v>
       </c>
-      <c r="D60" s="66"/>
-      <c r="E60" s="63"/>
-      <c r="F60" s="63"/>
-      <c r="G60" s="63"/>
-      <c r="H60" s="63"/>
-      <c r="I60" s="63"/>
-      <c r="J60" s="50" t="s">
-        <v>94</v>
+      <c r="B60" s="61"/>
+      <c r="C60" s="38" t="s">
+        <v>140</v>
       </c>
+      <c r="D60" s="66" t="s">
+        <v>33</v>
+      </c>
+      <c r="E60" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="F60" s="61">
+        <v>0</v>
+      </c>
+      <c r="G60" s="61">
+        <v>1</v>
+      </c>
+      <c r="H60" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="I60" s="61">
+        <v>0</v>
+      </c>
+      <c r="J60" s="45"/>
       <c r="K60" s="3"/>
       <c r="L60" s="3"/>
       <c r="M60" s="3"/>
@@ -3640,32 +3662,20 @@
       <c r="W60" s="1"/>
       <c r="X60" s="1"/>
     </row>
-    <row r="61" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="59"/>
-      <c r="B61" s="61"/>
-      <c r="C61" s="38" t="s">
-        <v>142</v>
+    <row r="61" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="95"/>
+      <c r="B61" s="62"/>
+      <c r="C61" s="51" t="s">
+        <v>141</v>
       </c>
-      <c r="D61" s="65" t="s">
-        <v>51</v>
-      </c>
-      <c r="E61" s="67" t="s">
-        <v>10</v>
-      </c>
-      <c r="F61" s="61">
-        <v>0</v>
-      </c>
-      <c r="G61" s="68" t="s">
-        <v>95</v>
-      </c>
-      <c r="H61" s="61" t="s">
-        <v>13</v>
-      </c>
-      <c r="I61" s="61">
-        <v>0</v>
-      </c>
-      <c r="J61" s="74" t="s">
-        <v>182</v>
+      <c r="D61" s="67"/>
+      <c r="E61" s="62"/>
+      <c r="F61" s="62"/>
+      <c r="G61" s="62"/>
+      <c r="H61" s="62"/>
+      <c r="I61" s="62"/>
+      <c r="J61" s="50" t="s">
+        <v>94</v>
       </c>
       <c r="K61" s="3"/>
       <c r="L61" s="3"/>
@@ -3682,19 +3692,33 @@
       <c r="W61" s="1"/>
       <c r="X61" s="1"/>
     </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A62" s="59"/>
-      <c r="B62" s="63"/>
+    <row r="62" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="95"/>
+      <c r="B62" s="61"/>
       <c r="C62" s="38" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
-      <c r="D62" s="66"/>
-      <c r="E62" s="67"/>
-      <c r="F62" s="63"/>
-      <c r="G62" s="69"/>
-      <c r="H62" s="63"/>
-      <c r="I62" s="63"/>
-      <c r="J62" s="75"/>
+      <c r="D62" s="66" t="s">
+        <v>51</v>
+      </c>
+      <c r="E62" s="68" t="s">
+        <v>10</v>
+      </c>
+      <c r="F62" s="61">
+        <v>0</v>
+      </c>
+      <c r="G62" s="92" t="s">
+        <v>95</v>
+      </c>
+      <c r="H62" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="I62" s="61">
+        <v>0</v>
+      </c>
+      <c r="J62" s="63" t="s">
+        <v>182</v>
+      </c>
       <c r="K62" s="3"/>
       <c r="L62" s="3"/>
       <c r="M62" s="3"/>
@@ -3710,33 +3734,19 @@
       <c r="W62" s="1"/>
       <c r="X62" s="1"/>
     </row>
-    <row r="63" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="59"/>
-      <c r="B63" s="61"/>
+    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A63" s="95"/>
+      <c r="B63" s="62"/>
       <c r="C63" s="38" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
-      <c r="D63" s="65" t="s">
-        <v>52</v>
-      </c>
-      <c r="E63" s="67" t="s">
-        <v>10</v>
-      </c>
-      <c r="F63" s="61">
-        <v>0</v>
-      </c>
-      <c r="G63" s="61" t="s">
-        <v>186</v>
-      </c>
-      <c r="H63" s="61" t="s">
-        <v>13</v>
-      </c>
-      <c r="I63" s="61" t="s">
-        <v>8</v>
-      </c>
-      <c r="J63" s="74" t="s">
-        <v>182</v>
-      </c>
+      <c r="D63" s="67"/>
+      <c r="E63" s="68"/>
+      <c r="F63" s="62"/>
+      <c r="G63" s="93"/>
+      <c r="H63" s="62"/>
+      <c r="I63" s="62"/>
+      <c r="J63" s="64"/>
       <c r="K63" s="3"/>
       <c r="L63" s="3"/>
       <c r="M63" s="3"/>
@@ -3753,18 +3763,32 @@
       <c r="X63" s="1"/>
     </row>
     <row r="64" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="59"/>
-      <c r="B64" s="63"/>
+      <c r="A64" s="95"/>
+      <c r="B64" s="61"/>
       <c r="C64" s="38" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
-      <c r="D64" s="66"/>
-      <c r="E64" s="67"/>
-      <c r="F64" s="63"/>
-      <c r="G64" s="63"/>
-      <c r="H64" s="63"/>
-      <c r="I64" s="63"/>
-      <c r="J64" s="75"/>
+      <c r="D64" s="66" t="s">
+        <v>52</v>
+      </c>
+      <c r="E64" s="68" t="s">
+        <v>10</v>
+      </c>
+      <c r="F64" s="61">
+        <v>0</v>
+      </c>
+      <c r="G64" s="61" t="s">
+        <v>186</v>
+      </c>
+      <c r="H64" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="I64" s="61" t="s">
+        <v>8</v>
+      </c>
+      <c r="J64" s="63" t="s">
+        <v>182</v>
+      </c>
       <c r="K64" s="3"/>
       <c r="L64" s="3"/>
       <c r="M64" s="3"/>
@@ -3781,32 +3805,18 @@
       <c r="X64" s="1"/>
     </row>
     <row r="65" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="59"/>
-      <c r="B65" s="61"/>
+      <c r="A65" s="95"/>
+      <c r="B65" s="62"/>
       <c r="C65" s="38" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
-      <c r="D65" s="65" t="s">
-        <v>53</v>
-      </c>
-      <c r="E65" s="67" t="s">
-        <v>10</v>
-      </c>
-      <c r="F65" s="61">
-        <v>0</v>
-      </c>
-      <c r="G65" s="68" t="s">
-        <v>95</v>
-      </c>
-      <c r="H65" s="61" t="s">
-        <v>13</v>
-      </c>
-      <c r="I65" s="61" t="s">
-        <v>8</v>
-      </c>
-      <c r="J65" s="74" t="s">
-        <v>182</v>
-      </c>
+      <c r="D65" s="67"/>
+      <c r="E65" s="68"/>
+      <c r="F65" s="62"/>
+      <c r="G65" s="62"/>
+      <c r="H65" s="62"/>
+      <c r="I65" s="62"/>
+      <c r="J65" s="64"/>
       <c r="K65" s="3"/>
       <c r="L65" s="3"/>
       <c r="M65" s="3"/>
@@ -3822,19 +3832,33 @@
       <c r="W65" s="1"/>
       <c r="X65" s="1"/>
     </row>
-    <row r="66" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A66" s="59"/>
-      <c r="B66" s="63"/>
+    <row r="66" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="95"/>
+      <c r="B66" s="61"/>
       <c r="C66" s="38" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
-      <c r="D66" s="66"/>
-      <c r="E66" s="67"/>
-      <c r="F66" s="63"/>
-      <c r="G66" s="69"/>
-      <c r="H66" s="63"/>
-      <c r="I66" s="63"/>
-      <c r="J66" s="75"/>
+      <c r="D66" s="66" t="s">
+        <v>53</v>
+      </c>
+      <c r="E66" s="68" t="s">
+        <v>10</v>
+      </c>
+      <c r="F66" s="61">
+        <v>0</v>
+      </c>
+      <c r="G66" s="92" t="s">
+        <v>95</v>
+      </c>
+      <c r="H66" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="I66" s="61" t="s">
+        <v>8</v>
+      </c>
+      <c r="J66" s="63" t="s">
+        <v>182</v>
+      </c>
       <c r="K66" s="3"/>
       <c r="L66" s="3"/>
       <c r="M66" s="3"/>
@@ -3850,33 +3874,19 @@
       <c r="W66" s="1"/>
       <c r="X66" s="1"/>
     </row>
-    <row r="67" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="59"/>
-      <c r="B67" s="61"/>
+    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A67" s="95"/>
+      <c r="B67" s="62"/>
       <c r="C67" s="38" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
-      <c r="D67" s="65" t="s">
-        <v>54</v>
-      </c>
-      <c r="E67" s="67" t="s">
-        <v>10</v>
-      </c>
-      <c r="F67" s="61">
-        <v>0</v>
-      </c>
-      <c r="G67" s="61" t="s">
-        <v>186</v>
-      </c>
-      <c r="H67" s="61" t="s">
-        <v>13</v>
-      </c>
-      <c r="I67" s="61" t="s">
-        <v>8</v>
-      </c>
-      <c r="J67" s="74" t="s">
-        <v>182</v>
-      </c>
+      <c r="D67" s="67"/>
+      <c r="E67" s="68"/>
+      <c r="F67" s="62"/>
+      <c r="G67" s="93"/>
+      <c r="H67" s="62"/>
+      <c r="I67" s="62"/>
+      <c r="J67" s="64"/>
       <c r="K67" s="3"/>
       <c r="L67" s="3"/>
       <c r="M67" s="3"/>
@@ -3893,18 +3903,32 @@
       <c r="X67" s="1"/>
     </row>
     <row r="68" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="59"/>
-      <c r="B68" s="63"/>
+      <c r="A68" s="95"/>
+      <c r="B68" s="61"/>
       <c r="C68" s="38" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
-      <c r="D68" s="66"/>
-      <c r="E68" s="67"/>
-      <c r="F68" s="63"/>
-      <c r="G68" s="63"/>
-      <c r="H68" s="63"/>
-      <c r="I68" s="63"/>
-      <c r="J68" s="75"/>
+      <c r="D68" s="66" t="s">
+        <v>54</v>
+      </c>
+      <c r="E68" s="68" t="s">
+        <v>10</v>
+      </c>
+      <c r="F68" s="61">
+        <v>0</v>
+      </c>
+      <c r="G68" s="61" t="s">
+        <v>186</v>
+      </c>
+      <c r="H68" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="I68" s="61" t="s">
+        <v>8</v>
+      </c>
+      <c r="J68" s="63" t="s">
+        <v>182</v>
+      </c>
       <c r="K68" s="3"/>
       <c r="L68" s="3"/>
       <c r="M68" s="3"/>
@@ -3921,32 +3945,18 @@
       <c r="X68" s="1"/>
     </row>
     <row r="69" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="59"/>
-      <c r="B69" s="61"/>
+      <c r="A69" s="95"/>
+      <c r="B69" s="62"/>
       <c r="C69" s="38" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
-      <c r="D69" s="65" t="s">
-        <v>55</v>
-      </c>
-      <c r="E69" s="67" t="s">
-        <v>10</v>
-      </c>
-      <c r="F69" s="61">
-        <v>0</v>
-      </c>
-      <c r="G69" s="68" t="s">
-        <v>95</v>
-      </c>
-      <c r="H69" s="61" t="s">
-        <v>13</v>
-      </c>
-      <c r="I69" s="61" t="s">
-        <v>8</v>
-      </c>
-      <c r="J69" s="74" t="s">
-        <v>182</v>
-      </c>
+      <c r="D69" s="67"/>
+      <c r="E69" s="68"/>
+      <c r="F69" s="62"/>
+      <c r="G69" s="62"/>
+      <c r="H69" s="62"/>
+      <c r="I69" s="62"/>
+      <c r="J69" s="64"/>
       <c r="K69" s="3"/>
       <c r="L69" s="3"/>
       <c r="M69" s="3"/>
@@ -3962,19 +3972,33 @@
       <c r="W69" s="1"/>
       <c r="X69" s="1"/>
     </row>
-    <row r="70" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A70" s="59"/>
-      <c r="B70" s="63"/>
+    <row r="70" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="95"/>
+      <c r="B70" s="61"/>
       <c r="C70" s="38" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
-      <c r="D70" s="66"/>
-      <c r="E70" s="67"/>
-      <c r="F70" s="63"/>
-      <c r="G70" s="69"/>
-      <c r="H70" s="63"/>
-      <c r="I70" s="63"/>
-      <c r="J70" s="75"/>
+      <c r="D70" s="66" t="s">
+        <v>55</v>
+      </c>
+      <c r="E70" s="68" t="s">
+        <v>10</v>
+      </c>
+      <c r="F70" s="61">
+        <v>0</v>
+      </c>
+      <c r="G70" s="92" t="s">
+        <v>95</v>
+      </c>
+      <c r="H70" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="I70" s="61" t="s">
+        <v>8</v>
+      </c>
+      <c r="J70" s="63" t="s">
+        <v>182</v>
+      </c>
       <c r="K70" s="3"/>
       <c r="L70" s="3"/>
       <c r="M70" s="3"/>
@@ -3990,33 +4014,19 @@
       <c r="W70" s="1"/>
       <c r="X70" s="1"/>
     </row>
-    <row r="71" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="59"/>
-      <c r="B71" s="61"/>
+    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A71" s="95"/>
+      <c r="B71" s="62"/>
       <c r="C71" s="38" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
-      <c r="D71" s="65" t="s">
-        <v>56</v>
-      </c>
-      <c r="E71" s="67" t="s">
-        <v>10</v>
-      </c>
-      <c r="F71" s="61">
-        <v>0</v>
-      </c>
-      <c r="G71" s="61" t="s">
-        <v>186</v>
-      </c>
-      <c r="H71" s="61" t="s">
-        <v>13</v>
-      </c>
-      <c r="I71" s="61" t="s">
-        <v>8</v>
-      </c>
-      <c r="J71" s="74" t="s">
-        <v>182</v>
-      </c>
+      <c r="D71" s="67"/>
+      <c r="E71" s="68"/>
+      <c r="F71" s="62"/>
+      <c r="G71" s="93"/>
+      <c r="H71" s="62"/>
+      <c r="I71" s="62"/>
+      <c r="J71" s="64"/>
       <c r="K71" s="3"/>
       <c r="L71" s="3"/>
       <c r="M71" s="3"/>
@@ -4033,18 +4043,32 @@
       <c r="X71" s="1"/>
     </row>
     <row r="72" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="59"/>
-      <c r="B72" s="63"/>
+      <c r="A72" s="95"/>
+      <c r="B72" s="61"/>
       <c r="C72" s="38" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
-      <c r="D72" s="66"/>
-      <c r="E72" s="67"/>
-      <c r="F72" s="63"/>
-      <c r="G72" s="63"/>
-      <c r="H72" s="63"/>
-      <c r="I72" s="63"/>
-      <c r="J72" s="75"/>
+      <c r="D72" s="66" t="s">
+        <v>56</v>
+      </c>
+      <c r="E72" s="68" t="s">
+        <v>10</v>
+      </c>
+      <c r="F72" s="61">
+        <v>0</v>
+      </c>
+      <c r="G72" s="61" t="s">
+        <v>186</v>
+      </c>
+      <c r="H72" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="I72" s="61" t="s">
+        <v>8</v>
+      </c>
+      <c r="J72" s="63" t="s">
+        <v>182</v>
+      </c>
       <c r="K72" s="3"/>
       <c r="L72" s="3"/>
       <c r="M72" s="3"/>
@@ -4061,32 +4085,18 @@
       <c r="X72" s="1"/>
     </row>
     <row r="73" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="59"/>
-      <c r="B73" s="61"/>
+      <c r="A73" s="95"/>
+      <c r="B73" s="62"/>
       <c r="C73" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
-      <c r="D73" s="65" t="s">
-        <v>57</v>
-      </c>
-      <c r="E73" s="67" t="s">
-        <v>10</v>
-      </c>
-      <c r="F73" s="61">
-        <v>0</v>
-      </c>
-      <c r="G73" s="68" t="s">
-        <v>95</v>
-      </c>
-      <c r="H73" s="61" t="s">
-        <v>13</v>
-      </c>
-      <c r="I73" s="61" t="s">
-        <v>8</v>
-      </c>
-      <c r="J73" s="74" t="s">
-        <v>182</v>
-      </c>
+      <c r="D73" s="67"/>
+      <c r="E73" s="68"/>
+      <c r="F73" s="62"/>
+      <c r="G73" s="62"/>
+      <c r="H73" s="62"/>
+      <c r="I73" s="62"/>
+      <c r="J73" s="64"/>
       <c r="K73" s="3"/>
       <c r="L73" s="3"/>
       <c r="M73" s="3"/>
@@ -4102,19 +4112,33 @@
       <c r="W73" s="1"/>
       <c r="X73" s="1"/>
     </row>
-    <row r="74" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A74" s="59"/>
-      <c r="B74" s="63"/>
+    <row r="74" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="95"/>
+      <c r="B74" s="61"/>
       <c r="C74" s="38" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
-      <c r="D74" s="66"/>
-      <c r="E74" s="67"/>
-      <c r="F74" s="63"/>
-      <c r="G74" s="69"/>
-      <c r="H74" s="63"/>
-      <c r="I74" s="63"/>
-      <c r="J74" s="75"/>
+      <c r="D74" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="E74" s="68" t="s">
+        <v>10</v>
+      </c>
+      <c r="F74" s="61">
+        <v>0</v>
+      </c>
+      <c r="G74" s="92" t="s">
+        <v>95</v>
+      </c>
+      <c r="H74" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="I74" s="61" t="s">
+        <v>8</v>
+      </c>
+      <c r="J74" s="63" t="s">
+        <v>182</v>
+      </c>
       <c r="K74" s="3"/>
       <c r="L74" s="3"/>
       <c r="M74" s="3"/>
@@ -4130,33 +4154,19 @@
       <c r="W74" s="1"/>
       <c r="X74" s="1"/>
     </row>
-    <row r="75" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="59"/>
-      <c r="B75" s="61"/>
+    <row r="75" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A75" s="95"/>
+      <c r="B75" s="62"/>
       <c r="C75" s="38" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
-      <c r="D75" s="65" t="s">
-        <v>96</v>
-      </c>
-      <c r="E75" s="67" t="s">
-        <v>10</v>
-      </c>
-      <c r="F75" s="61">
-        <v>0</v>
-      </c>
-      <c r="G75" s="61" t="s">
-        <v>186</v>
-      </c>
-      <c r="H75" s="61" t="s">
-        <v>13</v>
-      </c>
-      <c r="I75" s="61" t="s">
-        <v>8</v>
-      </c>
-      <c r="J75" s="74" t="s">
-        <v>182</v>
-      </c>
+      <c r="D75" s="67"/>
+      <c r="E75" s="68"/>
+      <c r="F75" s="62"/>
+      <c r="G75" s="93"/>
+      <c r="H75" s="62"/>
+      <c r="I75" s="62"/>
+      <c r="J75" s="64"/>
       <c r="K75" s="3"/>
       <c r="L75" s="3"/>
       <c r="M75" s="3"/>
@@ -4172,19 +4182,33 @@
       <c r="W75" s="1"/>
       <c r="X75" s="1"/>
     </row>
-    <row r="76" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="59"/>
-      <c r="B76" s="63"/>
+    <row r="76" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="95"/>
+      <c r="B76" s="61"/>
       <c r="C76" s="38" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
-      <c r="D76" s="66"/>
-      <c r="E76" s="67"/>
-      <c r="F76" s="63"/>
-      <c r="G76" s="63"/>
-      <c r="H76" s="63"/>
-      <c r="I76" s="63"/>
-      <c r="J76" s="75"/>
+      <c r="D76" s="66" t="s">
+        <v>96</v>
+      </c>
+      <c r="E76" s="68" t="s">
+        <v>10</v>
+      </c>
+      <c r="F76" s="61">
+        <v>0</v>
+      </c>
+      <c r="G76" s="61" t="s">
+        <v>186</v>
+      </c>
+      <c r="H76" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="I76" s="61" t="s">
+        <v>8</v>
+      </c>
+      <c r="J76" s="63" t="s">
+        <v>182</v>
+      </c>
       <c r="K76" s="3"/>
       <c r="L76" s="3"/>
       <c r="M76" s="3"/>
@@ -4201,32 +4225,18 @@
       <c r="X76" s="1"/>
     </row>
     <row r="77" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="59"/>
-      <c r="B77" s="61"/>
+      <c r="A77" s="95"/>
+      <c r="B77" s="62"/>
       <c r="C77" s="38" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
-      <c r="D77" s="65" t="s">
-        <v>97</v>
-      </c>
-      <c r="E77" s="67" t="s">
-        <v>10</v>
-      </c>
-      <c r="F77" s="61">
-        <v>0</v>
-      </c>
-      <c r="G77" s="68" t="s">
-        <v>95</v>
-      </c>
-      <c r="H77" s="61" t="s">
-        <v>13</v>
-      </c>
-      <c r="I77" s="61" t="s">
-        <v>8</v>
-      </c>
-      <c r="J77" s="74" t="s">
-        <v>182</v>
-      </c>
+      <c r="D77" s="67"/>
+      <c r="E77" s="68"/>
+      <c r="F77" s="62"/>
+      <c r="G77" s="62"/>
+      <c r="H77" s="62"/>
+      <c r="I77" s="62"/>
+      <c r="J77" s="64"/>
       <c r="K77" s="3"/>
       <c r="L77" s="3"/>
       <c r="M77" s="3"/>
@@ -4242,19 +4252,33 @@
       <c r="W77" s="1"/>
       <c r="X77" s="1"/>
     </row>
-    <row r="78" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="60"/>
-      <c r="B78" s="62"/>
+    <row r="78" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="95"/>
+      <c r="B78" s="61"/>
       <c r="C78" s="38" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
-      <c r="D78" s="66"/>
-      <c r="E78" s="67"/>
-      <c r="F78" s="63"/>
-      <c r="G78" s="69"/>
-      <c r="H78" s="63"/>
-      <c r="I78" s="63"/>
-      <c r="J78" s="75"/>
+      <c r="D78" s="66" t="s">
+        <v>97</v>
+      </c>
+      <c r="E78" s="68" t="s">
+        <v>10</v>
+      </c>
+      <c r="F78" s="61">
+        <v>0</v>
+      </c>
+      <c r="G78" s="92" t="s">
+        <v>95</v>
+      </c>
+      <c r="H78" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="I78" s="61" t="s">
+        <v>8</v>
+      </c>
+      <c r="J78" s="63" t="s">
+        <v>182</v>
+      </c>
       <c r="K78" s="3"/>
       <c r="L78" s="3"/>
       <c r="M78" s="3"/>
@@ -4271,34 +4295,18 @@
       <c r="X78" s="1"/>
     </row>
     <row r="79" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="79" t="s">
-        <v>81</v>
+      <c r="A79" s="96"/>
+      <c r="B79" s="97"/>
+      <c r="C79" s="38" t="s">
+        <v>159</v>
       </c>
-      <c r="B79" s="61"/>
-      <c r="C79" s="43" t="s">
-        <v>160</v>
-      </c>
-      <c r="D79" s="65" t="s">
-        <v>59</v>
-      </c>
-      <c r="E79" s="67" t="s">
-        <v>10</v>
-      </c>
-      <c r="F79" s="61">
-        <v>0</v>
-      </c>
-      <c r="G79" s="61">
-        <v>255</v>
-      </c>
-      <c r="H79" s="61" t="s">
-        <v>13</v>
-      </c>
-      <c r="I79" s="61">
-        <v>0</v>
-      </c>
-      <c r="J79" s="52" t="s">
-        <v>183</v>
-      </c>
+      <c r="D79" s="67"/>
+      <c r="E79" s="68"/>
+      <c r="F79" s="62"/>
+      <c r="G79" s="93"/>
+      <c r="H79" s="62"/>
+      <c r="I79" s="62"/>
+      <c r="J79" s="64"/>
       <c r="K79" s="3"/>
       <c r="L79" s="3"/>
       <c r="M79" s="3"/>
@@ -4314,20 +4322,34 @@
       <c r="W79" s="1"/>
       <c r="X79" s="1"/>
     </row>
-    <row r="80" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A80" s="80"/>
-      <c r="B80" s="63"/>
-      <c r="C80" s="51" t="s">
-        <v>161</v>
+    <row r="80" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="80" t="s">
+        <v>81</v>
       </c>
-      <c r="D80" s="66"/>
-      <c r="E80" s="67"/>
-      <c r="F80" s="63"/>
-      <c r="G80" s="63"/>
-      <c r="H80" s="63"/>
-      <c r="I80" s="63"/>
-      <c r="J80" s="53" t="s">
-        <v>94</v>
+      <c r="B80" s="61"/>
+      <c r="C80" s="43" t="s">
+        <v>160</v>
+      </c>
+      <c r="D80" s="66" t="s">
+        <v>59</v>
+      </c>
+      <c r="E80" s="68" t="s">
+        <v>10</v>
+      </c>
+      <c r="F80" s="61">
+        <v>0</v>
+      </c>
+      <c r="G80" s="61">
+        <v>255</v>
+      </c>
+      <c r="H80" s="61" t="s">
+        <v>13</v>
+      </c>
+      <c r="I80" s="61">
+        <v>0</v>
+      </c>
+      <c r="J80" s="52" t="s">
+        <v>183</v>
       </c>
       <c r="K80" s="3"/>
       <c r="L80" s="3"/>
@@ -4344,30 +4366,20 @@
       <c r="W80" s="1"/>
       <c r="X80" s="1"/>
     </row>
-    <row r="81" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="80"/>
-      <c r="B81" s="61"/>
-      <c r="C81" s="38" t="s">
-        <v>162</v>
+    <row r="81" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A81" s="81"/>
+      <c r="B81" s="62"/>
+      <c r="C81" s="51" t="s">
+        <v>161</v>
       </c>
-      <c r="D81" s="45" t="s">
-        <v>60</v>
-      </c>
-      <c r="E81" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="F81" s="19">
-        <v>1</v>
-      </c>
-      <c r="G81" s="19">
-        <v>15</v>
-      </c>
-      <c r="H81" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="I81" s="44"/>
-      <c r="J81" s="45" t="s">
-        <v>179</v>
+      <c r="D81" s="67"/>
+      <c r="E81" s="68"/>
+      <c r="F81" s="62"/>
+      <c r="G81" s="62"/>
+      <c r="H81" s="62"/>
+      <c r="I81" s="62"/>
+      <c r="J81" s="53" t="s">
+        <v>94</v>
       </c>
       <c r="K81" s="3"/>
       <c r="L81" s="3"/>
@@ -4384,14 +4396,14 @@
       <c r="W81" s="1"/>
       <c r="X81" s="1"/>
     </row>
-    <row r="82" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A82" s="80"/>
-      <c r="B82" s="63"/>
+    <row r="82" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="81"/>
+      <c r="B82" s="61"/>
       <c r="C82" s="38" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
-      <c r="D82" s="35" t="s">
-        <v>61</v>
+      <c r="D82" s="45" t="s">
+        <v>60</v>
       </c>
       <c r="E82" s="19" t="s">
         <v>15</v>
@@ -4400,13 +4412,15 @@
         <v>1</v>
       </c>
       <c r="G82" s="19">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="H82" s="19" t="s">
         <v>13</v>
       </c>
       <c r="I82" s="44"/>
-      <c r="J82" s="45"/>
+      <c r="J82" s="45" t="s">
+        <v>179</v>
+      </c>
       <c r="K82" s="3"/>
       <c r="L82" s="3"/>
       <c r="M82" s="3"/>
@@ -4423,32 +4437,28 @@
       <c r="X82" s="1"/>
     </row>
     <row r="83" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A83" s="80"/>
-      <c r="B83" s="61"/>
+      <c r="A83" s="81"/>
+      <c r="B83" s="62"/>
       <c r="C83" s="38" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
-      <c r="D83" s="78" t="s">
-        <v>62</v>
+      <c r="D83" s="35" t="s">
+        <v>61</v>
       </c>
-      <c r="E83" s="67" t="s">
-        <v>10</v>
+      <c r="E83" s="19" t="s">
+        <v>15</v>
       </c>
-      <c r="F83" s="67">
-        <v>0</v>
+      <c r="F83" s="19">
+        <v>1</v>
       </c>
-      <c r="G83" s="67">
-        <v>65535</v>
+      <c r="G83" s="19">
+        <v>4</v>
       </c>
-      <c r="H83" s="67" t="s">
+      <c r="H83" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="I83" s="61">
-        <v>1</v>
-      </c>
-      <c r="J83" s="74" t="s">
-        <v>180</v>
-      </c>
+      <c r="I83" s="44"/>
+      <c r="J83" s="45"/>
       <c r="K83" s="3"/>
       <c r="L83" s="3"/>
       <c r="M83" s="3"/>
@@ -4464,19 +4474,33 @@
       <c r="W83" s="1"/>
       <c r="X83" s="1"/>
     </row>
-    <row r="84" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="80"/>
-      <c r="B84" s="63"/>
+    <row r="84" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A84" s="81"/>
+      <c r="B84" s="61"/>
       <c r="C84" s="38" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
-      <c r="D84" s="78"/>
-      <c r="E84" s="67"/>
-      <c r="F84" s="67"/>
-      <c r="G84" s="67"/>
-      <c r="H84" s="67"/>
-      <c r="I84" s="63"/>
-      <c r="J84" s="75"/>
+      <c r="D84" s="85" t="s">
+        <v>62</v>
+      </c>
+      <c r="E84" s="68" t="s">
+        <v>10</v>
+      </c>
+      <c r="F84" s="68">
+        <v>0</v>
+      </c>
+      <c r="G84" s="68">
+        <v>65535</v>
+      </c>
+      <c r="H84" s="68" t="s">
+        <v>13</v>
+      </c>
+      <c r="I84" s="61">
+        <v>1</v>
+      </c>
+      <c r="J84" s="63" t="s">
+        <v>180</v>
+      </c>
       <c r="K84" s="3"/>
       <c r="L84" s="3"/>
       <c r="M84" s="3"/>
@@ -4492,39 +4516,25 @@
       <c r="W84" s="1"/>
       <c r="X84" s="1"/>
     </row>
-    <row r="85" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="80"/>
-      <c r="B85" s="61"/>
+    <row r="85" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="81"/>
+      <c r="B85" s="62"/>
       <c r="C85" s="38" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
-      <c r="D85" s="78" t="s">
-        <v>63</v>
-      </c>
-      <c r="E85" s="67" t="s">
-        <v>10</v>
-      </c>
-      <c r="F85" s="67">
-        <v>0</v>
-      </c>
-      <c r="G85" s="67" t="s">
-        <v>66</v>
-      </c>
-      <c r="H85" s="67" t="s">
-        <v>13</v>
-      </c>
-      <c r="I85" s="61">
-        <v>1</v>
-      </c>
-      <c r="J85" s="74" t="s">
-        <v>180</v>
-      </c>
+      <c r="D85" s="85"/>
+      <c r="E85" s="68"/>
+      <c r="F85" s="68"/>
+      <c r="G85" s="68"/>
+      <c r="H85" s="68"/>
+      <c r="I85" s="62"/>
+      <c r="J85" s="64"/>
       <c r="K85" s="3"/>
       <c r="L85" s="3"/>
-      <c r="M85" s="34"/>
-      <c r="N85" s="34"/>
-      <c r="O85" s="34"/>
-      <c r="P85" s="34"/>
+      <c r="M85" s="3"/>
+      <c r="N85" s="3"/>
+      <c r="O85" s="3"/>
+      <c r="P85" s="3"/>
       <c r="Q85" s="3"/>
       <c r="R85" s="3"/>
       <c r="S85" s="3"/>
@@ -4534,21 +4544,35 @@
       <c r="W85" s="1"/>
       <c r="X85" s="1"/>
     </row>
-    <row r="86" spans="1:24" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="80"/>
-      <c r="B86" s="63"/>
+    <row r="86" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="81"/>
+      <c r="B86" s="61"/>
       <c r="C86" s="38" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
-      <c r="D86" s="78"/>
-      <c r="E86" s="67"/>
-      <c r="F86" s="67"/>
-      <c r="G86" s="67"/>
-      <c r="H86" s="67"/>
-      <c r="I86" s="63"/>
-      <c r="J86" s="75"/>
-      <c r="K86" s="34"/>
-      <c r="L86" s="34"/>
+      <c r="D86" s="85" t="s">
+        <v>63</v>
+      </c>
+      <c r="E86" s="68" t="s">
+        <v>10</v>
+      </c>
+      <c r="F86" s="68">
+        <v>0</v>
+      </c>
+      <c r="G86" s="68" t="s">
+        <v>66</v>
+      </c>
+      <c r="H86" s="68" t="s">
+        <v>13</v>
+      </c>
+      <c r="I86" s="61">
+        <v>1</v>
+      </c>
+      <c r="J86" s="63" t="s">
+        <v>180</v>
+      </c>
+      <c r="K86" s="3"/>
+      <c r="L86" s="3"/>
       <c r="M86" s="34"/>
       <c r="N86" s="34"/>
       <c r="O86" s="34"/>
@@ -4562,31 +4586,19 @@
       <c r="W86" s="1"/>
       <c r="X86" s="1"/>
     </row>
-    <row r="87" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="80"/>
-      <c r="B87" s="61"/>
+    <row r="87" spans="1:24" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="81"/>
+      <c r="B87" s="62"/>
       <c r="C87" s="38" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
-      <c r="D87" s="78" t="s">
-        <v>65</v>
-      </c>
-      <c r="E87" s="67" t="s">
-        <v>10</v>
-      </c>
-      <c r="F87" s="67" t="s">
-        <v>67</v>
-      </c>
-      <c r="G87" s="67" t="s">
-        <v>68</v>
-      </c>
-      <c r="H87" s="67" t="s">
-        <v>13</v>
-      </c>
-      <c r="I87" s="61"/>
-      <c r="J87" s="64" t="s">
-        <v>85</v>
-      </c>
+      <c r="D87" s="85"/>
+      <c r="E87" s="68"/>
+      <c r="F87" s="68"/>
+      <c r="G87" s="68"/>
+      <c r="H87" s="68"/>
+      <c r="I87" s="62"/>
+      <c r="J87" s="64"/>
       <c r="K87" s="34"/>
       <c r="L87" s="34"/>
       <c r="M87" s="34"/>
@@ -4602,19 +4614,31 @@
       <c r="W87" s="1"/>
       <c r="X87" s="1"/>
     </row>
-    <row r="88" spans="1:24" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="80"/>
-      <c r="B88" s="63"/>
+    <row r="88" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="81"/>
+      <c r="B88" s="61"/>
       <c r="C88" s="38" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
-      <c r="D88" s="78"/>
-      <c r="E88" s="67"/>
-      <c r="F88" s="67"/>
-      <c r="G88" s="67"/>
-      <c r="H88" s="67"/>
-      <c r="I88" s="63"/>
-      <c r="J88" s="64"/>
+      <c r="D88" s="85" t="s">
+        <v>65</v>
+      </c>
+      <c r="E88" s="68" t="s">
+        <v>10</v>
+      </c>
+      <c r="F88" s="68" t="s">
+        <v>67</v>
+      </c>
+      <c r="G88" s="68" t="s">
+        <v>68</v>
+      </c>
+      <c r="H88" s="68" t="s">
+        <v>13</v>
+      </c>
+      <c r="I88" s="61"/>
+      <c r="J88" s="90" t="s">
+        <v>85</v>
+      </c>
       <c r="K88" s="34"/>
       <c r="L88" s="34"/>
       <c r="M88" s="34"/>
@@ -4630,37 +4654,25 @@
       <c r="W88" s="1"/>
       <c r="X88" s="1"/>
     </row>
-    <row r="89" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A89" s="80"/>
-      <c r="B89" s="61"/>
+    <row r="89" spans="1:24" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A89" s="81"/>
+      <c r="B89" s="62"/>
       <c r="C89" s="38" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
-      <c r="D89" s="78" t="s">
-        <v>64</v>
-      </c>
-      <c r="E89" s="67" t="s">
-        <v>10</v>
-      </c>
-      <c r="F89" s="67" t="s">
-        <v>67</v>
-      </c>
-      <c r="G89" s="67" t="s">
-        <v>68</v>
-      </c>
-      <c r="H89" s="67" t="s">
-        <v>13</v>
-      </c>
-      <c r="I89" s="61"/>
-      <c r="J89" s="64" t="s">
-        <v>86</v>
-      </c>
+      <c r="D89" s="85"/>
+      <c r="E89" s="68"/>
+      <c r="F89" s="68"/>
+      <c r="G89" s="68"/>
+      <c r="H89" s="68"/>
+      <c r="I89" s="62"/>
+      <c r="J89" s="90"/>
       <c r="K89" s="34"/>
       <c r="L89" s="34"/>
-      <c r="M89" s="3"/>
-      <c r="N89" s="3"/>
-      <c r="O89" s="3"/>
-      <c r="P89" s="3"/>
+      <c r="M89" s="34"/>
+      <c r="N89" s="34"/>
+      <c r="O89" s="34"/>
+      <c r="P89" s="34"/>
       <c r="Q89" s="3"/>
       <c r="R89" s="3"/>
       <c r="S89" s="3"/>
@@ -4672,19 +4684,31 @@
     </row>
     <row r="90" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A90" s="81"/>
-      <c r="B90" s="63"/>
+      <c r="B90" s="61"/>
       <c r="C90" s="38" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
-      <c r="D90" s="78"/>
-      <c r="E90" s="67"/>
-      <c r="F90" s="67"/>
-      <c r="G90" s="67"/>
-      <c r="H90" s="67"/>
-      <c r="I90" s="63"/>
-      <c r="J90" s="64"/>
-      <c r="K90" s="3"/>
-      <c r="L90" s="3"/>
+      <c r="D90" s="85" t="s">
+        <v>64</v>
+      </c>
+      <c r="E90" s="68" t="s">
+        <v>10</v>
+      </c>
+      <c r="F90" s="68" t="s">
+        <v>67</v>
+      </c>
+      <c r="G90" s="68" t="s">
+        <v>68</v>
+      </c>
+      <c r="H90" s="68" t="s">
+        <v>13</v>
+      </c>
+      <c r="I90" s="61"/>
+      <c r="J90" s="90" t="s">
+        <v>86</v>
+      </c>
+      <c r="K90" s="34"/>
+      <c r="L90" s="34"/>
       <c r="M90" s="3"/>
       <c r="N90" s="3"/>
       <c r="O90" s="3"/>
@@ -4699,20 +4723,20 @@
       <c r="X90" s="1"/>
     </row>
     <row r="91" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A91" s="24"/>
-      <c r="B91" s="23"/>
-      <c r="C91" s="44" t="s">
-        <v>172</v>
+      <c r="A91" s="82"/>
+      <c r="B91" s="62"/>
+      <c r="C91" s="38" t="s">
+        <v>171</v>
       </c>
-      <c r="D91" s="41"/>
-      <c r="E91" s="18"/>
-      <c r="F91" s="23"/>
-      <c r="G91" s="18"/>
-      <c r="H91" s="18"/>
-      <c r="I91" s="18"/>
-      <c r="J91" s="41"/>
-      <c r="K91" s="24"/>
-      <c r="L91" s="24"/>
+      <c r="D91" s="85"/>
+      <c r="E91" s="68"/>
+      <c r="F91" s="68"/>
+      <c r="G91" s="68"/>
+      <c r="H91" s="68"/>
+      <c r="I91" s="62"/>
+      <c r="J91" s="90"/>
+      <c r="K91" s="3"/>
+      <c r="L91" s="3"/>
       <c r="M91" s="3"/>
       <c r="N91" s="3"/>
       <c r="O91" s="3"/>
@@ -4729,11 +4753,13 @@
     <row r="92" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A92" s="24"/>
       <c r="B92" s="23"/>
-      <c r="C92" s="42"/>
-      <c r="D92" s="24"/>
+      <c r="C92" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="D92" s="41"/>
       <c r="E92" s="18"/>
       <c r="F92" s="23"/>
-      <c r="G92" s="23"/>
+      <c r="G92" s="18"/>
       <c r="H92" s="18"/>
       <c r="I92" s="18"/>
       <c r="J92" s="41"/>
@@ -4755,14 +4781,14 @@
     <row r="93" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A93" s="24"/>
       <c r="B93" s="23"/>
-      <c r="C93" s="18"/>
+      <c r="C93" s="42"/>
       <c r="D93" s="24"/>
       <c r="E93" s="18"/>
       <c r="F93" s="23"/>
       <c r="G93" s="23"/>
       <c r="H93" s="18"/>
       <c r="I93" s="18"/>
-      <c r="J93" s="3"/>
+      <c r="J93" s="41"/>
       <c r="K93" s="24"/>
       <c r="L93" s="24"/>
       <c r="M93" s="3"/>
@@ -4788,7 +4814,7 @@
       <c r="G94" s="23"/>
       <c r="H94" s="18"/>
       <c r="I94" s="18"/>
-      <c r="J94" s="24"/>
+      <c r="J94" s="3"/>
       <c r="K94" s="24"/>
       <c r="L94" s="24"/>
       <c r="M94" s="3"/>
@@ -5560,7 +5586,7 @@
     </row>
     <row r="124" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A124" s="24"/>
-      <c r="B124" s="18"/>
+      <c r="B124" s="23"/>
       <c r="C124" s="18"/>
       <c r="D124" s="24"/>
       <c r="E124" s="18"/>
@@ -7201,9 +7227,9 @@
       <c r="B187" s="18"/>
       <c r="C187" s="18"/>
       <c r="D187" s="24"/>
-      <c r="E187" s="8"/>
-      <c r="F187" s="24"/>
-      <c r="G187" s="24"/>
+      <c r="E187" s="18"/>
+      <c r="F187" s="23"/>
+      <c r="G187" s="23"/>
       <c r="H187" s="18"/>
       <c r="I187" s="18"/>
       <c r="J187" s="24"/>
@@ -8871,8 +8897,8 @@
       <c r="H251" s="18"/>
       <c r="I251" s="18"/>
       <c r="J251" s="24"/>
-      <c r="K251" s="3"/>
-      <c r="L251" s="3"/>
+      <c r="K251" s="24"/>
+      <c r="L251" s="24"/>
       <c r="M251" s="3"/>
       <c r="N251" s="3"/>
       <c r="O251" s="3"/>
@@ -8891,11 +8917,11 @@
       <c r="B252" s="18"/>
       <c r="C252" s="18"/>
       <c r="D252" s="24"/>
-      <c r="E252" s="6"/>
-      <c r="F252" s="3"/>
-      <c r="G252" s="3"/>
-      <c r="H252" s="16"/>
-      <c r="I252" s="16"/>
+      <c r="E252" s="8"/>
+      <c r="F252" s="24"/>
+      <c r="G252" s="24"/>
+      <c r="H252" s="18"/>
+      <c r="I252" s="18"/>
       <c r="J252" s="24"/>
       <c r="K252" s="3"/>
       <c r="L252" s="3"/>
@@ -8948,7 +8974,7 @@
       <c r="G254" s="3"/>
       <c r="H254" s="16"/>
       <c r="I254" s="16"/>
-      <c r="J254" s="3"/>
+      <c r="J254" s="24"/>
       <c r="K254" s="3"/>
       <c r="L254" s="3"/>
       <c r="M254" s="3"/>
@@ -9018,7 +9044,7 @@
     </row>
     <row r="257" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A257" s="24"/>
-      <c r="B257" s="8"/>
+      <c r="B257" s="18"/>
       <c r="C257" s="18"/>
       <c r="D257" s="24"/>
       <c r="E257" s="6"/>
@@ -9070,7 +9096,7 @@
     </row>
     <row r="259" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A259" s="24"/>
-      <c r="B259" s="24"/>
+      <c r="B259" s="8"/>
       <c r="C259" s="18"/>
       <c r="D259" s="24"/>
       <c r="E259" s="6"/>
@@ -9747,7 +9773,7 @@
     <row r="285" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A285" s="24"/>
       <c r="B285" s="24"/>
-      <c r="C285" s="8"/>
+      <c r="C285" s="18"/>
       <c r="D285" s="24"/>
       <c r="E285" s="6"/>
       <c r="F285" s="3"/>
@@ -10603,7 +10629,7 @@
       <c r="X317" s="1"/>
     </row>
     <row r="318" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A318" s="39"/>
+      <c r="A318" s="24"/>
       <c r="B318" s="24"/>
       <c r="C318" s="8"/>
       <c r="D318" s="24"/>
@@ -10620,11 +10646,11 @@
       <c r="O318" s="3"/>
       <c r="P318" s="3"/>
       <c r="Q318" s="3"/>
-      <c r="R318" s="1"/>
-      <c r="S318" s="1"/>
-      <c r="T318" s="1"/>
-      <c r="U318" s="1"/>
-      <c r="V318" s="1"/>
+      <c r="R318" s="3"/>
+      <c r="S318" s="3"/>
+      <c r="T318" s="3"/>
+      <c r="U318" s="3"/>
+      <c r="V318" s="3"/>
       <c r="W318" s="1"/>
       <c r="X318" s="1"/>
     </row>
@@ -10644,8 +10670,8 @@
       <c r="M319" s="3"/>
       <c r="N319" s="3"/>
       <c r="O319" s="3"/>
-      <c r="P319" s="1"/>
-      <c r="Q319" s="1"/>
+      <c r="P319" s="3"/>
+      <c r="Q319" s="3"/>
       <c r="R319" s="1"/>
       <c r="S319" s="1"/>
       <c r="T319" s="1"/>
@@ -10667,9 +10693,9 @@
       <c r="J320" s="3"/>
       <c r="K320" s="3"/>
       <c r="L320" s="3"/>
-      <c r="M320" s="1"/>
-      <c r="N320" s="1"/>
-      <c r="O320" s="1"/>
+      <c r="M320" s="3"/>
+      <c r="N320" s="3"/>
+      <c r="O320" s="3"/>
       <c r="P320" s="1"/>
       <c r="Q320" s="1"/>
       <c r="R320" s="1"/>
@@ -10691,8 +10717,8 @@
       <c r="H321" s="16"/>
       <c r="I321" s="16"/>
       <c r="J321" s="3"/>
-      <c r="K321" s="1"/>
-      <c r="L321" s="1"/>
+      <c r="K321" s="3"/>
+      <c r="L321" s="3"/>
       <c r="M321" s="1"/>
       <c r="N321" s="1"/>
       <c r="O321" s="1"/>
@@ -10768,7 +10794,7 @@
       <c r="G324" s="3"/>
       <c r="H324" s="16"/>
       <c r="I324" s="16"/>
-      <c r="J324" s="1"/>
+      <c r="J324" s="3"/>
       <c r="K324" s="1"/>
       <c r="L324" s="1"/>
       <c r="M324" s="1"/>
@@ -10786,7 +10812,7 @@
     </row>
     <row r="325" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A325" s="39"/>
-      <c r="B325" s="39"/>
+      <c r="B325" s="24"/>
       <c r="C325" s="8"/>
       <c r="D325" s="24"/>
       <c r="E325" s="6"/>
@@ -10839,11 +10865,11 @@
     <row r="327" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A327" s="39"/>
       <c r="B327" s="39"/>
-      <c r="C327" s="11"/>
-      <c r="D327" s="39"/>
-      <c r="E327" s="9"/>
-      <c r="F327" s="1"/>
-      <c r="G327" s="1"/>
+      <c r="C327" s="8"/>
+      <c r="D327" s="24"/>
+      <c r="E327" s="6"/>
+      <c r="F327" s="3"/>
+      <c r="G327" s="3"/>
       <c r="H327" s="16"/>
       <c r="I327" s="16"/>
       <c r="J327" s="1"/>
@@ -11331,7 +11357,7 @@
       <c r="X345" s="1"/>
     </row>
     <row r="346" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A346" s="40"/>
+      <c r="A346" s="39"/>
       <c r="B346" s="39"/>
       <c r="C346" s="11"/>
       <c r="D346" s="39"/>
@@ -11348,6 +11374,13 @@
       <c r="O346" s="1"/>
       <c r="P346" s="1"/>
       <c r="Q346" s="1"/>
+      <c r="R346" s="1"/>
+      <c r="S346" s="1"/>
+      <c r="T346" s="1"/>
+      <c r="U346" s="1"/>
+      <c r="V346" s="1"/>
+      <c r="W346" s="1"/>
+      <c r="X346" s="1"/>
     </row>
     <row r="347" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A347" s="40"/>
@@ -11365,6 +11398,8 @@
       <c r="M347" s="1"/>
       <c r="N347" s="1"/>
       <c r="O347" s="1"/>
+      <c r="P347" s="1"/>
+      <c r="Q347" s="1"/>
     </row>
     <row r="348" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A348" s="40"/>
@@ -11379,6 +11414,9 @@
       <c r="J348" s="1"/>
       <c r="K348" s="1"/>
       <c r="L348" s="1"/>
+      <c r="M348" s="1"/>
+      <c r="N348" s="1"/>
+      <c r="O348" s="1"/>
     </row>
     <row r="349" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A349" s="40"/>
@@ -11391,6 +11429,8 @@
       <c r="H349" s="16"/>
       <c r="I349" s="16"/>
       <c r="J349" s="1"/>
+      <c r="K349" s="1"/>
+      <c r="L349" s="1"/>
     </row>
     <row r="350" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A350" s="40"/>
@@ -11426,9 +11466,11 @@
       <c r="G352" s="1"/>
       <c r="H352" s="16"/>
       <c r="I352" s="16"/>
+      <c r="J352" s="1"/>
     </row>
     <row r="353" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A353" s="40"/>
+      <c r="B353" s="39"/>
       <c r="C353" s="11"/>
       <c r="D353" s="39"/>
       <c r="E353" s="9"/>
@@ -11449,7 +11491,13 @@
     </row>
     <row r="355" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A355" s="40"/>
-      <c r="D355" s="40"/>
+      <c r="C355" s="11"/>
+      <c r="D355" s="39"/>
+      <c r="E355" s="9"/>
+      <c r="F355" s="1"/>
+      <c r="G355" s="1"/>
+      <c r="H355" s="16"/>
+      <c r="I355" s="16"/>
     </row>
     <row r="356" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A356" s="40"/>
@@ -57976,172 +58024,77 @@
       <c r="D11986" s="40"/>
     </row>
     <row r="11987" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11987" s="40"/>
       <c r="D11987" s="40"/>
     </row>
     <row r="11988" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D11988" s="40"/>
     </row>
+    <row r="11989" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11989" s="40"/>
+    </row>
   </sheetData>
   <mergeCells count="243">
-    <mergeCell ref="I77:I78"/>
-    <mergeCell ref="J77:J78"/>
-    <mergeCell ref="I83:I84"/>
-    <mergeCell ref="J83:J84"/>
-    <mergeCell ref="J85:J86"/>
-    <mergeCell ref="I85:I86"/>
-    <mergeCell ref="I87:I88"/>
-    <mergeCell ref="I89:I90"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="D79:D80"/>
-    <mergeCell ref="E79:E80"/>
-    <mergeCell ref="F79:F80"/>
-    <mergeCell ref="G79:G80"/>
-    <mergeCell ref="H79:H80"/>
-    <mergeCell ref="I79:I80"/>
-    <mergeCell ref="D59:D60"/>
-    <mergeCell ref="E59:E60"/>
-    <mergeCell ref="F59:F60"/>
-    <mergeCell ref="G59:G60"/>
-    <mergeCell ref="H59:H60"/>
-    <mergeCell ref="I59:I60"/>
-    <mergeCell ref="H61:H62"/>
-    <mergeCell ref="I67:I68"/>
-    <mergeCell ref="J67:J68"/>
-    <mergeCell ref="I69:I70"/>
-    <mergeCell ref="J69:J70"/>
-    <mergeCell ref="I71:I72"/>
-    <mergeCell ref="J71:J72"/>
-    <mergeCell ref="I73:I74"/>
-    <mergeCell ref="J73:J74"/>
-    <mergeCell ref="I75:I76"/>
-    <mergeCell ref="J75:J76"/>
-    <mergeCell ref="I57:I58"/>
-    <mergeCell ref="I53:I54"/>
-    <mergeCell ref="J32:J33"/>
-    <mergeCell ref="J40:J41"/>
-    <mergeCell ref="J61:J62"/>
-    <mergeCell ref="I61:I62"/>
-    <mergeCell ref="I63:I64"/>
-    <mergeCell ref="J63:J64"/>
-    <mergeCell ref="I65:I66"/>
-    <mergeCell ref="J65:J66"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="A5:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B31:B32"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="A79:A90"/>
-    <mergeCell ref="B89:B90"/>
-    <mergeCell ref="A31:A38"/>
-    <mergeCell ref="A39:A58"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="A17:A30"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="B73:B74"/>
-    <mergeCell ref="E83:E84"/>
-    <mergeCell ref="E85:E86"/>
-    <mergeCell ref="E87:E88"/>
-    <mergeCell ref="E89:E90"/>
-    <mergeCell ref="D83:D84"/>
-    <mergeCell ref="D85:D86"/>
-    <mergeCell ref="D87:D88"/>
-    <mergeCell ref="D89:D90"/>
-    <mergeCell ref="B79:B80"/>
-    <mergeCell ref="B81:B82"/>
-    <mergeCell ref="G83:G84"/>
-    <mergeCell ref="F85:F86"/>
-    <mergeCell ref="G85:G86"/>
-    <mergeCell ref="G87:G88"/>
-    <mergeCell ref="F87:F88"/>
-    <mergeCell ref="F89:F90"/>
-    <mergeCell ref="G89:G90"/>
-    <mergeCell ref="H83:H84"/>
-    <mergeCell ref="H85:H86"/>
-    <mergeCell ref="H87:H88"/>
-    <mergeCell ref="H89:H90"/>
-    <mergeCell ref="F83:F84"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="I32:I33"/>
-    <mergeCell ref="J26:J27"/>
-    <mergeCell ref="I40:I41"/>
-    <mergeCell ref="I45:I46"/>
-    <mergeCell ref="H49:H50"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="H53:H54"/>
-    <mergeCell ref="H57:H58"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="G32:G33"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="F40:F41"/>
-    <mergeCell ref="G40:G41"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="D57:D58"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="G45:G46"/>
-    <mergeCell ref="E57:E58"/>
-    <mergeCell ref="F57:F58"/>
-    <mergeCell ref="G57:G58"/>
+    <mergeCell ref="A60:A79"/>
+    <mergeCell ref="B78:B79"/>
+    <mergeCell ref="B84:B85"/>
+    <mergeCell ref="B86:B87"/>
+    <mergeCell ref="B88:B89"/>
+    <mergeCell ref="J90:J91"/>
+    <mergeCell ref="J88:J89"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="D78:D79"/>
+    <mergeCell ref="E78:E79"/>
+    <mergeCell ref="F78:F79"/>
+    <mergeCell ref="G78:G79"/>
+    <mergeCell ref="H78:H79"/>
+    <mergeCell ref="D76:D77"/>
+    <mergeCell ref="E76:E77"/>
+    <mergeCell ref="F76:F77"/>
+    <mergeCell ref="G76:G77"/>
+    <mergeCell ref="H76:H77"/>
+    <mergeCell ref="D74:D75"/>
+    <mergeCell ref="E74:E75"/>
+    <mergeCell ref="E66:E67"/>
+    <mergeCell ref="G66:G67"/>
+    <mergeCell ref="F66:F67"/>
+    <mergeCell ref="F74:F75"/>
+    <mergeCell ref="G74:G75"/>
+    <mergeCell ref="H74:H75"/>
+    <mergeCell ref="D72:D73"/>
+    <mergeCell ref="E72:E73"/>
+    <mergeCell ref="F72:F73"/>
+    <mergeCell ref="G72:G73"/>
+    <mergeCell ref="H72:H73"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="F70:F71"/>
+    <mergeCell ref="G70:G71"/>
+    <mergeCell ref="H70:H71"/>
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="B76:B77"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="E62:E63"/>
+    <mergeCell ref="F62:F63"/>
+    <mergeCell ref="G62:G63"/>
+    <mergeCell ref="D64:D65"/>
+    <mergeCell ref="H46:H47"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="F50:F51"/>
+    <mergeCell ref="G50:G51"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="F54:F55"/>
+    <mergeCell ref="G54:G55"/>
+    <mergeCell ref="H66:H67"/>
+    <mergeCell ref="H64:H65"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="E68:E69"/>
+    <mergeCell ref="F68:F69"/>
+    <mergeCell ref="G68:G69"/>
+    <mergeCell ref="H68:H69"/>
+    <mergeCell ref="D66:D67"/>
+    <mergeCell ref="E64:E65"/>
+    <mergeCell ref="F64:F65"/>
+    <mergeCell ref="G64:G65"/>
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="B21:B22"/>
@@ -58166,66 +58119,165 @@
     <mergeCell ref="H9:H10"/>
     <mergeCell ref="H11:H12"/>
     <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B75:B76"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="E61:E62"/>
-    <mergeCell ref="F61:F62"/>
-    <mergeCell ref="G61:G62"/>
-    <mergeCell ref="D63:D64"/>
-    <mergeCell ref="H45:H46"/>
-    <mergeCell ref="E49:E50"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="G49:G50"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="F53:F54"/>
-    <mergeCell ref="G53:G54"/>
-    <mergeCell ref="H65:H66"/>
-    <mergeCell ref="H63:H64"/>
-    <mergeCell ref="D67:D68"/>
-    <mergeCell ref="E67:E68"/>
-    <mergeCell ref="F67:F68"/>
-    <mergeCell ref="G67:G68"/>
-    <mergeCell ref="H67:H68"/>
-    <mergeCell ref="D65:D66"/>
-    <mergeCell ref="E63:E64"/>
-    <mergeCell ref="F63:F64"/>
-    <mergeCell ref="G63:G64"/>
-    <mergeCell ref="G73:G74"/>
-    <mergeCell ref="H73:H74"/>
-    <mergeCell ref="D71:D72"/>
-    <mergeCell ref="E71:E72"/>
-    <mergeCell ref="F71:F72"/>
-    <mergeCell ref="G71:G72"/>
-    <mergeCell ref="H71:H72"/>
-    <mergeCell ref="E69:E70"/>
-    <mergeCell ref="F69:F70"/>
-    <mergeCell ref="G69:G70"/>
-    <mergeCell ref="H69:H70"/>
-    <mergeCell ref="D69:D70"/>
-    <mergeCell ref="A59:A78"/>
-    <mergeCell ref="B77:B78"/>
-    <mergeCell ref="B83:B84"/>
-    <mergeCell ref="B85:B86"/>
-    <mergeCell ref="B87:B88"/>
-    <mergeCell ref="J89:J90"/>
-    <mergeCell ref="J87:J88"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="D77:D78"/>
-    <mergeCell ref="E77:E78"/>
-    <mergeCell ref="F77:F78"/>
-    <mergeCell ref="G77:G78"/>
-    <mergeCell ref="H77:H78"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="E75:E76"/>
-    <mergeCell ref="F75:F76"/>
-    <mergeCell ref="G75:G76"/>
-    <mergeCell ref="H75:H76"/>
-    <mergeCell ref="D73:D74"/>
-    <mergeCell ref="E73:E74"/>
-    <mergeCell ref="E65:E66"/>
-    <mergeCell ref="G65:G66"/>
-    <mergeCell ref="F65:F66"/>
-    <mergeCell ref="F73:F74"/>
+    <mergeCell ref="H54:H55"/>
+    <mergeCell ref="H58:H59"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="G33:G34"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="F46:F47"/>
+    <mergeCell ref="G46:G47"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="F58:F59"/>
+    <mergeCell ref="G58:G59"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="I33:I34"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="I41:I42"/>
+    <mergeCell ref="I46:I47"/>
+    <mergeCell ref="H50:H51"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="G84:G85"/>
+    <mergeCell ref="F86:F87"/>
+    <mergeCell ref="G86:G87"/>
+    <mergeCell ref="G88:G89"/>
+    <mergeCell ref="F88:F89"/>
+    <mergeCell ref="F90:F91"/>
+    <mergeCell ref="G90:G91"/>
+    <mergeCell ref="H84:H85"/>
+    <mergeCell ref="H86:H87"/>
+    <mergeCell ref="H88:H89"/>
+    <mergeCell ref="H90:H91"/>
+    <mergeCell ref="F84:F85"/>
+    <mergeCell ref="E84:E85"/>
+    <mergeCell ref="E86:E87"/>
+    <mergeCell ref="E88:E89"/>
+    <mergeCell ref="E90:E91"/>
+    <mergeCell ref="D84:D85"/>
+    <mergeCell ref="D86:D87"/>
+    <mergeCell ref="D88:D89"/>
+    <mergeCell ref="D90:D91"/>
+    <mergeCell ref="B80:B81"/>
+    <mergeCell ref="B82:B83"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="A80:A91"/>
+    <mergeCell ref="B90:B91"/>
+    <mergeCell ref="A32:A39"/>
+    <mergeCell ref="A40:A59"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="A17:A30"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="B70:B71"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="A5:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="I54:I55"/>
+    <mergeCell ref="J33:J34"/>
+    <mergeCell ref="J41:J42"/>
+    <mergeCell ref="J62:J63"/>
+    <mergeCell ref="I62:I63"/>
+    <mergeCell ref="I64:I65"/>
+    <mergeCell ref="J64:J65"/>
+    <mergeCell ref="I66:I67"/>
+    <mergeCell ref="J66:J67"/>
+    <mergeCell ref="I70:I71"/>
+    <mergeCell ref="J70:J71"/>
+    <mergeCell ref="I72:I73"/>
+    <mergeCell ref="J72:J73"/>
+    <mergeCell ref="I74:I75"/>
+    <mergeCell ref="J74:J75"/>
+    <mergeCell ref="I76:I77"/>
+    <mergeCell ref="J76:J77"/>
+    <mergeCell ref="I58:I59"/>
+    <mergeCell ref="I78:I79"/>
+    <mergeCell ref="J78:J79"/>
+    <mergeCell ref="I84:I85"/>
+    <mergeCell ref="J84:J85"/>
+    <mergeCell ref="J86:J87"/>
+    <mergeCell ref="I86:I87"/>
+    <mergeCell ref="I88:I89"/>
+    <mergeCell ref="I90:I91"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="D80:D81"/>
+    <mergeCell ref="E80:E81"/>
+    <mergeCell ref="F80:F81"/>
+    <mergeCell ref="G80:G81"/>
+    <mergeCell ref="H80:H81"/>
+    <mergeCell ref="I80:I81"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="F60:F61"/>
+    <mergeCell ref="G60:G61"/>
+    <mergeCell ref="H60:H61"/>
+    <mergeCell ref="I60:I61"/>
+    <mergeCell ref="H62:H63"/>
+    <mergeCell ref="I68:I69"/>
+    <mergeCell ref="J68:J69"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="55" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -58236,7 +58288,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
@@ -58250,204 +58302,204 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="95" t="s">
+      <c r="A1" s="100" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="67">
+      <c r="B1" s="68">
         <v>1</v>
       </c>
       <c r="C1" s="19">
         <v>1</v>
       </c>
-      <c r="D1" s="64" t="s">
+      <c r="D1" s="90" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="67" t="s">
+      <c r="E1" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="67"/>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67" t="s">
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="95"/>
-      <c r="B2" s="67"/>
+      <c r="A2" s="100"/>
+      <c r="B2" s="68"/>
       <c r="C2" s="19">
         <v>2</v>
       </c>
-      <c r="D2" s="64"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
+      <c r="D2" s="90"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="95"/>
-      <c r="B3" s="67">
+      <c r="A3" s="100"/>
+      <c r="B3" s="68">
         <v>2</v>
       </c>
       <c r="C3" s="19">
         <v>3</v>
       </c>
-      <c r="D3" s="64" t="s">
+      <c r="D3" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="67" t="s">
+      <c r="E3" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67" t="s">
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="95"/>
-      <c r="B4" s="67"/>
+      <c r="A4" s="100"/>
+      <c r="B4" s="68"/>
       <c r="C4" s="19">
         <v>4</v>
       </c>
-      <c r="D4" s="64"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
+      <c r="D4" s="90"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="68"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="95"/>
-      <c r="B5" s="67">
+      <c r="A5" s="100"/>
+      <c r="B5" s="68">
         <v>3</v>
       </c>
       <c r="C5" s="19">
         <v>5</v>
       </c>
-      <c r="D5" s="64" t="s">
+      <c r="D5" s="90" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="67" t="s">
+      <c r="E5" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="67"/>
-      <c r="G5" s="67"/>
-      <c r="H5" s="67" t="s">
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="95"/>
-      <c r="B6" s="67"/>
+      <c r="A6" s="100"/>
+      <c r="B6" s="68"/>
       <c r="C6" s="19">
         <v>6</v>
       </c>
-      <c r="D6" s="64"/>
-      <c r="E6" s="67"/>
-      <c r="F6" s="67"/>
-      <c r="G6" s="67"/>
-      <c r="H6" s="67"/>
+      <c r="D6" s="90"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="68"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="95"/>
-      <c r="B7" s="77">
+      <c r="A7" s="100"/>
+      <c r="B7" s="101">
         <v>4</v>
       </c>
       <c r="C7" s="20">
         <v>7</v>
       </c>
-      <c r="D7" s="76" t="s">
+      <c r="D7" s="102" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="77" t="s">
+      <c r="E7" s="101" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="77"/>
-      <c r="G7" s="77"/>
-      <c r="H7" s="77" t="s">
+      <c r="F7" s="101"/>
+      <c r="G7" s="101"/>
+      <c r="H7" s="101" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="95"/>
-      <c r="B8" s="77"/>
+      <c r="A8" s="100"/>
+      <c r="B8" s="101"/>
       <c r="C8" s="20">
         <v>8</v>
       </c>
-      <c r="D8" s="76"/>
-      <c r="E8" s="77"/>
-      <c r="F8" s="77"/>
-      <c r="G8" s="77"/>
-      <c r="H8" s="77"/>
+      <c r="D8" s="102"/>
+      <c r="E8" s="101"/>
+      <c r="F8" s="101"/>
+      <c r="G8" s="101"/>
+      <c r="H8" s="101"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="95"/>
-      <c r="B9" s="67">
+      <c r="A9" s="100"/>
+      <c r="B9" s="68">
         <v>5</v>
       </c>
       <c r="C9" s="19">
         <v>9</v>
       </c>
-      <c r="D9" s="94" t="s">
+      <c r="D9" s="99" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="67" t="s">
+      <c r="E9" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="67"/>
-      <c r="G9" s="67"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="68"/>
       <c r="H9" s="19"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="95"/>
-      <c r="B10" s="67"/>
+      <c r="A10" s="100"/>
+      <c r="B10" s="68"/>
       <c r="C10" s="19">
         <v>10</v>
       </c>
-      <c r="D10" s="94"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="67"/>
+      <c r="D10" s="99"/>
+      <c r="E10" s="68"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="68"/>
       <c r="H10" s="19" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="93"/>
-      <c r="B11" s="67">
+      <c r="A11" s="98"/>
+      <c r="B11" s="68">
         <v>6</v>
       </c>
       <c r="C11" s="19">
         <v>11</v>
       </c>
-      <c r="D11" s="64" t="s">
+      <c r="D11" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="67" t="s">
+      <c r="E11" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="67"/>
-      <c r="G11" s="67"/>
-      <c r="H11" s="67" t="s">
+      <c r="F11" s="68"/>
+      <c r="G11" s="68"/>
+      <c r="H11" s="68" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="93"/>
-      <c r="B12" s="67"/>
+      <c r="A12" s="98"/>
+      <c r="B12" s="68"/>
       <c r="C12" s="19">
         <v>12</v>
       </c>
-      <c r="D12" s="64"/>
-      <c r="E12" s="67"/>
-      <c r="F12" s="67"/>
-      <c r="G12" s="67"/>
-      <c r="H12" s="67"/>
+      <c r="D12" s="90"/>
+      <c r="E12" s="68"/>
+      <c r="F12" s="68"/>
+      <c r="G12" s="68"/>
+      <c r="H12" s="68"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="93" t="s">
+      <c r="A14" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="93"/>
+      <c r="B14" s="98"/>
       <c r="C14" s="25" t="s">
         <v>9</v>
       </c>
@@ -58612,10 +58664,10 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="67" t="s">
+      <c r="A33" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="67"/>
+      <c r="B33" s="68"/>
       <c r="C33" s="32" t="s">
         <v>9</v>
       </c>
@@ -58633,7 +58685,7 @@
       <c r="E34" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="F34" s="97" t="s">
+      <c r="F34" s="58" t="s">
         <v>192</v>
       </c>
     </row>
@@ -58644,7 +58696,7 @@
       <c r="E35" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="F35" s="98" t="s">
+      <c r="F35" s="59" t="s">
         <v>193</v>
       </c>
     </row>
@@ -58663,7 +58715,7 @@
       <c r="D37" t="s">
         <v>205</v>
       </c>
-      <c r="E37" s="99" t="s">
+      <c r="E37" s="60" t="s">
         <v>196</v>
       </c>
       <c r="F37" t="s">
@@ -58674,7 +58726,7 @@
       <c r="D38" t="s">
         <v>206</v>
       </c>
-      <c r="E38" s="99" t="s">
+      <c r="E38" s="60" t="s">
         <v>198</v>
       </c>
       <c r="F38" t="s">
@@ -58685,7 +58737,7 @@
       <c r="D39" t="s">
         <v>207</v>
       </c>
-      <c r="E39" s="99" t="s">
+      <c r="E39" s="60" t="s">
         <v>200</v>
       </c>
       <c r="F39" t="s">
@@ -58694,6 +58746,29 @@
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="H11:H12"/>
@@ -58710,29 +58785,6 @@
     <mergeCell ref="F11:F12"/>
     <mergeCell ref="A1:A10"/>
     <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
copleted with config map, need some validation
</commit_message>
<xml_diff>
--- a/Карта конфигурации.xlsx
+++ b/Карта конфигурации.xlsx
@@ -1051,29 +1051,19 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1084,34 +1074,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1120,11 +1086,20 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1132,17 +1107,32 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
@@ -1155,45 +1145,49 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1202,6 +1196,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1512,8 +1512,8 @@
   </sheetPr>
   <dimension ref="A1:X11989"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66:D67"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="G132" sqref="G132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1531,18 +1531,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="115" t="s">
+      <c r="A1" s="72" t="s">
         <v>191</v>
       </c>
-      <c r="B1" s="115"/>
-      <c r="C1" s="115"/>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="115"/>
-      <c r="G1" s="115"/>
-      <c r="H1" s="115"/>
-      <c r="I1" s="115"/>
-      <c r="J1" s="115"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B2" s="23"/>
@@ -1552,15 +1552,15 @@
       <c r="A3" s="32" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="85">
+      <c r="B3" s="107">
         <v>1000</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
+      <c r="C3" s="107"/>
+      <c r="D3" s="107"/>
+      <c r="E3" s="107"/>
+      <c r="F3" s="107"/>
+      <c r="G3" s="107"/>
+      <c r="H3" s="107"/>
       <c r="I3" s="42"/>
       <c r="J3" s="44"/>
       <c r="K3" s="2"/>
@@ -1623,28 +1623,28 @@
       <c r="X4" s="1"/>
     </row>
     <row r="5" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="107" t="s">
+      <c r="A5" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="86">
+      <c r="B5" s="90">
         <v>0</v>
       </c>
       <c r="C5" s="49">
         <v>0</v>
       </c>
-      <c r="D5" s="87" t="s">
+      <c r="D5" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="86" t="s">
+      <c r="E5" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="86"/>
-      <c r="G5" s="86"/>
-      <c r="H5" s="86" t="s">
+      <c r="F5" s="90"/>
+      <c r="G5" s="90"/>
+      <c r="H5" s="90" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="94"/>
-      <c r="J5" s="87" t="s">
+      <c r="I5" s="85"/>
+      <c r="J5" s="80" t="s">
         <v>173</v>
       </c>
       <c r="K5" s="3"/>
@@ -1663,18 +1663,18 @@
       <c r="X5" s="1"/>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="107"/>
-      <c r="B6" s="86"/>
+      <c r="A6" s="87"/>
+      <c r="B6" s="90"/>
       <c r="C6" s="49">
         <v>1</v>
       </c>
-      <c r="D6" s="87"/>
-      <c r="E6" s="86"/>
-      <c r="F6" s="86"/>
-      <c r="G6" s="86"/>
-      <c r="H6" s="86"/>
-      <c r="I6" s="95"/>
-      <c r="J6" s="87"/>
+      <c r="D6" s="80"/>
+      <c r="E6" s="90"/>
+      <c r="F6" s="90"/>
+      <c r="G6" s="90"/>
+      <c r="H6" s="90"/>
+      <c r="I6" s="86"/>
+      <c r="J6" s="80"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
@@ -1691,28 +1691,28 @@
       <c r="X6" s="1"/>
     </row>
     <row r="7" spans="1:24" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="107"/>
-      <c r="B7" s="79">
+      <c r="A7" s="87"/>
+      <c r="B7" s="75">
         <v>1</v>
       </c>
       <c r="C7" s="34">
         <v>2</v>
       </c>
-      <c r="D7" s="74" t="s">
+      <c r="D7" s="108" t="s">
         <v>91</v>
       </c>
-      <c r="E7" s="79" t="s">
+      <c r="E7" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="79">
+      <c r="F7" s="75">
         <v>1</v>
       </c>
-      <c r="G7" s="79"/>
-      <c r="H7" s="79" t="s">
+      <c r="G7" s="75"/>
+      <c r="H7" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="105"/>
-      <c r="J7" s="109" t="s">
+      <c r="I7" s="81"/>
+      <c r="J7" s="89" t="s">
         <v>92</v>
       </c>
       <c r="K7" s="3"/>
@@ -1731,18 +1731,18 @@
       <c r="X7" s="1"/>
     </row>
     <row r="8" spans="1:24" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="107"/>
-      <c r="B8" s="79"/>
+      <c r="A8" s="87"/>
+      <c r="B8" s="75"/>
       <c r="C8" s="34">
         <v>3</v>
       </c>
-      <c r="D8" s="74"/>
-      <c r="E8" s="79"/>
-      <c r="F8" s="79"/>
-      <c r="G8" s="79"/>
-      <c r="H8" s="79"/>
-      <c r="I8" s="106"/>
-      <c r="J8" s="109"/>
+      <c r="D8" s="108"/>
+      <c r="E8" s="75"/>
+      <c r="F8" s="75"/>
+      <c r="G8" s="75"/>
+      <c r="H8" s="75"/>
+      <c r="I8" s="82"/>
+      <c r="J8" s="89"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
@@ -1759,26 +1759,26 @@
       <c r="X8" s="1"/>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A9" s="107"/>
-      <c r="B9" s="79">
+      <c r="A9" s="87"/>
+      <c r="B9" s="75">
         <v>2</v>
       </c>
       <c r="C9" s="34">
         <v>4</v>
       </c>
-      <c r="D9" s="74" t="s">
+      <c r="D9" s="108" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="79" t="s">
+      <c r="E9" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="79"/>
-      <c r="G9" s="79"/>
-      <c r="H9" s="79" t="s">
+      <c r="F9" s="75"/>
+      <c r="G9" s="75"/>
+      <c r="H9" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="105"/>
-      <c r="J9" s="109" t="s">
+      <c r="I9" s="81"/>
+      <c r="J9" s="89" t="s">
         <v>95</v>
       </c>
       <c r="K9" s="3"/>
@@ -1797,18 +1797,18 @@
       <c r="X9" s="1"/>
     </row>
     <row r="10" spans="1:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="107"/>
-      <c r="B10" s="79"/>
+      <c r="A10" s="87"/>
+      <c r="B10" s="75"/>
       <c r="C10" s="34">
         <v>5</v>
       </c>
-      <c r="D10" s="74"/>
-      <c r="E10" s="79"/>
-      <c r="F10" s="79"/>
-      <c r="G10" s="79"/>
-      <c r="H10" s="79"/>
-      <c r="I10" s="106"/>
-      <c r="J10" s="109"/>
+      <c r="D10" s="108"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="75"/>
+      <c r="I10" s="82"/>
+      <c r="J10" s="89"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
@@ -1825,26 +1825,26 @@
       <c r="X10" s="1"/>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A11" s="107"/>
-      <c r="B11" s="111">
+      <c r="A11" s="87"/>
+      <c r="B11" s="93">
         <v>3</v>
       </c>
       <c r="C11" s="50">
         <v>6</v>
       </c>
-      <c r="D11" s="112" t="s">
+      <c r="D11" s="94" t="s">
         <v>190</v>
       </c>
-      <c r="E11" s="111" t="s">
+      <c r="E11" s="93" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="111"/>
-      <c r="G11" s="111"/>
-      <c r="H11" s="88" t="s">
+      <c r="F11" s="93"/>
+      <c r="G11" s="93"/>
+      <c r="H11" s="109" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="105"/>
-      <c r="J11" s="109" t="s">
+      <c r="I11" s="81"/>
+      <c r="J11" s="89" t="s">
         <v>93</v>
       </c>
       <c r="K11" s="3"/>
@@ -1863,18 +1863,18 @@
       <c r="X11" s="1"/>
     </row>
     <row r="12" spans="1:24" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="107"/>
-      <c r="B12" s="111"/>
+      <c r="A12" s="87"/>
+      <c r="B12" s="93"/>
       <c r="C12" s="50">
         <v>7</v>
       </c>
-      <c r="D12" s="112"/>
-      <c r="E12" s="111"/>
-      <c r="F12" s="111"/>
-      <c r="G12" s="111"/>
-      <c r="H12" s="88"/>
-      <c r="I12" s="106"/>
-      <c r="J12" s="109"/>
+      <c r="D12" s="94"/>
+      <c r="E12" s="93"/>
+      <c r="F12" s="93"/>
+      <c r="G12" s="93"/>
+      <c r="H12" s="109"/>
+      <c r="I12" s="82"/>
+      <c r="J12" s="89"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
@@ -1891,27 +1891,27 @@
       <c r="X12" s="1"/>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A13" s="107"/>
-      <c r="B13" s="89">
+      <c r="A13" s="87"/>
+      <c r="B13" s="92">
         <v>4</v>
       </c>
       <c r="C13" s="46">
         <v>8</v>
       </c>
-      <c r="D13" s="110" t="s">
+      <c r="D13" s="91" t="s">
         <v>90</v>
       </c>
-      <c r="E13" s="89" t="s">
+      <c r="E13" s="92" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="89" t="s">
+      <c r="F13" s="92" t="s">
         <v>209</v>
       </c>
-      <c r="G13" s="89"/>
-      <c r="H13" s="75" t="s">
+      <c r="G13" s="92"/>
+      <c r="H13" s="83" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="75"/>
+      <c r="I13" s="83"/>
       <c r="J13" s="63"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
@@ -1929,17 +1929,17 @@
       <c r="X13" s="1"/>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A14" s="107"/>
-      <c r="B14" s="89"/>
+      <c r="A14" s="87"/>
+      <c r="B14" s="92"/>
       <c r="C14" s="46">
         <v>9</v>
       </c>
-      <c r="D14" s="110"/>
-      <c r="E14" s="89"/>
-      <c r="F14" s="89"/>
-      <c r="G14" s="89"/>
-      <c r="H14" s="76"/>
-      <c r="I14" s="76"/>
+      <c r="D14" s="91"/>
+      <c r="E14" s="92"/>
+      <c r="F14" s="92"/>
+      <c r="G14" s="92"/>
+      <c r="H14" s="84"/>
+      <c r="I14" s="84"/>
       <c r="J14" s="63"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
@@ -1957,26 +1957,26 @@
       <c r="X14" s="1"/>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A15" s="108"/>
-      <c r="B15" s="98" t="s">
+      <c r="A15" s="88"/>
+      <c r="B15" s="104" t="s">
         <v>203</v>
       </c>
       <c r="C15" s="49">
         <v>10.11</v>
       </c>
-      <c r="D15" s="87" t="s">
+      <c r="D15" s="80" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="86" t="s">
+      <c r="E15" s="90" t="s">
         <v>195</v>
       </c>
-      <c r="F15" s="86"/>
-      <c r="G15" s="86"/>
-      <c r="H15" s="86" t="s">
+      <c r="F15" s="90"/>
+      <c r="G15" s="90"/>
+      <c r="H15" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="I15" s="94"/>
-      <c r="J15" s="87" t="s">
+      <c r="I15" s="85"/>
+      <c r="J15" s="80" t="s">
         <v>173</v>
       </c>
       <c r="K15" s="3"/>
@@ -1995,18 +1995,18 @@
       <c r="X15" s="1"/>
     </row>
     <row r="16" spans="1:24" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="108"/>
-      <c r="B16" s="86"/>
+      <c r="A16" s="88"/>
+      <c r="B16" s="90"/>
       <c r="C16" s="49">
         <v>12.13</v>
       </c>
-      <c r="D16" s="87"/>
-      <c r="E16" s="86"/>
-      <c r="F16" s="86"/>
-      <c r="G16" s="86"/>
-      <c r="H16" s="86"/>
-      <c r="I16" s="95"/>
-      <c r="J16" s="87"/>
+      <c r="D16" s="80"/>
+      <c r="E16" s="90"/>
+      <c r="F16" s="90"/>
+      <c r="G16" s="90"/>
+      <c r="H16" s="90"/>
+      <c r="I16" s="86"/>
+      <c r="J16" s="80"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
@@ -2023,10 +2023,10 @@
       <c r="X16" s="1"/>
     </row>
     <row r="17" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="100" t="s">
+      <c r="A17" s="96" t="s">
         <v>84</v>
       </c>
-      <c r="B17" s="86">
+      <c r="B17" s="90">
         <v>1</v>
       </c>
       <c r="C17" s="49" t="s">
@@ -2069,8 +2069,8 @@
       <c r="X17" s="1"/>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A18" s="101"/>
-      <c r="B18" s="86"/>
+      <c r="A18" s="97"/>
+      <c r="B18" s="90"/>
       <c r="C18" s="49" t="s">
         <v>99</v>
       </c>
@@ -2109,29 +2109,29 @@
       <c r="X18" s="1"/>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A19" s="101"/>
-      <c r="B19" s="86">
+      <c r="A19" s="97"/>
+      <c r="B19" s="90">
         <v>2</v>
       </c>
       <c r="C19" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="D19" s="87" t="s">
+      <c r="D19" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="86" t="s">
+      <c r="E19" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="F19" s="86">
+      <c r="F19" s="90">
         <v>1200</v>
       </c>
-      <c r="G19" s="86">
+      <c r="G19" s="90">
         <v>57600</v>
       </c>
-      <c r="H19" s="86" t="s">
+      <c r="H19" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="I19" s="94">
+      <c r="I19" s="85">
         <v>9600</v>
       </c>
       <c r="J19" s="51"/>
@@ -2151,17 +2151,17 @@
       <c r="X19" s="1"/>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A20" s="101"/>
-      <c r="B20" s="86"/>
+      <c r="A20" s="97"/>
+      <c r="B20" s="90"/>
       <c r="C20" s="49" t="s">
         <v>101</v>
       </c>
-      <c r="D20" s="87"/>
-      <c r="E20" s="86"/>
-      <c r="F20" s="86"/>
-      <c r="G20" s="86"/>
-      <c r="H20" s="86"/>
-      <c r="I20" s="95"/>
+      <c r="D20" s="80"/>
+      <c r="E20" s="90"/>
+      <c r="F20" s="90"/>
+      <c r="G20" s="90"/>
+      <c r="H20" s="90"/>
+      <c r="I20" s="86"/>
       <c r="J20" s="51"/>
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
@@ -2179,8 +2179,8 @@
       <c r="X20" s="1"/>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A21" s="101"/>
-      <c r="B21" s="86">
+      <c r="A21" s="97"/>
+      <c r="B21" s="90">
         <v>3</v>
       </c>
       <c r="C21" s="49" t="s">
@@ -2221,8 +2221,8 @@
       <c r="X21" s="1"/>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A22" s="101"/>
-      <c r="B22" s="86"/>
+      <c r="A22" s="97"/>
+      <c r="B22" s="90"/>
       <c r="C22" s="49" t="s">
         <v>103</v>
       </c>
@@ -2263,8 +2263,8 @@
       <c r="X22" s="1"/>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A23" s="101"/>
-      <c r="B23" s="86">
+      <c r="A23" s="97"/>
+      <c r="B23" s="90">
         <v>4</v>
       </c>
       <c r="C23" s="49" t="s">
@@ -2305,8 +2305,8 @@
       <c r="X23" s="1"/>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A24" s="101"/>
-      <c r="B24" s="86"/>
+      <c r="A24" s="97"/>
+      <c r="B24" s="90"/>
       <c r="C24" s="49" t="s">
         <v>105</v>
       </c>
@@ -2347,8 +2347,8 @@
       <c r="X24" s="1"/>
     </row>
     <row r="25" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="101"/>
-      <c r="B25" s="86">
+      <c r="A25" s="97"/>
+      <c r="B25" s="90">
         <v>5</v>
       </c>
       <c r="C25" s="49" t="s">
@@ -2391,30 +2391,30 @@
       <c r="X25" s="1"/>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A26" s="101"/>
-      <c r="B26" s="86"/>
+      <c r="A26" s="97"/>
+      <c r="B26" s="90"/>
       <c r="C26" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="D26" s="92" t="s">
+      <c r="D26" s="102" t="s">
         <v>30</v>
       </c>
-      <c r="E26" s="86" t="s">
+      <c r="E26" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="F26" s="94">
+      <c r="F26" s="85">
         <v>0</v>
       </c>
-      <c r="G26" s="94">
+      <c r="G26" s="85">
         <v>65535</v>
       </c>
       <c r="H26" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="I26" s="94">
+      <c r="I26" s="85">
         <v>200</v>
       </c>
-      <c r="J26" s="92" t="s">
+      <c r="J26" s="102" t="s">
         <v>177</v>
       </c>
       <c r="K26" s="3"/>
@@ -2433,22 +2433,22 @@
       <c r="X26" s="1"/>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A27" s="101"/>
-      <c r="B27" s="86">
+      <c r="A27" s="97"/>
+      <c r="B27" s="90">
         <v>6</v>
       </c>
       <c r="C27" s="49" t="s">
         <v>108</v>
       </c>
-      <c r="D27" s="93"/>
-      <c r="E27" s="86"/>
-      <c r="F27" s="95"/>
-      <c r="G27" s="95"/>
+      <c r="D27" s="103"/>
+      <c r="E27" s="90"/>
+      <c r="F27" s="86"/>
+      <c r="G27" s="86"/>
       <c r="H27" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="I27" s="95"/>
-      <c r="J27" s="93"/>
+      <c r="I27" s="86"/>
+      <c r="J27" s="103"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
       <c r="M27" s="3"/>
@@ -2465,8 +2465,8 @@
       <c r="X27" s="1"/>
     </row>
     <row r="28" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="101"/>
-      <c r="B28" s="86"/>
+      <c r="A28" s="97"/>
+      <c r="B28" s="90"/>
       <c r="C28" s="49" t="s">
         <v>109</v>
       </c>
@@ -2507,8 +2507,8 @@
       <c r="X28" s="1"/>
     </row>
     <row r="29" spans="1:24" ht="60" x14ac:dyDescent="0.25">
-      <c r="A29" s="101"/>
-      <c r="B29" s="86">
+      <c r="A29" s="97"/>
+      <c r="B29" s="90">
         <v>7</v>
       </c>
       <c r="C29" s="49" t="s">
@@ -2551,8 +2551,8 @@
       <c r="X29" s="1"/>
     </row>
     <row r="30" spans="1:24" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="102"/>
-      <c r="B30" s="86"/>
+      <c r="A30" s="98"/>
+      <c r="B30" s="90"/>
       <c r="C30" s="49" t="s">
         <v>111</v>
       </c>
@@ -2621,10 +2621,10 @@
       <c r="X31" s="61"/>
     </row>
     <row r="32" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="100" t="s">
+      <c r="A32" s="96" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="84"/>
+      <c r="B32" s="95"/>
       <c r="C32" s="64" t="s">
         <v>112</v>
       </c>
@@ -2663,30 +2663,30 @@
       <c r="X32" s="1"/>
     </row>
     <row r="33" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A33" s="101"/>
-      <c r="B33" s="84"/>
+      <c r="A33" s="97"/>
+      <c r="B33" s="95"/>
       <c r="C33" s="64" t="s">
         <v>113</v>
       </c>
-      <c r="D33" s="90" t="s">
+      <c r="D33" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="E33" s="84" t="s">
+      <c r="E33" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="F33" s="82">
+      <c r="F33" s="76">
         <v>0</v>
       </c>
-      <c r="G33" s="82">
+      <c r="G33" s="76">
         <v>65535</v>
       </c>
       <c r="H33" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="I33" s="82">
+      <c r="I33" s="76">
         <v>10</v>
       </c>
-      <c r="J33" s="90" t="s">
+      <c r="J33" s="78" t="s">
         <v>177</v>
       </c>
       <c r="K33" s="3"/>
@@ -2705,20 +2705,20 @@
       <c r="X33" s="1"/>
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A34" s="101"/>
-      <c r="B34" s="84"/>
+      <c r="A34" s="97"/>
+      <c r="B34" s="95"/>
       <c r="C34" s="64" t="s">
         <v>114</v>
       </c>
-      <c r="D34" s="91"/>
-      <c r="E34" s="84"/>
-      <c r="F34" s="83"/>
-      <c r="G34" s="83"/>
+      <c r="D34" s="79"/>
+      <c r="E34" s="95"/>
+      <c r="F34" s="77"/>
+      <c r="G34" s="77"/>
       <c r="H34" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="I34" s="83"/>
-      <c r="J34" s="91"/>
+      <c r="I34" s="77"/>
+      <c r="J34" s="79"/>
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
@@ -2735,8 +2735,8 @@
       <c r="X34" s="1"/>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A35" s="101"/>
-      <c r="B35" s="84"/>
+      <c r="A35" s="97"/>
+      <c r="B35" s="95"/>
       <c r="C35" s="64" t="s">
         <v>115</v>
       </c>
@@ -2767,8 +2767,8 @@
       <c r="X35" s="1"/>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A36" s="101"/>
-      <c r="B36" s="84"/>
+      <c r="A36" s="97"/>
+      <c r="B36" s="95"/>
       <c r="C36" s="64" t="s">
         <v>116</v>
       </c>
@@ -2799,8 +2799,8 @@
       <c r="X36" s="1"/>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A37" s="101"/>
-      <c r="B37" s="84"/>
+      <c r="A37" s="97"/>
+      <c r="B37" s="95"/>
       <c r="C37" s="64" t="s">
         <v>117</v>
       </c>
@@ -2831,8 +2831,8 @@
       <c r="X37" s="1"/>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A38" s="101"/>
-      <c r="B38" s="84"/>
+      <c r="A38" s="97"/>
+      <c r="B38" s="95"/>
       <c r="C38" s="64" t="s">
         <v>118</v>
       </c>
@@ -2863,8 +2863,8 @@
       <c r="X38" s="1"/>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A39" s="101"/>
-      <c r="B39" s="84"/>
+      <c r="A39" s="97"/>
+      <c r="B39" s="95"/>
       <c r="C39" s="64" t="s">
         <v>119</v>
       </c>
@@ -2895,10 +2895,10 @@
       <c r="X39" s="1"/>
     </row>
     <row r="40" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="100" t="s">
+      <c r="A40" s="96" t="s">
         <v>35</v>
       </c>
-      <c r="B40" s="82"/>
+      <c r="B40" s="76"/>
       <c r="C40" s="64" t="s">
         <v>120</v>
       </c>
@@ -2937,30 +2937,30 @@
       <c r="X40" s="1"/>
     </row>
     <row r="41" spans="1:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="103"/>
-      <c r="B41" s="83"/>
+      <c r="A41" s="99"/>
+      <c r="B41" s="77"/>
       <c r="C41" s="64" t="s">
         <v>121</v>
       </c>
-      <c r="D41" s="96" t="s">
+      <c r="D41" s="105" t="s">
         <v>36</v>
       </c>
-      <c r="E41" s="84" t="s">
+      <c r="E41" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="F41" s="82">
+      <c r="F41" s="76">
         <v>0</v>
       </c>
-      <c r="G41" s="82">
+      <c r="G41" s="76">
         <v>65535</v>
       </c>
       <c r="H41" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="I41" s="82">
+      <c r="I41" s="76">
         <v>10</v>
       </c>
-      <c r="J41" s="90" t="s">
+      <c r="J41" s="78" t="s">
         <v>177</v>
       </c>
       <c r="K41" s="3"/>
@@ -2979,20 +2979,20 @@
       <c r="X41" s="1"/>
     </row>
     <row r="42" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A42" s="103"/>
-      <c r="B42" s="82"/>
+      <c r="A42" s="99"/>
+      <c r="B42" s="76"/>
       <c r="C42" s="64" t="s">
         <v>122</v>
       </c>
-      <c r="D42" s="97"/>
-      <c r="E42" s="84"/>
-      <c r="F42" s="83"/>
-      <c r="G42" s="83"/>
+      <c r="D42" s="106"/>
+      <c r="E42" s="95"/>
+      <c r="F42" s="77"/>
+      <c r="G42" s="77"/>
       <c r="H42" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="I42" s="83"/>
-      <c r="J42" s="91"/>
+      <c r="I42" s="77"/>
+      <c r="J42" s="79"/>
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
       <c r="M42" s="3"/>
@@ -3009,8 +3009,8 @@
       <c r="X42" s="1"/>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A43" s="103"/>
-      <c r="B43" s="83"/>
+      <c r="A43" s="99"/>
+      <c r="B43" s="77"/>
       <c r="C43" s="64" t="s">
         <v>123</v>
       </c>
@@ -3041,8 +3041,8 @@
       <c r="X43" s="1"/>
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A44" s="103"/>
-      <c r="B44" s="82"/>
+      <c r="A44" s="99"/>
+      <c r="B44" s="76"/>
       <c r="C44" s="64" t="s">
         <v>124</v>
       </c>
@@ -3083,8 +3083,8 @@
       <c r="X44" s="1"/>
     </row>
     <row r="45" spans="1:24" ht="45" x14ac:dyDescent="0.25">
-      <c r="A45" s="103"/>
-      <c r="B45" s="83"/>
+      <c r="A45" s="99"/>
+      <c r="B45" s="77"/>
       <c r="C45" s="64" t="s">
         <v>125</v>
       </c>
@@ -3125,27 +3125,27 @@
       <c r="X45" s="1"/>
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A46" s="103"/>
-      <c r="B46" s="82"/>
+      <c r="A46" s="99"/>
+      <c r="B46" s="76"/>
       <c r="C46" s="64" t="s">
         <v>126</v>
       </c>
-      <c r="D46" s="90" t="s">
+      <c r="D46" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="E46" s="84" t="s">
+      <c r="E46" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="F46" s="82" t="s">
+      <c r="F46" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="G46" s="82" t="s">
+      <c r="G46" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="H46" s="82" t="s">
+      <c r="H46" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="I46" s="82">
+      <c r="I46" s="76">
         <v>0</v>
       </c>
       <c r="J46" s="65" t="s">
@@ -3167,17 +3167,17 @@
       <c r="X46" s="1"/>
     </row>
     <row r="47" spans="1:24" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="103"/>
-      <c r="B47" s="83"/>
+      <c r="A47" s="99"/>
+      <c r="B47" s="77"/>
       <c r="C47" s="64" t="s">
         <v>127</v>
       </c>
-      <c r="D47" s="91"/>
-      <c r="E47" s="84"/>
-      <c r="F47" s="83"/>
-      <c r="G47" s="83"/>
-      <c r="H47" s="83"/>
-      <c r="I47" s="83"/>
+      <c r="D47" s="79"/>
+      <c r="E47" s="95"/>
+      <c r="F47" s="77"/>
+      <c r="G47" s="77"/>
+      <c r="H47" s="77"/>
+      <c r="I47" s="77"/>
       <c r="J47" s="65" t="s">
         <v>181</v>
       </c>
@@ -3197,8 +3197,8 @@
       <c r="X47" s="1"/>
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A48" s="103"/>
-      <c r="B48" s="82"/>
+      <c r="A48" s="99"/>
+      <c r="B48" s="76"/>
       <c r="C48" s="64" t="s">
         <v>128</v>
       </c>
@@ -3239,8 +3239,8 @@
       <c r="X48" s="1"/>
     </row>
     <row r="49" spans="1:24" ht="45" x14ac:dyDescent="0.25">
-      <c r="A49" s="103"/>
-      <c r="B49" s="83"/>
+      <c r="A49" s="99"/>
+      <c r="B49" s="77"/>
       <c r="C49" s="64" t="s">
         <v>129</v>
       </c>
@@ -3281,24 +3281,24 @@
       <c r="X49" s="1"/>
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A50" s="103"/>
-      <c r="B50" s="82"/>
+      <c r="A50" s="99"/>
+      <c r="B50" s="76"/>
       <c r="C50" s="64" t="s">
         <v>130</v>
       </c>
-      <c r="D50" s="90" t="s">
+      <c r="D50" s="78" t="s">
         <v>45</v>
       </c>
-      <c r="E50" s="84" t="s">
+      <c r="E50" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="F50" s="82" t="s">
+      <c r="F50" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="G50" s="82" t="s">
+      <c r="G50" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="H50" s="82" t="s">
+      <c r="H50" s="76" t="s">
         <v>13</v>
       </c>
       <c r="I50" s="66">
@@ -3323,16 +3323,16 @@
       <c r="X50" s="1"/>
     </row>
     <row r="51" spans="1:24" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="103"/>
-      <c r="B51" s="83"/>
+      <c r="A51" s="99"/>
+      <c r="B51" s="77"/>
       <c r="C51" s="64" t="s">
         <v>131</v>
       </c>
-      <c r="D51" s="91"/>
-      <c r="E51" s="84"/>
-      <c r="F51" s="83"/>
-      <c r="G51" s="83"/>
-      <c r="H51" s="83"/>
+      <c r="D51" s="79"/>
+      <c r="E51" s="95"/>
+      <c r="F51" s="77"/>
+      <c r="G51" s="77"/>
+      <c r="H51" s="77"/>
       <c r="I51" s="66"/>
       <c r="J51" s="65" t="s">
         <v>181</v>
@@ -3353,8 +3353,8 @@
       <c r="X51" s="1"/>
     </row>
     <row r="52" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A52" s="103"/>
-      <c r="B52" s="82"/>
+      <c r="A52" s="99"/>
+      <c r="B52" s="76"/>
       <c r="C52" s="64" t="s">
         <v>132</v>
       </c>
@@ -3395,8 +3395,8 @@
       <c r="X52" s="1"/>
     </row>
     <row r="53" spans="1:24" ht="45" x14ac:dyDescent="0.25">
-      <c r="A53" s="103"/>
-      <c r="B53" s="83"/>
+      <c r="A53" s="99"/>
+      <c r="B53" s="77"/>
       <c r="C53" s="64" t="s">
         <v>133</v>
       </c>
@@ -3437,27 +3437,27 @@
       <c r="X53" s="1"/>
     </row>
     <row r="54" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A54" s="103"/>
-      <c r="B54" s="82"/>
+      <c r="A54" s="99"/>
+      <c r="B54" s="76"/>
       <c r="C54" s="64" t="s">
         <v>134</v>
       </c>
-      <c r="D54" s="90" t="s">
+      <c r="D54" s="78" t="s">
         <v>46</v>
       </c>
-      <c r="E54" s="84" t="s">
+      <c r="E54" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="F54" s="82" t="s">
+      <c r="F54" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="G54" s="82" t="s">
+      <c r="G54" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="H54" s="82" t="s">
+      <c r="H54" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="I54" s="82">
+      <c r="I54" s="76">
         <v>0</v>
       </c>
       <c r="J54" s="65" t="s">
@@ -3479,17 +3479,17 @@
       <c r="X54" s="1"/>
     </row>
     <row r="55" spans="1:24" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="103"/>
-      <c r="B55" s="83"/>
+      <c r="A55" s="99"/>
+      <c r="B55" s="77"/>
       <c r="C55" s="64" t="s">
         <v>135</v>
       </c>
-      <c r="D55" s="91"/>
-      <c r="E55" s="84"/>
-      <c r="F55" s="83"/>
-      <c r="G55" s="83"/>
-      <c r="H55" s="83"/>
-      <c r="I55" s="83"/>
+      <c r="D55" s="79"/>
+      <c r="E55" s="95"/>
+      <c r="F55" s="77"/>
+      <c r="G55" s="77"/>
+      <c r="H55" s="77"/>
+      <c r="I55" s="77"/>
       <c r="J55" s="65" t="s">
         <v>181</v>
       </c>
@@ -3509,8 +3509,8 @@
       <c r="X55" s="1"/>
     </row>
     <row r="56" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A56" s="103"/>
-      <c r="B56" s="82"/>
+      <c r="A56" s="99"/>
+      <c r="B56" s="76"/>
       <c r="C56" s="64" t="s">
         <v>136</v>
       </c>
@@ -3551,8 +3551,8 @@
       <c r="X56" s="1"/>
     </row>
     <row r="57" spans="1:24" ht="45" x14ac:dyDescent="0.25">
-      <c r="A57" s="103"/>
-      <c r="B57" s="83"/>
+      <c r="A57" s="99"/>
+      <c r="B57" s="77"/>
       <c r="C57" s="64" t="s">
         <v>137</v>
       </c>
@@ -3593,27 +3593,27 @@
       <c r="X57" s="1"/>
     </row>
     <row r="58" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A58" s="103"/>
-      <c r="B58" s="82"/>
+      <c r="A58" s="99"/>
+      <c r="B58" s="76"/>
       <c r="C58" s="64" t="s">
         <v>138</v>
       </c>
-      <c r="D58" s="90" t="s">
+      <c r="D58" s="78" t="s">
         <v>49</v>
       </c>
-      <c r="E58" s="84" t="s">
+      <c r="E58" s="95" t="s">
         <v>10</v>
       </c>
-      <c r="F58" s="82" t="s">
+      <c r="F58" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="G58" s="82" t="s">
+      <c r="G58" s="76" t="s">
         <v>40</v>
       </c>
-      <c r="H58" s="82" t="s">
+      <c r="H58" s="76" t="s">
         <v>13</v>
       </c>
-      <c r="I58" s="82">
+      <c r="I58" s="76">
         <v>0</v>
       </c>
       <c r="J58" s="65" t="s">
@@ -3635,17 +3635,17 @@
       <c r="X58" s="1"/>
     </row>
     <row r="59" spans="1:24" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="104"/>
-      <c r="B59" s="83"/>
+      <c r="A59" s="100"/>
+      <c r="B59" s="77"/>
       <c r="C59" s="64" t="s">
         <v>139</v>
       </c>
-      <c r="D59" s="91"/>
-      <c r="E59" s="84"/>
-      <c r="F59" s="83"/>
-      <c r="G59" s="83"/>
-      <c r="H59" s="83"/>
-      <c r="I59" s="83"/>
+      <c r="D59" s="79"/>
+      <c r="E59" s="95"/>
+      <c r="F59" s="77"/>
+      <c r="G59" s="77"/>
+      <c r="H59" s="77"/>
+      <c r="I59" s="77"/>
       <c r="J59" s="65" t="s">
         <v>181</v>
       </c>
@@ -3665,29 +3665,29 @@
       <c r="X59" s="1"/>
     </row>
     <row r="60" spans="1:24" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="68" t="s">
+      <c r="A60" s="112" t="s">
         <v>50</v>
       </c>
-      <c r="B60" s="71"/>
+      <c r="B60" s="68"/>
       <c r="C60" s="34" t="s">
         <v>140</v>
       </c>
-      <c r="D60" s="77" t="s">
+      <c r="D60" s="73" t="s">
         <v>33</v>
       </c>
-      <c r="E60" s="71" t="s">
+      <c r="E60" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="F60" s="71">
+      <c r="F60" s="68">
         <v>0</v>
       </c>
-      <c r="G60" s="71">
+      <c r="G60" s="68">
         <v>1</v>
       </c>
-      <c r="H60" s="71" t="s">
+      <c r="H60" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="I60" s="71">
+      <c r="I60" s="68">
         <v>0</v>
       </c>
       <c r="J60" s="41"/>
@@ -3707,17 +3707,17 @@
       <c r="X60" s="1"/>
     </row>
     <row r="61" spans="1:24" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="69"/>
-      <c r="B61" s="73"/>
+      <c r="A61" s="113"/>
+      <c r="B61" s="69"/>
       <c r="C61" s="46" t="s">
         <v>141</v>
       </c>
-      <c r="D61" s="78"/>
-      <c r="E61" s="73"/>
-      <c r="F61" s="73"/>
-      <c r="G61" s="73"/>
-      <c r="H61" s="73"/>
-      <c r="I61" s="73"/>
+      <c r="D61" s="74"/>
+      <c r="E61" s="69"/>
+      <c r="F61" s="69"/>
+      <c r="G61" s="69"/>
+      <c r="H61" s="69"/>
+      <c r="I61" s="69"/>
       <c r="J61" s="45"/>
       <c r="K61" s="3"/>
       <c r="L61" s="3"/>
@@ -3735,30 +3735,30 @@
       <c r="X61" s="1"/>
     </row>
     <row r="62" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="69"/>
-      <c r="B62" s="71"/>
+      <c r="A62" s="113"/>
+      <c r="B62" s="68"/>
       <c r="C62" s="34" t="s">
         <v>142</v>
       </c>
-      <c r="D62" s="77" t="s">
+      <c r="D62" s="73" t="s">
         <v>51</v>
       </c>
-      <c r="E62" s="79" t="s">
+      <c r="E62" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="F62" s="71">
+      <c r="F62" s="68">
         <v>0</v>
       </c>
-      <c r="G62" s="80" t="s">
+      <c r="G62" s="110" t="s">
         <v>95</v>
       </c>
-      <c r="H62" s="71" t="s">
+      <c r="H62" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="I62" s="71">
+      <c r="I62" s="68">
         <v>0</v>
       </c>
-      <c r="J62" s="113" t="s">
+      <c r="J62" s="70" t="s">
         <v>182</v>
       </c>
       <c r="K62" s="3"/>
@@ -3777,18 +3777,18 @@
       <c r="X62" s="1"/>
     </row>
     <row r="63" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A63" s="69"/>
-      <c r="B63" s="73"/>
+      <c r="A63" s="113"/>
+      <c r="B63" s="69"/>
       <c r="C63" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="D63" s="78"/>
-      <c r="E63" s="79"/>
-      <c r="F63" s="73"/>
-      <c r="G63" s="81"/>
-      <c r="H63" s="73"/>
-      <c r="I63" s="73"/>
-      <c r="J63" s="114"/>
+      <c r="D63" s="74"/>
+      <c r="E63" s="75"/>
+      <c r="F63" s="69"/>
+      <c r="G63" s="111"/>
+      <c r="H63" s="69"/>
+      <c r="I63" s="69"/>
+      <c r="J63" s="71"/>
       <c r="K63" s="3"/>
       <c r="L63" s="3"/>
       <c r="M63" s="3"/>
@@ -3805,30 +3805,30 @@
       <c r="X63" s="1"/>
     </row>
     <row r="64" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="69"/>
-      <c r="B64" s="71"/>
+      <c r="A64" s="113"/>
+      <c r="B64" s="68"/>
       <c r="C64" s="34" t="s">
         <v>144</v>
       </c>
-      <c r="D64" s="77" t="s">
+      <c r="D64" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="E64" s="79" t="s">
+      <c r="E64" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="F64" s="71">
+      <c r="F64" s="68">
         <v>0</v>
       </c>
-      <c r="G64" s="71" t="s">
+      <c r="G64" s="68" t="s">
         <v>186</v>
       </c>
-      <c r="H64" s="71" t="s">
+      <c r="H64" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="I64" s="71" t="s">
+      <c r="I64" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="J64" s="113" t="s">
+      <c r="J64" s="70" t="s">
         <v>182</v>
       </c>
       <c r="K64" s="3"/>
@@ -3847,18 +3847,18 @@
       <c r="X64" s="1"/>
     </row>
     <row r="65" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="69"/>
-      <c r="B65" s="73"/>
+      <c r="A65" s="113"/>
+      <c r="B65" s="69"/>
       <c r="C65" s="34" t="s">
         <v>145</v>
       </c>
-      <c r="D65" s="78"/>
-      <c r="E65" s="79"/>
-      <c r="F65" s="73"/>
-      <c r="G65" s="73"/>
-      <c r="H65" s="73"/>
-      <c r="I65" s="73"/>
-      <c r="J65" s="114"/>
+      <c r="D65" s="74"/>
+      <c r="E65" s="75"/>
+      <c r="F65" s="69"/>
+      <c r="G65" s="69"/>
+      <c r="H65" s="69"/>
+      <c r="I65" s="69"/>
+      <c r="J65" s="71"/>
       <c r="K65" s="3"/>
       <c r="L65" s="3"/>
       <c r="M65" s="3"/>
@@ -3875,30 +3875,30 @@
       <c r="X65" s="1"/>
     </row>
     <row r="66" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="69"/>
-      <c r="B66" s="71"/>
+      <c r="A66" s="113"/>
+      <c r="B66" s="68"/>
       <c r="C66" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="D66" s="77" t="s">
+      <c r="D66" s="73" t="s">
         <v>53</v>
       </c>
-      <c r="E66" s="79" t="s">
+      <c r="E66" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="F66" s="71">
+      <c r="F66" s="68">
         <v>0</v>
       </c>
-      <c r="G66" s="80" t="s">
+      <c r="G66" s="110" t="s">
         <v>95</v>
       </c>
-      <c r="H66" s="71" t="s">
+      <c r="H66" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="I66" s="71" t="s">
+      <c r="I66" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="J66" s="113" t="s">
+      <c r="J66" s="70" t="s">
         <v>182</v>
       </c>
       <c r="K66" s="3"/>
@@ -3917,18 +3917,18 @@
       <c r="X66" s="1"/>
     </row>
     <row r="67" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A67" s="69"/>
-      <c r="B67" s="73"/>
+      <c r="A67" s="113"/>
+      <c r="B67" s="69"/>
       <c r="C67" s="34" t="s">
         <v>147</v>
       </c>
-      <c r="D67" s="78"/>
-      <c r="E67" s="79"/>
-      <c r="F67" s="73"/>
-      <c r="G67" s="81"/>
-      <c r="H67" s="73"/>
-      <c r="I67" s="73"/>
-      <c r="J67" s="114"/>
+      <c r="D67" s="74"/>
+      <c r="E67" s="75"/>
+      <c r="F67" s="69"/>
+      <c r="G67" s="111"/>
+      <c r="H67" s="69"/>
+      <c r="I67" s="69"/>
+      <c r="J67" s="71"/>
       <c r="K67" s="3"/>
       <c r="L67" s="3"/>
       <c r="M67" s="3"/>
@@ -3945,30 +3945,30 @@
       <c r="X67" s="1"/>
     </row>
     <row r="68" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="69"/>
-      <c r="B68" s="71"/>
+      <c r="A68" s="113"/>
+      <c r="B68" s="68"/>
       <c r="C68" s="34" t="s">
         <v>148</v>
       </c>
-      <c r="D68" s="77" t="s">
+      <c r="D68" s="73" t="s">
         <v>54</v>
       </c>
-      <c r="E68" s="79" t="s">
+      <c r="E68" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="F68" s="71">
+      <c r="F68" s="68">
         <v>0</v>
       </c>
-      <c r="G68" s="71" t="s">
+      <c r="G68" s="68" t="s">
         <v>186</v>
       </c>
-      <c r="H68" s="71" t="s">
+      <c r="H68" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="I68" s="71" t="s">
+      <c r="I68" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="J68" s="113" t="s">
+      <c r="J68" s="70" t="s">
         <v>182</v>
       </c>
       <c r="K68" s="3"/>
@@ -3987,18 +3987,18 @@
       <c r="X68" s="1"/>
     </row>
     <row r="69" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="69"/>
-      <c r="B69" s="73"/>
+      <c r="A69" s="113"/>
+      <c r="B69" s="69"/>
       <c r="C69" s="34" t="s">
         <v>149</v>
       </c>
-      <c r="D69" s="78"/>
-      <c r="E69" s="79"/>
-      <c r="F69" s="73"/>
-      <c r="G69" s="73"/>
-      <c r="H69" s="73"/>
-      <c r="I69" s="73"/>
-      <c r="J69" s="114"/>
+      <c r="D69" s="74"/>
+      <c r="E69" s="75"/>
+      <c r="F69" s="69"/>
+      <c r="G69" s="69"/>
+      <c r="H69" s="69"/>
+      <c r="I69" s="69"/>
+      <c r="J69" s="71"/>
       <c r="K69" s="3"/>
       <c r="L69" s="3"/>
       <c r="M69" s="3"/>
@@ -4015,30 +4015,30 @@
       <c r="X69" s="1"/>
     </row>
     <row r="70" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="69"/>
-      <c r="B70" s="71"/>
+      <c r="A70" s="113"/>
+      <c r="B70" s="68"/>
       <c r="C70" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="D70" s="77" t="s">
+      <c r="D70" s="73" t="s">
         <v>55</v>
       </c>
-      <c r="E70" s="79" t="s">
+      <c r="E70" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="F70" s="71">
+      <c r="F70" s="68">
         <v>0</v>
       </c>
-      <c r="G70" s="80" t="s">
+      <c r="G70" s="110" t="s">
         <v>95</v>
       </c>
-      <c r="H70" s="71" t="s">
+      <c r="H70" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="I70" s="71" t="s">
+      <c r="I70" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="J70" s="113" t="s">
+      <c r="J70" s="70" t="s">
         <v>182</v>
       </c>
       <c r="K70" s="3"/>
@@ -4057,18 +4057,18 @@
       <c r="X70" s="1"/>
     </row>
     <row r="71" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A71" s="69"/>
-      <c r="B71" s="73"/>
+      <c r="A71" s="113"/>
+      <c r="B71" s="69"/>
       <c r="C71" s="34" t="s">
         <v>151</v>
       </c>
-      <c r="D71" s="78"/>
-      <c r="E71" s="79"/>
-      <c r="F71" s="73"/>
-      <c r="G71" s="81"/>
-      <c r="H71" s="73"/>
-      <c r="I71" s="73"/>
-      <c r="J71" s="114"/>
+      <c r="D71" s="74"/>
+      <c r="E71" s="75"/>
+      <c r="F71" s="69"/>
+      <c r="G71" s="111"/>
+      <c r="H71" s="69"/>
+      <c r="I71" s="69"/>
+      <c r="J71" s="71"/>
       <c r="K71" s="3"/>
       <c r="L71" s="3"/>
       <c r="M71" s="3"/>
@@ -4085,30 +4085,30 @@
       <c r="X71" s="1"/>
     </row>
     <row r="72" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="69"/>
-      <c r="B72" s="71"/>
+      <c r="A72" s="113"/>
+      <c r="B72" s="68"/>
       <c r="C72" s="34" t="s">
         <v>152</v>
       </c>
-      <c r="D72" s="77" t="s">
+      <c r="D72" s="73" t="s">
         <v>56</v>
       </c>
-      <c r="E72" s="79" t="s">
+      <c r="E72" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="F72" s="71">
+      <c r="F72" s="68">
         <v>0</v>
       </c>
-      <c r="G72" s="71" t="s">
+      <c r="G72" s="68" t="s">
         <v>186</v>
       </c>
-      <c r="H72" s="71" t="s">
+      <c r="H72" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="I72" s="71" t="s">
+      <c r="I72" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="J72" s="113" t="s">
+      <c r="J72" s="70" t="s">
         <v>182</v>
       </c>
       <c r="K72" s="3"/>
@@ -4127,18 +4127,18 @@
       <c r="X72" s="1"/>
     </row>
     <row r="73" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="69"/>
-      <c r="B73" s="73"/>
+      <c r="A73" s="113"/>
+      <c r="B73" s="69"/>
       <c r="C73" s="34" t="s">
         <v>153</v>
       </c>
-      <c r="D73" s="78"/>
-      <c r="E73" s="79"/>
-      <c r="F73" s="73"/>
-      <c r="G73" s="73"/>
-      <c r="H73" s="73"/>
-      <c r="I73" s="73"/>
-      <c r="J73" s="114"/>
+      <c r="D73" s="74"/>
+      <c r="E73" s="75"/>
+      <c r="F73" s="69"/>
+      <c r="G73" s="69"/>
+      <c r="H73" s="69"/>
+      <c r="I73" s="69"/>
+      <c r="J73" s="71"/>
       <c r="K73" s="3"/>
       <c r="L73" s="3"/>
       <c r="M73" s="3"/>
@@ -4155,30 +4155,30 @@
       <c r="X73" s="1"/>
     </row>
     <row r="74" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="69"/>
-      <c r="B74" s="71"/>
+      <c r="A74" s="113"/>
+      <c r="B74" s="68"/>
       <c r="C74" s="34" t="s">
         <v>154</v>
       </c>
-      <c r="D74" s="77" t="s">
+      <c r="D74" s="73" t="s">
         <v>57</v>
       </c>
-      <c r="E74" s="79" t="s">
+      <c r="E74" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="F74" s="71">
+      <c r="F74" s="68">
         <v>0</v>
       </c>
-      <c r="G74" s="80" t="s">
+      <c r="G74" s="110" t="s">
         <v>95</v>
       </c>
-      <c r="H74" s="71" t="s">
+      <c r="H74" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="I74" s="71" t="s">
+      <c r="I74" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="J74" s="113" t="s">
+      <c r="J74" s="70" t="s">
         <v>182</v>
       </c>
       <c r="K74" s="3"/>
@@ -4197,18 +4197,18 @@
       <c r="X74" s="1"/>
     </row>
     <row r="75" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A75" s="69"/>
-      <c r="B75" s="73"/>
+      <c r="A75" s="113"/>
+      <c r="B75" s="69"/>
       <c r="C75" s="34" t="s">
         <v>155</v>
       </c>
-      <c r="D75" s="78"/>
-      <c r="E75" s="79"/>
-      <c r="F75" s="73"/>
-      <c r="G75" s="81"/>
-      <c r="H75" s="73"/>
-      <c r="I75" s="73"/>
-      <c r="J75" s="114"/>
+      <c r="D75" s="74"/>
+      <c r="E75" s="75"/>
+      <c r="F75" s="69"/>
+      <c r="G75" s="111"/>
+      <c r="H75" s="69"/>
+      <c r="I75" s="69"/>
+      <c r="J75" s="71"/>
       <c r="K75" s="3"/>
       <c r="L75" s="3"/>
       <c r="M75" s="3"/>
@@ -4225,30 +4225,30 @@
       <c r="X75" s="1"/>
     </row>
     <row r="76" spans="1:24" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="69"/>
-      <c r="B76" s="71"/>
+      <c r="A76" s="113"/>
+      <c r="B76" s="68"/>
       <c r="C76" s="34" t="s">
         <v>156</v>
       </c>
-      <c r="D76" s="77" t="s">
+      <c r="D76" s="73" t="s">
         <v>96</v>
       </c>
-      <c r="E76" s="79" t="s">
+      <c r="E76" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="F76" s="71">
+      <c r="F76" s="68">
         <v>0</v>
       </c>
-      <c r="G76" s="71" t="s">
+      <c r="G76" s="68" t="s">
         <v>186</v>
       </c>
-      <c r="H76" s="71" t="s">
+      <c r="H76" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="I76" s="71" t="s">
+      <c r="I76" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="J76" s="113" t="s">
+      <c r="J76" s="70" t="s">
         <v>182</v>
       </c>
       <c r="K76" s="3"/>
@@ -4267,18 +4267,18 @@
       <c r="X76" s="1"/>
     </row>
     <row r="77" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="69"/>
-      <c r="B77" s="73"/>
+      <c r="A77" s="113"/>
+      <c r="B77" s="69"/>
       <c r="C77" s="34" t="s">
         <v>157</v>
       </c>
-      <c r="D77" s="78"/>
-      <c r="E77" s="79"/>
-      <c r="F77" s="73"/>
-      <c r="G77" s="73"/>
-      <c r="H77" s="73"/>
-      <c r="I77" s="73"/>
-      <c r="J77" s="114"/>
+      <c r="D77" s="74"/>
+      <c r="E77" s="75"/>
+      <c r="F77" s="69"/>
+      <c r="G77" s="69"/>
+      <c r="H77" s="69"/>
+      <c r="I77" s="69"/>
+      <c r="J77" s="71"/>
       <c r="K77" s="3"/>
       <c r="L77" s="3"/>
       <c r="M77" s="3"/>
@@ -4295,30 +4295,30 @@
       <c r="X77" s="1"/>
     </row>
     <row r="78" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="69"/>
-      <c r="B78" s="71"/>
+      <c r="A78" s="113"/>
+      <c r="B78" s="68"/>
       <c r="C78" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="D78" s="77" t="s">
+      <c r="D78" s="73" t="s">
         <v>97</v>
       </c>
-      <c r="E78" s="79" t="s">
+      <c r="E78" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="F78" s="71">
+      <c r="F78" s="68">
         <v>0</v>
       </c>
-      <c r="G78" s="80" t="s">
+      <c r="G78" s="110" t="s">
         <v>95</v>
       </c>
-      <c r="H78" s="71" t="s">
+      <c r="H78" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="I78" s="71" t="s">
+      <c r="I78" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="J78" s="113" t="s">
+      <c r="J78" s="70" t="s">
         <v>182</v>
       </c>
       <c r="K78" s="3"/>
@@ -4337,18 +4337,18 @@
       <c r="X78" s="1"/>
     </row>
     <row r="79" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="70"/>
-      <c r="B79" s="72"/>
+      <c r="A79" s="114"/>
+      <c r="B79" s="115"/>
       <c r="C79" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="D79" s="78"/>
-      <c r="E79" s="79"/>
-      <c r="F79" s="73"/>
-      <c r="G79" s="81"/>
-      <c r="H79" s="73"/>
-      <c r="I79" s="73"/>
-      <c r="J79" s="114"/>
+      <c r="D79" s="74"/>
+      <c r="E79" s="75"/>
+      <c r="F79" s="69"/>
+      <c r="G79" s="111"/>
+      <c r="H79" s="69"/>
+      <c r="I79" s="69"/>
+      <c r="J79" s="71"/>
       <c r="K79" s="3"/>
       <c r="L79" s="3"/>
       <c r="M79" s="3"/>
@@ -4365,29 +4365,29 @@
       <c r="X79" s="1"/>
     </row>
     <row r="80" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="100" t="s">
+      <c r="A80" s="96" t="s">
         <v>81</v>
       </c>
-      <c r="B80" s="71"/>
+      <c r="B80" s="68"/>
       <c r="C80" s="39" t="s">
         <v>160</v>
       </c>
-      <c r="D80" s="77" t="s">
+      <c r="D80" s="73" t="s">
         <v>59</v>
       </c>
-      <c r="E80" s="79" t="s">
+      <c r="E80" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="F80" s="71">
+      <c r="F80" s="68">
         <v>0</v>
       </c>
-      <c r="G80" s="71">
+      <c r="G80" s="68">
         <v>255</v>
       </c>
-      <c r="H80" s="71" t="s">
+      <c r="H80" s="68" t="s">
         <v>13</v>
       </c>
-      <c r="I80" s="71">
+      <c r="I80" s="68">
         <v>0</v>
       </c>
       <c r="J80" s="47" t="s">
@@ -4409,17 +4409,17 @@
       <c r="X80" s="1"/>
     </row>
     <row r="81" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A81" s="101"/>
-      <c r="B81" s="73"/>
+      <c r="A81" s="97"/>
+      <c r="B81" s="69"/>
       <c r="C81" s="46" t="s">
         <v>161</v>
       </c>
-      <c r="D81" s="78"/>
-      <c r="E81" s="79"/>
-      <c r="F81" s="73"/>
-      <c r="G81" s="73"/>
-      <c r="H81" s="73"/>
-      <c r="I81" s="73"/>
+      <c r="D81" s="74"/>
+      <c r="E81" s="75"/>
+      <c r="F81" s="69"/>
+      <c r="G81" s="69"/>
+      <c r="H81" s="69"/>
+      <c r="I81" s="69"/>
       <c r="J81" s="48" t="s">
         <v>94</v>
       </c>
@@ -4439,8 +4439,8 @@
       <c r="X81" s="1"/>
     </row>
     <row r="82" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="101"/>
-      <c r="B82" s="71"/>
+      <c r="A82" s="97"/>
+      <c r="B82" s="68"/>
       <c r="C82" s="34" t="s">
         <v>162</v>
       </c>
@@ -4454,7 +4454,7 @@
         <v>1</v>
       </c>
       <c r="G82" s="18">
-        <v>15</v>
+        <v>247</v>
       </c>
       <c r="H82" s="18" t="s">
         <v>13</v>
@@ -4479,8 +4479,8 @@
       <c r="X82" s="1"/>
     </row>
     <row r="83" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A83" s="101"/>
-      <c r="B83" s="73"/>
+      <c r="A83" s="97"/>
+      <c r="B83" s="69"/>
       <c r="C83" s="34" t="s">
         <v>163</v>
       </c>
@@ -4517,30 +4517,30 @@
       <c r="X83" s="1"/>
     </row>
     <row r="84" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A84" s="101"/>
-      <c r="B84" s="71"/>
+      <c r="A84" s="97"/>
+      <c r="B84" s="68"/>
       <c r="C84" s="34" t="s">
         <v>164</v>
       </c>
-      <c r="D84" s="99" t="s">
+      <c r="D84" s="101" t="s">
         <v>62</v>
       </c>
-      <c r="E84" s="79" t="s">
+      <c r="E84" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="F84" s="79">
+      <c r="F84" s="75">
         <v>0</v>
       </c>
-      <c r="G84" s="79">
+      <c r="G84" s="75">
         <v>65535</v>
       </c>
-      <c r="H84" s="79" t="s">
+      <c r="H84" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="I84" s="71">
+      <c r="I84" s="68">
         <v>1</v>
       </c>
-      <c r="J84" s="113" t="s">
+      <c r="J84" s="70" t="s">
         <v>180</v>
       </c>
       <c r="K84" s="3"/>
@@ -4559,18 +4559,18 @@
       <c r="X84" s="1"/>
     </row>
     <row r="85" spans="1:24" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="101"/>
-      <c r="B85" s="73"/>
+      <c r="A85" s="97"/>
+      <c r="B85" s="69"/>
       <c r="C85" s="34" t="s">
         <v>165</v>
       </c>
-      <c r="D85" s="99"/>
-      <c r="E85" s="79"/>
-      <c r="F85" s="79"/>
-      <c r="G85" s="79"/>
-      <c r="H85" s="79"/>
-      <c r="I85" s="73"/>
-      <c r="J85" s="114"/>
+      <c r="D85" s="101"/>
+      <c r="E85" s="75"/>
+      <c r="F85" s="75"/>
+      <c r="G85" s="75"/>
+      <c r="H85" s="75"/>
+      <c r="I85" s="69"/>
+      <c r="J85" s="71"/>
       <c r="K85" s="3"/>
       <c r="L85" s="3"/>
       <c r="M85" s="3"/>
@@ -4587,30 +4587,30 @@
       <c r="X85" s="1"/>
     </row>
     <row r="86" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="101"/>
-      <c r="B86" s="71"/>
+      <c r="A86" s="97"/>
+      <c r="B86" s="68"/>
       <c r="C86" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="D86" s="99" t="s">
+      <c r="D86" s="101" t="s">
         <v>63</v>
       </c>
-      <c r="E86" s="79" t="s">
+      <c r="E86" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="F86" s="79">
+      <c r="F86" s="75">
         <v>0</v>
       </c>
-      <c r="G86" s="79" t="s">
+      <c r="G86" s="75" t="s">
         <v>66</v>
       </c>
-      <c r="H86" s="79" t="s">
+      <c r="H86" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="I86" s="71">
+      <c r="I86" s="68">
         <v>1</v>
       </c>
-      <c r="J86" s="113" t="s">
+      <c r="J86" s="70" t="s">
         <v>180</v>
       </c>
       <c r="K86" s="3"/>
@@ -4629,18 +4629,18 @@
       <c r="X86" s="1"/>
     </row>
     <row r="87" spans="1:24" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="101"/>
-      <c r="B87" s="73"/>
+      <c r="A87" s="97"/>
+      <c r="B87" s="69"/>
       <c r="C87" s="34" t="s">
         <v>167</v>
       </c>
-      <c r="D87" s="99"/>
-      <c r="E87" s="79"/>
-      <c r="F87" s="79"/>
-      <c r="G87" s="79"/>
-      <c r="H87" s="79"/>
-      <c r="I87" s="73"/>
-      <c r="J87" s="114"/>
+      <c r="D87" s="101"/>
+      <c r="E87" s="75"/>
+      <c r="F87" s="75"/>
+      <c r="G87" s="75"/>
+      <c r="H87" s="75"/>
+      <c r="I87" s="69"/>
+      <c r="J87" s="71"/>
       <c r="K87" s="30"/>
       <c r="L87" s="30"/>
       <c r="M87" s="30"/>
@@ -4657,28 +4657,28 @@
       <c r="X87" s="1"/>
     </row>
     <row r="88" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="101"/>
-      <c r="B88" s="71"/>
+      <c r="A88" s="97"/>
+      <c r="B88" s="68"/>
       <c r="C88" s="34" t="s">
         <v>168</v>
       </c>
-      <c r="D88" s="99" t="s">
+      <c r="D88" s="101" t="s">
         <v>65</v>
       </c>
-      <c r="E88" s="79" t="s">
+      <c r="E88" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="F88" s="79" t="s">
+      <c r="F88" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="G88" s="79" t="s">
+      <c r="G88" s="75" t="s">
         <v>68</v>
       </c>
-      <c r="H88" s="79" t="s">
+      <c r="H88" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="I88" s="71"/>
-      <c r="J88" s="74" t="s">
+      <c r="I88" s="68"/>
+      <c r="J88" s="108" t="s">
         <v>85</v>
       </c>
       <c r="K88" s="30"/>
@@ -4697,18 +4697,18 @@
       <c r="X88" s="1"/>
     </row>
     <row r="89" spans="1:24" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A89" s="101"/>
-      <c r="B89" s="73"/>
+      <c r="A89" s="97"/>
+      <c r="B89" s="69"/>
       <c r="C89" s="34" t="s">
         <v>169</v>
       </c>
-      <c r="D89" s="99"/>
-      <c r="E89" s="79"/>
-      <c r="F89" s="79"/>
-      <c r="G89" s="79"/>
-      <c r="H89" s="79"/>
-      <c r="I89" s="73"/>
-      <c r="J89" s="74"/>
+      <c r="D89" s="101"/>
+      <c r="E89" s="75"/>
+      <c r="F89" s="75"/>
+      <c r="G89" s="75"/>
+      <c r="H89" s="75"/>
+      <c r="I89" s="69"/>
+      <c r="J89" s="108"/>
       <c r="K89" s="30"/>
       <c r="L89" s="30"/>
       <c r="M89" s="30"/>
@@ -4725,28 +4725,28 @@
       <c r="X89" s="1"/>
     </row>
     <row r="90" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A90" s="101"/>
-      <c r="B90" s="71"/>
+      <c r="A90" s="97"/>
+      <c r="B90" s="68"/>
       <c r="C90" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="D90" s="99" t="s">
+      <c r="D90" s="101" t="s">
         <v>64</v>
       </c>
-      <c r="E90" s="79" t="s">
+      <c r="E90" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="F90" s="79" t="s">
+      <c r="F90" s="75" t="s">
         <v>67</v>
       </c>
-      <c r="G90" s="79" t="s">
+      <c r="G90" s="75" t="s">
         <v>68</v>
       </c>
-      <c r="H90" s="79" t="s">
+      <c r="H90" s="75" t="s">
         <v>13</v>
       </c>
-      <c r="I90" s="71"/>
-      <c r="J90" s="74" t="s">
+      <c r="I90" s="68"/>
+      <c r="J90" s="108" t="s">
         <v>86</v>
       </c>
       <c r="K90" s="30"/>
@@ -4765,18 +4765,18 @@
       <c r="X90" s="1"/>
     </row>
     <row r="91" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A91" s="102"/>
-      <c r="B91" s="73"/>
+      <c r="A91" s="98"/>
+      <c r="B91" s="69"/>
       <c r="C91" s="34" t="s">
         <v>171</v>
       </c>
-      <c r="D91" s="99"/>
-      <c r="E91" s="79"/>
-      <c r="F91" s="79"/>
-      <c r="G91" s="79"/>
-      <c r="H91" s="79"/>
-      <c r="I91" s="73"/>
-      <c r="J91" s="74"/>
+      <c r="D91" s="101"/>
+      <c r="E91" s="75"/>
+      <c r="F91" s="75"/>
+      <c r="G91" s="75"/>
+      <c r="H91" s="75"/>
+      <c r="I91" s="69"/>
+      <c r="J91" s="108"/>
       <c r="K91" s="3"/>
       <c r="L91" s="3"/>
       <c r="M91" s="3"/>
@@ -58077,6 +58077,225 @@
     </row>
   </sheetData>
   <mergeCells count="243">
+    <mergeCell ref="A60:A79"/>
+    <mergeCell ref="B78:B79"/>
+    <mergeCell ref="B84:B85"/>
+    <mergeCell ref="B86:B87"/>
+    <mergeCell ref="B88:B89"/>
+    <mergeCell ref="J90:J91"/>
+    <mergeCell ref="J88:J89"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="D78:D79"/>
+    <mergeCell ref="E78:E79"/>
+    <mergeCell ref="F78:F79"/>
+    <mergeCell ref="G78:G79"/>
+    <mergeCell ref="H78:H79"/>
+    <mergeCell ref="D76:D77"/>
+    <mergeCell ref="E76:E77"/>
+    <mergeCell ref="F76:F77"/>
+    <mergeCell ref="G76:G77"/>
+    <mergeCell ref="H76:H77"/>
+    <mergeCell ref="D74:D75"/>
+    <mergeCell ref="E74:E75"/>
+    <mergeCell ref="E66:E67"/>
+    <mergeCell ref="G66:G67"/>
+    <mergeCell ref="F66:F67"/>
+    <mergeCell ref="F74:F75"/>
+    <mergeCell ref="G74:G75"/>
+    <mergeCell ref="H74:H75"/>
+    <mergeCell ref="D72:D73"/>
+    <mergeCell ref="E72:E73"/>
+    <mergeCell ref="F72:F73"/>
+    <mergeCell ref="G72:G73"/>
+    <mergeCell ref="H72:H73"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="F70:F71"/>
+    <mergeCell ref="G70:G71"/>
+    <mergeCell ref="H70:H71"/>
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="B76:B77"/>
+    <mergeCell ref="D62:D63"/>
+    <mergeCell ref="E62:E63"/>
+    <mergeCell ref="F62:F63"/>
+    <mergeCell ref="G62:G63"/>
+    <mergeCell ref="D64:D65"/>
+    <mergeCell ref="H46:H47"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="F50:F51"/>
+    <mergeCell ref="G50:G51"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="F54:F55"/>
+    <mergeCell ref="G54:G55"/>
+    <mergeCell ref="H66:H67"/>
+    <mergeCell ref="H64:H65"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="E68:E69"/>
+    <mergeCell ref="F68:F69"/>
+    <mergeCell ref="G68:G69"/>
+    <mergeCell ref="H68:H69"/>
+    <mergeCell ref="D66:D67"/>
+    <mergeCell ref="E64:E65"/>
+    <mergeCell ref="F64:F65"/>
+    <mergeCell ref="G64:G65"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="H54:H55"/>
+    <mergeCell ref="H58:H59"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="F33:F34"/>
+    <mergeCell ref="G33:G34"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="D58:D59"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="F46:F47"/>
+    <mergeCell ref="G46:G47"/>
+    <mergeCell ref="E58:E59"/>
+    <mergeCell ref="F58:F59"/>
+    <mergeCell ref="G58:G59"/>
+    <mergeCell ref="I19:I20"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="I33:I34"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="I41:I42"/>
+    <mergeCell ref="I46:I47"/>
+    <mergeCell ref="H50:H51"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="G15:G16"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B19:B20"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="G84:G85"/>
+    <mergeCell ref="F86:F87"/>
+    <mergeCell ref="G86:G87"/>
+    <mergeCell ref="G88:G89"/>
+    <mergeCell ref="F88:F89"/>
+    <mergeCell ref="F90:F91"/>
+    <mergeCell ref="G90:G91"/>
+    <mergeCell ref="H84:H85"/>
+    <mergeCell ref="H86:H87"/>
+    <mergeCell ref="H88:H89"/>
+    <mergeCell ref="H90:H91"/>
+    <mergeCell ref="F84:F85"/>
+    <mergeCell ref="E84:E85"/>
+    <mergeCell ref="E86:E87"/>
+    <mergeCell ref="E88:E89"/>
+    <mergeCell ref="E90:E91"/>
+    <mergeCell ref="D84:D85"/>
+    <mergeCell ref="D86:D87"/>
+    <mergeCell ref="D88:D89"/>
+    <mergeCell ref="D90:D91"/>
+    <mergeCell ref="B80:B81"/>
+    <mergeCell ref="B82:B83"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="A80:A91"/>
+    <mergeCell ref="B90:B91"/>
+    <mergeCell ref="A32:A39"/>
+    <mergeCell ref="A40:A59"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="B58:B59"/>
+    <mergeCell ref="A17:A30"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="B70:B71"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="J15:J16"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="I13:I14"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="A5:A14"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="J11:J12"/>
+    <mergeCell ref="H15:H16"/>
+    <mergeCell ref="J9:J10"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="F13:F14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="I54:I55"/>
+    <mergeCell ref="J33:J34"/>
+    <mergeCell ref="J41:J42"/>
+    <mergeCell ref="J62:J63"/>
+    <mergeCell ref="I62:I63"/>
+    <mergeCell ref="I64:I65"/>
+    <mergeCell ref="J64:J65"/>
+    <mergeCell ref="I66:I67"/>
+    <mergeCell ref="J66:J67"/>
+    <mergeCell ref="I70:I71"/>
+    <mergeCell ref="J70:J71"/>
+    <mergeCell ref="I72:I73"/>
+    <mergeCell ref="J72:J73"/>
+    <mergeCell ref="I74:I75"/>
+    <mergeCell ref="J74:J75"/>
+    <mergeCell ref="I76:I77"/>
+    <mergeCell ref="J76:J77"/>
+    <mergeCell ref="I58:I59"/>
     <mergeCell ref="I78:I79"/>
     <mergeCell ref="J78:J79"/>
     <mergeCell ref="I84:I85"/>
@@ -58101,225 +58320,6 @@
     <mergeCell ref="H62:H63"/>
     <mergeCell ref="I68:I69"/>
     <mergeCell ref="J68:J69"/>
-    <mergeCell ref="I70:I71"/>
-    <mergeCell ref="J70:J71"/>
-    <mergeCell ref="I72:I73"/>
-    <mergeCell ref="J72:J73"/>
-    <mergeCell ref="I74:I75"/>
-    <mergeCell ref="J74:J75"/>
-    <mergeCell ref="I76:I77"/>
-    <mergeCell ref="J76:J77"/>
-    <mergeCell ref="I58:I59"/>
-    <mergeCell ref="I54:I55"/>
-    <mergeCell ref="J33:J34"/>
-    <mergeCell ref="J41:J42"/>
-    <mergeCell ref="J62:J63"/>
-    <mergeCell ref="I62:I63"/>
-    <mergeCell ref="I64:I65"/>
-    <mergeCell ref="J64:J65"/>
-    <mergeCell ref="I66:I67"/>
-    <mergeCell ref="J66:J67"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="J15:J16"/>
-    <mergeCell ref="I7:I8"/>
-    <mergeCell ref="I9:I10"/>
-    <mergeCell ref="I11:I12"/>
-    <mergeCell ref="I13:I14"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="A5:A14"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="J11:J12"/>
-    <mergeCell ref="H15:H16"/>
-    <mergeCell ref="J9:J10"/>
-    <mergeCell ref="D13:D14"/>
-    <mergeCell ref="E13:E14"/>
-    <mergeCell ref="F13:F14"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="E11:E12"/>
-    <mergeCell ref="F11:F12"/>
-    <mergeCell ref="G11:G12"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B36:B37"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="A80:A91"/>
-    <mergeCell ref="B90:B91"/>
-    <mergeCell ref="A32:A39"/>
-    <mergeCell ref="A40:A59"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="B56:B57"/>
-    <mergeCell ref="B58:B59"/>
-    <mergeCell ref="A17:A30"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="B66:B67"/>
-    <mergeCell ref="B68:B69"/>
-    <mergeCell ref="B70:B71"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="E84:E85"/>
-    <mergeCell ref="E86:E87"/>
-    <mergeCell ref="E88:E89"/>
-    <mergeCell ref="E90:E91"/>
-    <mergeCell ref="D84:D85"/>
-    <mergeCell ref="D86:D87"/>
-    <mergeCell ref="D88:D89"/>
-    <mergeCell ref="D90:D91"/>
-    <mergeCell ref="B80:B81"/>
-    <mergeCell ref="B82:B83"/>
-    <mergeCell ref="G84:G85"/>
-    <mergeCell ref="F86:F87"/>
-    <mergeCell ref="G86:G87"/>
-    <mergeCell ref="G88:G89"/>
-    <mergeCell ref="F88:F89"/>
-    <mergeCell ref="F90:F91"/>
-    <mergeCell ref="G90:G91"/>
-    <mergeCell ref="H84:H85"/>
-    <mergeCell ref="H86:H87"/>
-    <mergeCell ref="H88:H89"/>
-    <mergeCell ref="H90:H91"/>
-    <mergeCell ref="F84:F85"/>
-    <mergeCell ref="I19:I20"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="I33:I34"/>
-    <mergeCell ref="J26:J27"/>
-    <mergeCell ref="I41:I42"/>
-    <mergeCell ref="I46:I47"/>
-    <mergeCell ref="H50:H51"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="G15:G16"/>
-    <mergeCell ref="B42:B43"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="B19:B20"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="H54:H55"/>
-    <mergeCell ref="H58:H59"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="F33:F34"/>
-    <mergeCell ref="G33:G34"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="D46:D47"/>
-    <mergeCell ref="D50:D51"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="D58:D59"/>
-    <mergeCell ref="E46:E47"/>
-    <mergeCell ref="F46:F47"/>
-    <mergeCell ref="G46:G47"/>
-    <mergeCell ref="E58:E59"/>
-    <mergeCell ref="F58:F59"/>
-    <mergeCell ref="G58:G59"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B17:B18"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="F9:F10"/>
-    <mergeCell ref="G9:G10"/>
-    <mergeCell ref="H9:H10"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B76:B77"/>
-    <mergeCell ref="D62:D63"/>
-    <mergeCell ref="E62:E63"/>
-    <mergeCell ref="F62:F63"/>
-    <mergeCell ref="G62:G63"/>
-    <mergeCell ref="D64:D65"/>
-    <mergeCell ref="H46:H47"/>
-    <mergeCell ref="E50:E51"/>
-    <mergeCell ref="F50:F51"/>
-    <mergeCell ref="G50:G51"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="F54:F55"/>
-    <mergeCell ref="G54:G55"/>
-    <mergeCell ref="H66:H67"/>
-    <mergeCell ref="H64:H65"/>
-    <mergeCell ref="D68:D69"/>
-    <mergeCell ref="E68:E69"/>
-    <mergeCell ref="F68:F69"/>
-    <mergeCell ref="G68:G69"/>
-    <mergeCell ref="H68:H69"/>
-    <mergeCell ref="D66:D67"/>
-    <mergeCell ref="E64:E65"/>
-    <mergeCell ref="F64:F65"/>
-    <mergeCell ref="G64:G65"/>
-    <mergeCell ref="G74:G75"/>
-    <mergeCell ref="H74:H75"/>
-    <mergeCell ref="D72:D73"/>
-    <mergeCell ref="E72:E73"/>
-    <mergeCell ref="F72:F73"/>
-    <mergeCell ref="G72:G73"/>
-    <mergeCell ref="H72:H73"/>
-    <mergeCell ref="E70:E71"/>
-    <mergeCell ref="F70:F71"/>
-    <mergeCell ref="G70:G71"/>
-    <mergeCell ref="H70:H71"/>
-    <mergeCell ref="D70:D71"/>
-    <mergeCell ref="A60:A79"/>
-    <mergeCell ref="B78:B79"/>
-    <mergeCell ref="B84:B85"/>
-    <mergeCell ref="B86:B87"/>
-    <mergeCell ref="B88:B89"/>
-    <mergeCell ref="J90:J91"/>
-    <mergeCell ref="J88:J89"/>
-    <mergeCell ref="H13:H14"/>
-    <mergeCell ref="D78:D79"/>
-    <mergeCell ref="E78:E79"/>
-    <mergeCell ref="F78:F79"/>
-    <mergeCell ref="G78:G79"/>
-    <mergeCell ref="H78:H79"/>
-    <mergeCell ref="D76:D77"/>
-    <mergeCell ref="E76:E77"/>
-    <mergeCell ref="F76:F77"/>
-    <mergeCell ref="G76:G77"/>
-    <mergeCell ref="H76:H77"/>
-    <mergeCell ref="D74:D75"/>
-    <mergeCell ref="E74:E75"/>
-    <mergeCell ref="E66:E67"/>
-    <mergeCell ref="G66:G67"/>
-    <mergeCell ref="F66:F67"/>
-    <mergeCell ref="F74:F75"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="55" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -58344,204 +58344,204 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="120" t="s">
+      <c r="A1" s="118" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="79">
+      <c r="B1" s="75">
         <v>1</v>
       </c>
       <c r="C1" s="18">
         <v>1</v>
       </c>
-      <c r="D1" s="74" t="s">
+      <c r="D1" s="108" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="79" t="s">
+      <c r="E1" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="79"/>
-      <c r="G1" s="79"/>
-      <c r="H1" s="79" t="s">
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="120"/>
-      <c r="B2" s="79"/>
+      <c r="A2" s="118"/>
+      <c r="B2" s="75"/>
       <c r="C2" s="18">
         <v>2</v>
       </c>
-      <c r="D2" s="74"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="79"/>
-      <c r="G2" s="79"/>
-      <c r="H2" s="79"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="120"/>
-      <c r="B3" s="79">
+      <c r="A3" s="118"/>
+      <c r="B3" s="75">
         <v>2</v>
       </c>
       <c r="C3" s="18">
         <v>3</v>
       </c>
-      <c r="D3" s="74" t="s">
+      <c r="D3" s="108" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="79" t="s">
+      <c r="E3" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79" t="s">
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="120"/>
-      <c r="B4" s="79"/>
+      <c r="A4" s="118"/>
+      <c r="B4" s="75"/>
       <c r="C4" s="18">
         <v>4</v>
       </c>
-      <c r="D4" s="74"/>
-      <c r="E4" s="79"/>
-      <c r="F4" s="79"/>
-      <c r="G4" s="79"/>
-      <c r="H4" s="79"/>
+      <c r="D4" s="108"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="120"/>
-      <c r="B5" s="79">
+      <c r="A5" s="118"/>
+      <c r="B5" s="75">
         <v>3</v>
       </c>
       <c r="C5" s="18">
         <v>5</v>
       </c>
-      <c r="D5" s="74" t="s">
+      <c r="D5" s="108" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="79" t="s">
+      <c r="E5" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="79"/>
-      <c r="G5" s="79"/>
-      <c r="H5" s="79" t="s">
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="75" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="120"/>
-      <c r="B6" s="79"/>
+      <c r="A6" s="118"/>
+      <c r="B6" s="75"/>
       <c r="C6" s="18">
         <v>6</v>
       </c>
-      <c r="D6" s="74"/>
-      <c r="E6" s="79"/>
-      <c r="F6" s="79"/>
-      <c r="G6" s="79"/>
-      <c r="H6" s="79"/>
+      <c r="D6" s="108"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
+      <c r="G6" s="75"/>
+      <c r="H6" s="75"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="120"/>
-      <c r="B7" s="116">
+      <c r="A7" s="118"/>
+      <c r="B7" s="119">
         <v>4</v>
       </c>
       <c r="C7" s="19">
         <v>7</v>
       </c>
-      <c r="D7" s="117" t="s">
+      <c r="D7" s="120" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="116" t="s">
+      <c r="E7" s="119" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="116"/>
-      <c r="G7" s="116"/>
-      <c r="H7" s="116" t="s">
+      <c r="F7" s="119"/>
+      <c r="G7" s="119"/>
+      <c r="H7" s="119" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="120"/>
-      <c r="B8" s="116"/>
+      <c r="A8" s="118"/>
+      <c r="B8" s="119"/>
       <c r="C8" s="19">
         <v>8</v>
       </c>
-      <c r="D8" s="117"/>
-      <c r="E8" s="116"/>
-      <c r="F8" s="116"/>
-      <c r="G8" s="116"/>
-      <c r="H8" s="116"/>
+      <c r="D8" s="120"/>
+      <c r="E8" s="119"/>
+      <c r="F8" s="119"/>
+      <c r="G8" s="119"/>
+      <c r="H8" s="119"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="120"/>
-      <c r="B9" s="79">
+      <c r="A9" s="118"/>
+      <c r="B9" s="75">
         <v>5</v>
       </c>
       <c r="C9" s="18">
         <v>9</v>
       </c>
-      <c r="D9" s="119" t="s">
+      <c r="D9" s="117" t="s">
         <v>8</v>
       </c>
-      <c r="E9" s="79" t="s">
+      <c r="E9" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="F9" s="79"/>
-      <c r="G9" s="79"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="75"/>
       <c r="H9" s="18"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="120"/>
-      <c r="B10" s="79"/>
+      <c r="A10" s="118"/>
+      <c r="B10" s="75"/>
       <c r="C10" s="18">
         <v>10</v>
       </c>
-      <c r="D10" s="119"/>
-      <c r="E10" s="79"/>
-      <c r="F10" s="79"/>
-      <c r="G10" s="79"/>
+      <c r="D10" s="117"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="75"/>
       <c r="H10" s="18" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="118"/>
-      <c r="B11" s="79">
+      <c r="A11" s="116"/>
+      <c r="B11" s="75">
         <v>6</v>
       </c>
       <c r="C11" s="18">
         <v>11</v>
       </c>
-      <c r="D11" s="74" t="s">
+      <c r="D11" s="108" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="79" t="s">
+      <c r="E11" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="79"/>
-      <c r="G11" s="79"/>
-      <c r="H11" s="79" t="s">
+      <c r="F11" s="75"/>
+      <c r="G11" s="75"/>
+      <c r="H11" s="75" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="118"/>
-      <c r="B12" s="79"/>
+      <c r="A12" s="116"/>
+      <c r="B12" s="75"/>
       <c r="C12" s="18">
         <v>12</v>
       </c>
-      <c r="D12" s="74"/>
-      <c r="E12" s="79"/>
-      <c r="F12" s="79"/>
-      <c r="G12" s="79"/>
-      <c r="H12" s="79"/>
+      <c r="D12" s="108"/>
+      <c r="E12" s="75"/>
+      <c r="F12" s="75"/>
+      <c r="G12" s="75"/>
+      <c r="H12" s="75"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="118" t="s">
+      <c r="A14" s="116" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="118"/>
+      <c r="B14" s="116"/>
       <c r="C14" s="22" t="s">
         <v>9</v>
       </c>
@@ -58706,10 +58706,10 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="79" t="s">
+      <c r="A33" s="75" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="79"/>
+      <c r="B33" s="75"/>
       <c r="C33" s="29" t="s">
         <v>9</v>
       </c>
@@ -58788,6 +58788,29 @@
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H5:H6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="G11:G12"/>
     <mergeCell ref="H11:H12"/>
@@ -58804,29 +58827,6 @@
     <mergeCell ref="F11:F12"/>
     <mergeCell ref="A1:A10"/>
     <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="E3:E4"/>
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="G3:G4"/>
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>